<commit_message>
Preliminary simulations on nrel24b!
More reorganization to get files in the right places and better handle
national vs pnw (vs others in the future). Able to register/retrieve
values on the runner. Added weather files.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -947,30 +947,12 @@
     <t>SetResStockMode</t>
   </si>
   <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>mode</t>
-  </si>
-  <si>
     <t>National</t>
   </si>
   <si>
     <t>Set Res Stock Mode - National</t>
   </si>
   <si>
-    <t>measures</t>
-  </si>
-  <si>
-    <t>analysis</t>
-  </si>
-  <si>
-    <t>weather/*.epw</t>
-  </si>
-  <si>
-    <t>seeds/EmptySeedModel.osm</t>
-  </si>
-  <si>
     <t>Set Location Sample Value</t>
   </si>
   <si>
@@ -981,6 +963,24 @@
   </si>
   <si>
     <t>Set Wall Insulation</t>
+  </si>
+  <si>
+    <t>res_stock_mode</t>
+  </si>
+  <si>
+    <t>Res Stock Mode</t>
+  </si>
+  <si>
+    <t>../measures</t>
+  </si>
+  <si>
+    <t>../seeds/EmptySeedModel.osm</t>
+  </si>
+  <si>
+    <t>../analysis_results</t>
+  </si>
+  <si>
+    <t>../weather/national/*.*</t>
   </si>
 </sst>
 </file>
@@ -4540,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4723,7 +4723,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>160</v>
@@ -4734,7 +4734,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>160</v>
@@ -5069,7 +5069,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5101,7 +5101,7 @@
         <v>38</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>59</v>
@@ -5199,7 +5199,7 @@
   <dimension ref="A1:Z63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5382,7 +5382,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>301</v>
@@ -5401,10 +5401,10 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -5492,7 +5492,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>293</v>
@@ -5501,19 +5501,19 @@
         <v>174</v>
       </c>
       <c r="I8" s="39">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="K8" s="39">
+        <v>0</v>
+      </c>
+      <c r="L8" s="39">
         <v>1</v>
       </c>
-      <c r="L8" s="39">
-        <v>100</v>
-      </c>
       <c r="M8" s="39">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="N8" s="39">
-        <v>16.66667</v>
+        <v>0.1666667</v>
       </c>
       <c r="R8" s="39" t="s">
         <v>279</v>
@@ -5579,7 +5579,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>293</v>
@@ -5588,19 +5588,19 @@
         <v>174</v>
       </c>
       <c r="I11" s="39">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="K11" s="39">
+        <v>0</v>
+      </c>
+      <c r="L11" s="39">
         <v>1</v>
       </c>
-      <c r="L11" s="39">
-        <v>100</v>
-      </c>
       <c r="M11" s="39">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="N11" s="39">
-        <v>16.66667</v>
+        <v>0.1666667</v>
       </c>
       <c r="R11" s="39" t="s">
         <v>279</v>
@@ -5611,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>291</v>
@@ -5666,7 +5666,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E14" s="39" t="s">
         <v>293</v>
@@ -5675,19 +5675,19 @@
         <v>174</v>
       </c>
       <c r="I14" s="39">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="39">
+        <v>0</v>
+      </c>
+      <c r="L14" s="39">
         <v>1</v>
       </c>
-      <c r="L14" s="39">
-        <v>100</v>
-      </c>
       <c r="M14" s="39">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="N14" s="39">
-        <v>16.66667</v>
+        <v>0.1666667</v>
       </c>
       <c r="R14" s="39" t="s">
         <v>279</v>

</xml_diff>

<commit_message>
Split location.txt into location_region.txt and location_epw.txt. Tested with wall insulation. Fixes #2.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="317">
   <si>
     <t>type</t>
   </si>
@@ -929,18 +929,12 @@
     <t>probability_file</t>
   </si>
   <si>
-    <t>location.txt</t>
-  </si>
-  <si>
     <t>vintage.txt</t>
   </si>
   <si>
     <t>insulation_wall.txt</t>
   </si>
   <si>
-    <t>Set Location</t>
-  </si>
-  <si>
     <t>Set Vintage</t>
   </si>
   <si>
@@ -953,9 +947,6 @@
     <t>Set Res Stock Mode - National</t>
   </si>
   <si>
-    <t>Set Location Sample Value</t>
-  </si>
-  <si>
     <t>Set Vintage Sample Value</t>
   </si>
   <si>
@@ -981,6 +972,24 @@
   </si>
   <si>
     <t>../weather/national/*.*</t>
+  </si>
+  <si>
+    <t>location_epw.txt</t>
+  </si>
+  <si>
+    <t>Set Location EPW</t>
+  </si>
+  <si>
+    <t>Set Location Region</t>
+  </si>
+  <si>
+    <t>location_region.txt</t>
+  </si>
+  <si>
+    <t>Set Location Region Sample Value</t>
+  </si>
+  <si>
+    <t>Set Location EPW Sample Value</t>
   </si>
 </sst>
 </file>
@@ -4723,7 +4732,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>160</v>
@@ -4734,7 +4743,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>160</v>
@@ -5069,7 +5078,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5101,7 +5110,7 @@
         <v>38</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>59</v>
@@ -5196,10 +5205,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z63"/>
+  <dimension ref="A1:Z66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5382,13 +5391,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>42</v>
@@ -5401,10 +5410,10 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
@@ -5412,7 +5421,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -5437,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>291</v>
@@ -5467,7 +5476,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -5492,7 +5501,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>293</v>
@@ -5524,7 +5533,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>291</v>
@@ -5554,7 +5563,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -5579,7 +5588,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>293</v>
@@ -5611,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>291</v>
@@ -5641,7 +5650,7 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -5666,7 +5675,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E14" s="39" t="s">
         <v>293</v>
@@ -5693,44 +5702,43 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-    </row>
-    <row r="16" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>295</v>
+      </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>297</v>
+      </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -5749,35 +5757,39 @@
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
     </row>
-    <row r="17" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-    </row>
-    <row r="18" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="39">
+        <v>0</v>
+      </c>
+      <c r="L17" s="39">
+        <v>1</v>
+      </c>
+      <c r="M17" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N17" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R17" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -5834,7 +5846,7 @@
       <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -5861,7 +5873,7 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -5902,11 +5914,11 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
@@ -5917,7 +5929,7 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -5958,7 +5970,7 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
@@ -5973,7 +5985,7 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -6253,19 +6265,19 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -6281,20 +6293,20 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
+    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
@@ -6309,24 +6321,24 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
+    <row r="37" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
@@ -6352,8 +6364,8 @@
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
-      <c r="O38" s="38"/>
-      <c r="P38" s="38"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>
@@ -6436,8 +6448,8 @@
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
       <c r="S41" s="15"/>
@@ -6505,7 +6517,7 @@
       <c r="Y43" s="15"/>
       <c r="Z43" s="15"/>
     </row>
-    <row r="44" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -6519,9 +6531,9 @@
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="38"/>
-      <c r="P44" s="38"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="15"/>
@@ -6589,7 +6601,7 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -6603,9 +6615,9 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
@@ -6701,8 +6713,8 @@
       <c r="Y50" s="15"/>
       <c r="Z50" s="15"/>
     </row>
-    <row r="51" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
@@ -6716,8 +6728,8 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
-      <c r="O51" s="38"/>
-      <c r="P51" s="38"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
       <c r="S51" s="15"/>
@@ -6772,8 +6784,8 @@
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
-      <c r="O53" s="38"/>
-      <c r="P53" s="38"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="15"/>
@@ -6785,8 +6797,8 @@
       <c r="Y53" s="15"/>
       <c r="Z53" s="15"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+    <row r="54" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -6884,8 +6896,8 @@
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
+      <c r="O57" s="38"/>
+      <c r="P57" s="38"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
@@ -6912,8 +6924,8 @@
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
-      <c r="O58" s="38"/>
-      <c r="P58" s="38"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="15"/>
@@ -6940,8 +6952,8 @@
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
+      <c r="O59" s="38"/>
+      <c r="P59" s="38"/>
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
@@ -6968,8 +6980,8 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
       <c r="N60" s="15"/>
-      <c r="O60" s="38"/>
-      <c r="P60" s="38"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
       <c r="S60" s="15"/>
@@ -6996,8 +7008,8 @@
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
       <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
-      <c r="P61" s="15"/>
+      <c r="O61" s="38"/>
+      <c r="P61" s="38"/>
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
       <c r="S61" s="15"/>
@@ -7024,8 +7036,8 @@
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
-      <c r="O62" s="38"/>
-      <c r="P62" s="38"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
       <c r="S62" s="15"/>
@@ -7052,8 +7064,8 @@
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
-      <c r="P63" s="15"/>
+      <c r="O63" s="38"/>
+      <c r="P63" s="38"/>
       <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
       <c r="S63" s="15"/>
@@ -7064,6 +7076,90 @@
       <c r="X63" s="15"/>
       <c r="Y63" s="15"/>
       <c r="Z63" s="15"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="15"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="15"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="15"/>
+      <c r="X64" s="15"/>
+      <c r="Y64" s="15"/>
+      <c r="Z64" s="15"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="38"/>
+      <c r="P65" s="38"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
+      <c r="S65" s="15"/>
+      <c r="T65" s="15"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="15"/>
+      <c r="X65" s="15"/>
+      <c r="Y65" s="15"/>
+      <c r="Z65" s="15"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+      <c r="T66" s="15"/>
+      <c r="U66" s="15"/>
+      <c r="V66" s="15"/>
+      <c r="W66" s="15"/>
+      <c r="X66" s="15"/>
+      <c r="Y66" s="15"/>
+      <c r="Z66" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>

</xml_diff>

<commit_message>
First cut at geometry, addresses #3. Added enough constructions to get simulations running. Added run.rb to perform integrity checks.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="368">
   <si>
     <t>type</t>
   </si>
@@ -923,9 +923,6 @@
     <t>sample_value</t>
   </si>
   <si>
-    <t>Set Probability Distributions File</t>
-  </si>
-  <si>
     <t>probability_file</t>
   </si>
   <si>
@@ -947,15 +944,6 @@
     <t>Set Res Stock Mode - National</t>
   </si>
   <si>
-    <t>Set Vintage Sample Value</t>
-  </si>
-  <si>
-    <t>Set Wall Insulation Sample Value</t>
-  </si>
-  <si>
-    <t>Set Wall Insulation</t>
-  </si>
-  <si>
     <t>res_stock_mode</t>
   </si>
   <si>
@@ -986,10 +974,175 @@
     <t>location_region.txt</t>
   </si>
   <si>
-    <t>Set Location Region Sample Value</t>
-  </si>
-  <si>
-    <t>Set Location EPW Sample Value</t>
+    <t>Probability Distributions File</t>
+  </si>
+  <si>
+    <t>Location Region Sample Value</t>
+  </si>
+  <si>
+    <t>Location EPW Sample Value</t>
+  </si>
+  <si>
+    <t>Vintage Sample Value</t>
+  </si>
+  <si>
+    <t>geometry_foundation_type.txt</t>
+  </si>
+  <si>
+    <t>geometry_size.txt</t>
+  </si>
+  <si>
+    <t>geometry_stories.txt</t>
+  </si>
+  <si>
+    <t>geometry_garage.txt</t>
+  </si>
+  <si>
+    <t>Set Geometry</t>
+  </si>
+  <si>
+    <t>Geometry Sample Value</t>
+  </si>
+  <si>
+    <t>geometry.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Walls</t>
+  </si>
+  <si>
+    <t>Insulation Walls Sample Value</t>
+  </si>
+  <si>
+    <t>Set Geometry Garage</t>
+  </si>
+  <si>
+    <t>Geometry Garage Sample Value</t>
+  </si>
+  <si>
+    <t>Set Geometry Stories</t>
+  </si>
+  <si>
+    <t>Geometry Stories Sample Value</t>
+  </si>
+  <si>
+    <t>Set Geometry House Size</t>
+  </si>
+  <si>
+    <t>Geometry House Size Sample Value</t>
+  </si>
+  <si>
+    <t>Set Geometry Foundation Type</t>
+  </si>
+  <si>
+    <t>Geometry Foundation Type Sample Value</t>
+  </si>
+  <si>
+    <t>Set Insulation Walls Interzonal</t>
+  </si>
+  <si>
+    <t>Insulation Walls Interzonal Sample Value</t>
+  </si>
+  <si>
+    <t>insulation_wall_interzonal.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Slab</t>
+  </si>
+  <si>
+    <t>Insulation Slab Sample Value</t>
+  </si>
+  <si>
+    <t>insulation_slab.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Crawl</t>
+  </si>
+  <si>
+    <t>Insulation Crawl Sample Value</t>
+  </si>
+  <si>
+    <t>insulation_crawlspace.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Unfinished Basement</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Basement Sample Value</t>
+  </si>
+  <si>
+    <t>insulation_basement_unfinished.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Finished Basement</t>
+  </si>
+  <si>
+    <t>Insulation Finished Basement Sample Value</t>
+  </si>
+  <si>
+    <t>insulation_basement_finished.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Pier &amp; Beam</t>
+  </si>
+  <si>
+    <t>Insulation Pier &amp; Beam Sample Value</t>
+  </si>
+  <si>
+    <t>insulation_pier_beam.txt</t>
+  </si>
+  <si>
+    <t>insulation_unfinished_attic.txt</t>
+  </si>
+  <si>
+    <t>Set Insulation Unfinished Attic</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Attic Sample Value</t>
+  </si>
+  <si>
+    <t>Insulation Floors Interzonal Sample Value</t>
+  </si>
+  <si>
+    <t>Set Insulation Floors Interzonal</t>
+  </si>
+  <si>
+    <t>insulation_floor_interzonal.txt</t>
+  </si>
+  <si>
+    <t>Set Uninsulated Floor</t>
+  </si>
+  <si>
+    <t>Uninsulated Floor Sample Value</t>
+  </si>
+  <si>
+    <t>uninsulated_floor.txt</t>
+  </si>
+  <si>
+    <t>Set Uninsulated Roof</t>
+  </si>
+  <si>
+    <t>Uninsulated Roof Sample Value</t>
+  </si>
+  <si>
+    <t>uninsulated_roof.txt</t>
+  </si>
+  <si>
+    <t>Set Uninsulated Slab</t>
+  </si>
+  <si>
+    <t>Uninsulated Slab Sample Value</t>
+  </si>
+  <si>
+    <t>uninsulated_slab.txt</t>
+  </si>
+  <si>
+    <t>Set Uninsulated Walls</t>
+  </si>
+  <si>
+    <t>Uninsulated Walls Sample Value</t>
+  </si>
+  <si>
+    <t>uninsulated_walls.txt</t>
   </si>
 </sst>
 </file>
@@ -4549,8 +4702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4732,7 +4885,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>160</v>
@@ -4743,7 +4896,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>160</v>
@@ -5078,7 +5231,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5110,7 +5263,7 @@
         <v>38</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>59</v>
@@ -5205,10 +5358,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:Z81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5391,13 +5544,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>42</v>
@@ -5410,10 +5563,10 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
@@ -5421,7 +5574,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -5446,7 +5599,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>291</v>
@@ -5465,10 +5618,10 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>295</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
@@ -5476,7 +5629,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -5501,7 +5654,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>293</v>
@@ -5533,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>291</v>
@@ -5552,10 +5705,10 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>295</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
@@ -5563,7 +5716,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -5588,7 +5741,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>293</v>
@@ -5620,7 +5773,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>291</v>
@@ -5639,10 +5792,10 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>295</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
@@ -5650,7 +5803,7 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -5675,7 +5828,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="E14" s="39" t="s">
         <v>293</v>
@@ -5707,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>304</v>
+        <v>330</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>291</v>
@@ -5726,10 +5879,10 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>295</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
@@ -5737,7 +5890,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -5762,7 +5915,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="E17" s="39" t="s">
         <v>293</v>
@@ -5789,44 +5942,43 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-    </row>
-    <row r="19" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="B19" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="I19" s="10" t="s">
+        <v>316</v>
+      </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -5845,72 +5997,75 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-    </row>
-    <row r="21" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-    </row>
-    <row r="22" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I20" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="39">
+        <v>0</v>
+      </c>
+      <c r="L20" s="39">
+        <v>1</v>
+      </c>
+      <c r="M20" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N20" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R20" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>317</v>
+      </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -5929,80 +6084,83 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-    </row>
-    <row r="25" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I23" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="39">
+        <v>0</v>
+      </c>
+      <c r="L23" s="39">
+        <v>1</v>
+      </c>
+      <c r="M23" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N23" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R23" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+      <c r="I25" s="10" t="s">
+        <v>318</v>
+      </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
@@ -6013,80 +6171,83 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K26" s="39">
+        <v>0</v>
+      </c>
+      <c r="L26" s="39">
+        <v>1</v>
+      </c>
+      <c r="M26" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N26" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R26" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="G28" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
+      <c r="I28" s="10" t="s">
+        <v>321</v>
+      </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="38"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
@@ -6097,80 +6258,83 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="15"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="39">
+        <v>0</v>
+      </c>
+      <c r="L29" s="39">
+        <v>1</v>
+      </c>
+      <c r="M29" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N29" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R29" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
+      <c r="I31" s="10" t="s">
+        <v>350</v>
+      </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="38"/>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="38"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
@@ -6181,80 +6345,83 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
-    </row>
-    <row r="34" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>352</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I32" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K32" s="39">
+        <v>0</v>
+      </c>
+      <c r="L32" s="39">
+        <v>1</v>
+      </c>
+      <c r="M32" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N32" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R32" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
+      <c r="B34" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="G34" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="I34" s="10" t="s">
+        <v>296</v>
+      </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="38"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
@@ -6265,80 +6432,83 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
-      <c r="Z35" s="15"/>
-    </row>
-    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
-    </row>
-    <row r="37" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G35" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I35" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K35" s="39">
+        <v>0</v>
+      </c>
+      <c r="L35" s="39">
+        <v>1</v>
+      </c>
+      <c r="M35" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N35" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R35" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
+      <c r="B37" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>294</v>
+      </c>
       <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="I37" s="10" t="s">
+        <v>334</v>
+      </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="38"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
@@ -6349,75 +6519,78 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
-      <c r="V39" s="15"/>
-      <c r="W39" s="15"/>
-      <c r="X39" s="15"/>
-      <c r="Y39" s="15"/>
-      <c r="Z39" s="15"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
+    <row r="38" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G38" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I38" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K38" s="39">
+        <v>0</v>
+      </c>
+      <c r="L38" s="39">
+        <v>1</v>
+      </c>
+      <c r="M38" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N38" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R38" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -6433,75 +6606,78 @@
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-      <c r="X41" s="15"/>
-      <c r="Y41" s="15"/>
-      <c r="Z41" s="15"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
-      <c r="X42" s="15"/>
-      <c r="Y42" s="15"/>
-      <c r="Z42" s="15"/>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
+    <row r="41" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G41" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I41" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K41" s="39">
+        <v>0</v>
+      </c>
+      <c r="L41" s="39">
+        <v>1</v>
+      </c>
+      <c r="M41" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N41" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R41" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
@@ -6517,75 +6693,78 @@
       <c r="Y43" s="15"/>
       <c r="Z43" s="15"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="15"/>
-      <c r="Z45" s="15"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
+    <row r="44" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>339</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G44" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I44" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K44" s="39">
+        <v>0</v>
+      </c>
+      <c r="L44" s="39">
+        <v>1</v>
+      </c>
+      <c r="M44" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N44" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R44" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>341</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
@@ -6601,75 +6780,78 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-      <c r="V47" s="15"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="15"/>
-      <c r="Z47" s="15"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="15"/>
-      <c r="Z48" s="15"/>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
+    <row r="47" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="E47" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G47" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I47" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K47" s="39">
+        <v>0</v>
+      </c>
+      <c r="L47" s="39">
+        <v>1</v>
+      </c>
+      <c r="M47" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N47" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R47" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
       <c r="O49" s="15"/>
@@ -6685,75 +6867,78 @@
       <c r="Y49" s="15"/>
       <c r="Z49" s="15"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="15"/>
-      <c r="P50" s="15"/>
-      <c r="Q50" s="15"/>
-      <c r="R50" s="15"/>
-      <c r="S50" s="15"/>
-      <c r="T50" s="15"/>
-      <c r="U50" s="15"/>
-      <c r="V50" s="15"/>
-      <c r="W50" s="15"/>
-      <c r="X50" s="15"/>
-      <c r="Y50" s="15"/>
-      <c r="Z50" s="15"/>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="15"/>
-      <c r="U51" s="15"/>
-      <c r="V51" s="15"/>
-      <c r="W51" s="15"/>
-      <c r="X51" s="15"/>
-      <c r="Y51" s="15"/>
-      <c r="Z51" s="15"/>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
+    <row r="50" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I50" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K50" s="39">
+        <v>0</v>
+      </c>
+      <c r="L50" s="39">
+        <v>1</v>
+      </c>
+      <c r="M50" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N50" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R50" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>347</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
       <c r="O52" s="15"/>
@@ -6769,75 +6954,78 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="15"/>
-      <c r="U53" s="15"/>
-      <c r="V53" s="15"/>
-      <c r="W53" s="15"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="15"/>
-      <c r="Z53" s="15"/>
-    </row>
-    <row r="54" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="38"/>
-      <c r="P54" s="38"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="15"/>
-      <c r="T54" s="15"/>
-      <c r="U54" s="15"/>
-      <c r="V54" s="15"/>
-      <c r="W54" s="15"/>
-      <c r="X54" s="15"/>
-      <c r="Y54" s="15"/>
-      <c r="Z54" s="15"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
+    <row r="53" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G53" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I53" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K53" s="39">
+        <v>0</v>
+      </c>
+      <c r="L53" s="39">
+        <v>1</v>
+      </c>
+      <c r="M53" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N53" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R53" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
       <c r="O55" s="15"/>
@@ -6853,75 +7041,78 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="15"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="15"/>
-      <c r="O56" s="38"/>
-      <c r="P56" s="38"/>
-      <c r="Q56" s="15"/>
-      <c r="R56" s="15"/>
-      <c r="S56" s="15"/>
-      <c r="T56" s="15"/>
-      <c r="U56" s="15"/>
-      <c r="V56" s="15"/>
-      <c r="W56" s="15"/>
-      <c r="X56" s="15"/>
-      <c r="Y56" s="15"/>
-      <c r="Z56" s="15"/>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="38"/>
-      <c r="P57" s="38"/>
-      <c r="Q57" s="15"/>
-      <c r="R57" s="15"/>
-      <c r="S57" s="15"/>
-      <c r="T57" s="15"/>
-      <c r="U57" s="15"/>
-      <c r="V57" s="15"/>
-      <c r="W57" s="15"/>
-      <c r="X57" s="15"/>
-      <c r="Y57" s="15"/>
-      <c r="Z57" s="15"/>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
+    <row r="56" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I56" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K56" s="39">
+        <v>0</v>
+      </c>
+      <c r="L56" s="39">
+        <v>1</v>
+      </c>
+      <c r="M56" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N56" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R56" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
       <c r="O58" s="15"/>
@@ -6937,79 +7128,82 @@
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="38"/>
-      <c r="P59" s="38"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="15"/>
-      <c r="S59" s="15"/>
-      <c r="T59" s="15"/>
-      <c r="U59" s="15"/>
-      <c r="V59" s="15"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="15"/>
-      <c r="Y59" s="15"/>
-      <c r="Z59" s="15"/>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="15"/>
-      <c r="Z60" s="15"/>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
+    <row r="59" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>357</v>
+      </c>
+      <c r="E59" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G59" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I59" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K59" s="39">
+        <v>0</v>
+      </c>
+      <c r="L59" s="39">
+        <v>1</v>
+      </c>
+      <c r="M59" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N59" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R59" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B60" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E60" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
       <c r="M61" s="15"/>
       <c r="N61" s="15"/>
-      <c r="O61" s="38"/>
-      <c r="P61" s="38"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
       <c r="S61" s="15"/>
@@ -7021,75 +7215,78 @@
       <c r="Y61" s="15"/>
       <c r="Z61" s="15"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
-      <c r="J62" s="15"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="15"/>
-      <c r="P62" s="15"/>
-      <c r="Q62" s="15"/>
-      <c r="R62" s="15"/>
-      <c r="S62" s="15"/>
-      <c r="T62" s="15"/>
-      <c r="U62" s="15"/>
-      <c r="V62" s="15"/>
-      <c r="W62" s="15"/>
-      <c r="X62" s="15"/>
-      <c r="Y62" s="15"/>
-      <c r="Z62" s="15"/>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="38"/>
-      <c r="P63" s="38"/>
-      <c r="Q63" s="15"/>
-      <c r="R63" s="15"/>
-      <c r="S63" s="15"/>
-      <c r="T63" s="15"/>
-      <c r="U63" s="15"/>
-      <c r="V63" s="15"/>
-      <c r="W63" s="15"/>
-      <c r="X63" s="15"/>
-      <c r="Y63" s="15"/>
-      <c r="Z63" s="15"/>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
+    <row r="62" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="39" t="s">
+        <v>360</v>
+      </c>
+      <c r="E62" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G62" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I62" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K62" s="39">
+        <v>0</v>
+      </c>
+      <c r="L62" s="39">
+        <v>1</v>
+      </c>
+      <c r="M62" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N62" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R62" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B63" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D63" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E63" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
       <c r="M64" s="15"/>
       <c r="N64" s="15"/>
       <c r="O64" s="15"/>
@@ -7105,61 +7302,488 @@
       <c r="Y64" s="15"/>
       <c r="Z64" s="15"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="15"/>
-      <c r="Z66" s="15"/>
+    <row r="65" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="E65" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G65" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I65" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K65" s="39">
+        <v>0</v>
+      </c>
+      <c r="L65" s="39">
+        <v>1</v>
+      </c>
+      <c r="M65" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N65" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R65" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B66" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="C66" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E66" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+      <c r="U67" s="15"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="15"/>
+      <c r="X67" s="15"/>
+      <c r="Y67" s="15"/>
+      <c r="Z67" s="15"/>
+    </row>
+    <row r="68" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D68" s="39" t="s">
+        <v>366</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="G68" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="I68" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="K68" s="39">
+        <v>0</v>
+      </c>
+      <c r="L68" s="39">
+        <v>1</v>
+      </c>
+      <c r="M68" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="N68" s="39">
+        <v>0.1666667</v>
+      </c>
+      <c r="R68" s="39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="38"/>
+      <c r="P69" s="38"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="15"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
+      <c r="Z69" s="15"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="38"/>
+      <c r="P71" s="38"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="38"/>
+      <c r="P72" s="38"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="38"/>
+      <c r="P74" s="38"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="15"/>
+      <c r="Y75" s="15"/>
+      <c r="Z75" s="15"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="38"/>
+      <c r="P76" s="38"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="15"/>
+      <c r="X76" s="15"/>
+      <c r="Y76" s="15"/>
+      <c r="Z76" s="15"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="15"/>
+      <c r="X77" s="15"/>
+      <c r="Y77" s="15"/>
+      <c r="Z77" s="15"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="38"/>
+      <c r="P78" s="38"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="15"/>
+      <c r="X78" s="15"/>
+      <c r="Y78" s="15"/>
+      <c r="Z78" s="15"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A79" s="15"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
+      <c r="S79" s="15"/>
+      <c r="T79" s="15"/>
+      <c r="U79" s="15"/>
+      <c r="V79" s="15"/>
+      <c r="W79" s="15"/>
+      <c r="X79" s="15"/>
+      <c r="Y79" s="15"/>
+      <c r="Z79" s="15"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A80" s="15"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="38"/>
+      <c r="P80" s="38"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="15"/>
+      <c r="X80" s="15"/>
+      <c r="Y80" s="15"/>
+      <c r="Z80" s="15"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A81" s="15"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+      <c r="Q81" s="15"/>
+      <c r="R81" s="15"/>
+      <c r="S81" s="15"/>
+      <c r="T81" s="15"/>
+      <c r="U81" s="15"/>
+      <c r="V81" s="15"/>
+      <c r="W81" s="15"/>
+      <c r="X81" s="15"/>
+      <c r="Y81" s="15"/>
+      <c r="Z81" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -7180,9 +7804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7316,10 +7940,10 @@
         <v>41</v>
       </c>
       <c r="G4" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="15" t="b">
         <v>1</v>
@@ -7351,10 +7975,10 @@
         <v>41</v>
       </c>
       <c r="G5" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="15" t="b">
         <v>1</v>
@@ -7387,7 +8011,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="15" t="b">
         <v>0</v>
@@ -7416,7 +8040,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="15" t="b">
         <v>0</v>
@@ -7445,7 +8069,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="15" t="b">
         <v>0</v>
@@ -7474,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="15" t="b">
         <v>0</v>
@@ -7503,7 +8127,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="15" t="b">
         <v>0</v>
@@ -7532,7 +8156,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="15" t="b">
         <v>0</v>
@@ -7561,7 +8185,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="15" t="b">
         <v>0</v>
@@ -7590,7 +8214,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="15" t="b">
         <v>0</v>
@@ -7619,7 +8243,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="15" t="b">
         <v>0</v>
@@ -7648,7 +8272,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="15" t="b">
         <v>0</v>
@@ -7677,7 +8301,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="15" t="b">
         <v>0</v>
@@ -7706,7 +8330,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="15" t="b">
         <v>0</v>
@@ -7735,7 +8359,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="15" t="b">
         <v>0</v>
@@ -7764,7 +8388,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="15" t="b">
         <v>0</v>
@@ -7793,7 +8417,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="15" t="b">
         <v>0</v>
@@ -7822,7 +8446,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="15" t="b">
         <v>0</v>
@@ -7851,7 +8475,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="15" t="b">
         <v>0</v>
@@ -7880,7 +8504,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="15" t="b">
         <v>0</v>
@@ -7909,7 +8533,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="15" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added more envelope measures into the workflow.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="401">
   <si>
     <t>type</t>
   </si>
@@ -1143,6 +1143,105 @@
   </si>
   <si>
     <t>uninsulated_walls.txt</t>
+  </si>
+  <si>
+    <t>Set Wall Sheathing</t>
+  </si>
+  <si>
+    <t>Wall Sheathing Sample Value</t>
+  </si>
+  <si>
+    <t>wall_sheathing.txt</t>
+  </si>
+  <si>
+    <t>Set Exterior Finish</t>
+  </si>
+  <si>
+    <t>Exterior Finish Sample Value</t>
+  </si>
+  <si>
+    <t>exterior_finish.txt</t>
+  </si>
+  <si>
+    <t>Set Roof Material</t>
+  </si>
+  <si>
+    <t>Roof Material Sample Value</t>
+  </si>
+  <si>
+    <t>roof_material.txt</t>
+  </si>
+  <si>
+    <t>Set Floor Covering</t>
+  </si>
+  <si>
+    <t>Floor Covering Sample Value</t>
+  </si>
+  <si>
+    <t>floor_covering.txt</t>
+  </si>
+  <si>
+    <t>Set Floor Mass</t>
+  </si>
+  <si>
+    <t>Floor Mass Sample Value</t>
+  </si>
+  <si>
+    <t>mass_floor.txt</t>
+  </si>
+  <si>
+    <t>Set Exterior Wall Mass</t>
+  </si>
+  <si>
+    <t>Exterior Wall Mass Sample Value</t>
+  </si>
+  <si>
+    <t>mass_exterior_wall.txt</t>
+  </si>
+  <si>
+    <t>Set Partition Wall Mass</t>
+  </si>
+  <si>
+    <t>Partition Wall Mass Sample Value</t>
+  </si>
+  <si>
+    <t>mass_partition_wall.txt</t>
+  </si>
+  <si>
+    <t>Set Ceiling Mass</t>
+  </si>
+  <si>
+    <t>Ceiling Mass Sample Value</t>
+  </si>
+  <si>
+    <t>mass_ceiling.txt</t>
+  </si>
+  <si>
+    <t>Set Orientation</t>
+  </si>
+  <si>
+    <t>Orientation Sample Value</t>
+  </si>
+  <si>
+    <t>orientation.txt</t>
+  </si>
+  <si>
+    <t>Set Door Area</t>
+  </si>
+  <si>
+    <t>Door Area Sample Value</t>
+  </si>
+  <si>
+    <t>door_area.txt</t>
+  </si>
+  <si>
+    <t>Set Doors</t>
+  </si>
+  <si>
+    <t>Doors Sample Value</t>
+  </si>
+  <si>
+    <t>doors.txt</t>
   </si>
 </sst>
 </file>
@@ -2806,7 +2905,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2887,9 +2986,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -5238,7 +5334,7 @@
       <c r="A42" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="39" t="s">
         <v>63</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -5358,10 +5454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z81"/>
+  <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5416,14 +5512,14 @@
       <c r="R1" s="31"/>
       <c r="S1" s="28"/>
       <c r="T1" s="28"/>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -5649,35 +5745,35 @@
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+    <row r="8" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="38">
         <v>0.5</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="38">
         <v>0</v>
       </c>
-      <c r="L8" s="39">
+      <c r="L8" s="38">
         <v>1</v>
       </c>
-      <c r="M8" s="39">
+      <c r="M8" s="38">
         <v>0.5</v>
       </c>
-      <c r="N8" s="39">
+      <c r="N8" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R8" s="39" t="s">
+      <c r="R8" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5736,35 +5832,35 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="38">
         <v>0.5</v>
       </c>
-      <c r="K11" s="39">
+      <c r="K11" s="38">
         <v>0</v>
       </c>
-      <c r="L11" s="39">
+      <c r="L11" s="38">
         <v>1</v>
       </c>
-      <c r="M11" s="39">
+      <c r="M11" s="38">
         <v>0.5</v>
       </c>
-      <c r="N11" s="39">
+      <c r="N11" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R11" s="39" t="s">
+      <c r="R11" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5823,35 +5919,35 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+    <row r="14" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>0.5</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="38">
         <v>0</v>
       </c>
-      <c r="L14" s="39">
+      <c r="L14" s="38">
         <v>1</v>
       </c>
-      <c r="M14" s="39">
+      <c r="M14" s="38">
         <v>0.5</v>
       </c>
-      <c r="N14" s="39">
+      <c r="N14" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R14" s="39" t="s">
+      <c r="R14" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5910,35 +6006,35 @@
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
     </row>
-    <row r="17" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+    <row r="17" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="38">
         <v>0.5</v>
       </c>
-      <c r="K17" s="39">
+      <c r="K17" s="38">
         <v>0</v>
       </c>
-      <c r="L17" s="39">
+      <c r="L17" s="38">
         <v>1</v>
       </c>
-      <c r="M17" s="39">
+      <c r="M17" s="38">
         <v>0.5</v>
       </c>
-      <c r="N17" s="39">
+      <c r="N17" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R17" s="39" t="s">
+      <c r="R17" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5997,35 +6093,35 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39" t="s">
+    <row r="20" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="38" t="s">
         <v>329</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="38">
         <v>0.5</v>
       </c>
-      <c r="K20" s="39">
+      <c r="K20" s="38">
         <v>0</v>
       </c>
-      <c r="L20" s="39">
+      <c r="L20" s="38">
         <v>1</v>
       </c>
-      <c r="M20" s="39">
+      <c r="M20" s="38">
         <v>0.5</v>
       </c>
-      <c r="N20" s="39">
+      <c r="N20" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R20" s="39" t="s">
+      <c r="R20" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6084,35 +6180,35 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
+    <row r="23" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="38">
         <v>0.5</v>
       </c>
-      <c r="K23" s="39">
+      <c r="K23" s="38">
         <v>0</v>
       </c>
-      <c r="L23" s="39">
+      <c r="L23" s="38">
         <v>1</v>
       </c>
-      <c r="M23" s="39">
+      <c r="M23" s="38">
         <v>0.5</v>
       </c>
-      <c r="N23" s="39">
+      <c r="N23" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R23" s="39" t="s">
+      <c r="R23" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6171,35 +6267,35 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+    <row r="26" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G26" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="38">
         <v>0.5</v>
       </c>
-      <c r="K26" s="39">
+      <c r="K26" s="38">
         <v>0</v>
       </c>
-      <c r="L26" s="39">
+      <c r="L26" s="38">
         <v>1</v>
       </c>
-      <c r="M26" s="39">
+      <c r="M26" s="38">
         <v>0.5</v>
       </c>
-      <c r="N26" s="39">
+      <c r="N26" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R26" s="39" t="s">
+      <c r="R26" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6258,35 +6354,35 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+    <row r="29" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I29" s="39">
+      <c r="I29" s="38">
         <v>0.5</v>
       </c>
-      <c r="K29" s="39">
+      <c r="K29" s="38">
         <v>0</v>
       </c>
-      <c r="L29" s="39">
+      <c r="L29" s="38">
         <v>1</v>
       </c>
-      <c r="M29" s="39">
+      <c r="M29" s="38">
         <v>0.5</v>
       </c>
-      <c r="N29" s="39">
+      <c r="N29" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R29" s="39" t="s">
+      <c r="R29" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6295,7 +6391,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>351</v>
+        <v>392</v>
       </c>
       <c r="C30" s="37" t="s">
         <v>291</v>
@@ -6325,7 +6421,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -6345,35 +6441,35 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="39" t="s">
+    <row r="32" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="39" t="s">
-        <v>352</v>
-      </c>
-      <c r="E32" s="39" t="s">
+      <c r="D32" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="E32" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="38">
         <v>0.5</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K32" s="38">
         <v>0</v>
       </c>
-      <c r="L32" s="39">
+      <c r="L32" s="38">
         <v>1</v>
       </c>
-      <c r="M32" s="39">
+      <c r="M32" s="38">
         <v>0.5</v>
       </c>
-      <c r="N32" s="39">
+      <c r="N32" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R32" s="39" t="s">
+      <c r="R32" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6382,7 +6478,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="C33" s="37" t="s">
         <v>291</v>
@@ -6412,7 +6508,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>296</v>
+        <v>350</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -6432,35 +6528,35 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="s">
+    <row r="35" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="39" t="s">
-        <v>323</v>
-      </c>
-      <c r="E35" s="39" t="s">
+      <c r="D35" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="E35" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G35" s="39" t="s">
+      <c r="G35" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I35" s="39">
+      <c r="I35" s="38">
         <v>0.5</v>
       </c>
-      <c r="K35" s="39">
+      <c r="K35" s="38">
         <v>0</v>
       </c>
-      <c r="L35" s="39">
+      <c r="L35" s="38">
         <v>1</v>
       </c>
-      <c r="M35" s="39">
+      <c r="M35" s="38">
         <v>0.5</v>
       </c>
-      <c r="N35" s="39">
+      <c r="N35" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R35" s="39" t="s">
+      <c r="R35" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6469,7 +6565,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>291</v>
@@ -6499,7 +6595,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>334</v>
+        <v>296</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -6519,35 +6615,35 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="39" t="s">
+    <row r="38" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="39" t="s">
-        <v>333</v>
-      </c>
-      <c r="E38" s="39" t="s">
+      <c r="D38" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="E38" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G38" s="39" t="s">
+      <c r="G38" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I38" s="39">
+      <c r="I38" s="38">
         <v>0.5</v>
       </c>
-      <c r="K38" s="39">
+      <c r="K38" s="38">
         <v>0</v>
       </c>
-      <c r="L38" s="39">
+      <c r="L38" s="38">
         <v>1</v>
       </c>
-      <c r="M38" s="39">
+      <c r="M38" s="38">
         <v>0.5</v>
       </c>
-      <c r="N38" s="39">
+      <c r="N38" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R38" s="39" t="s">
+      <c r="R38" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6556,7 +6652,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C39" s="37" t="s">
         <v>291</v>
@@ -6586,7 +6682,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -6606,35 +6702,35 @@
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="39" t="s">
+    <row r="41" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="39" t="s">
-        <v>336</v>
-      </c>
-      <c r="E41" s="39" t="s">
+      <c r="D41" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="E41" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G41" s="39" t="s">
+      <c r="G41" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I41" s="39">
+      <c r="I41" s="38">
         <v>0.5</v>
       </c>
-      <c r="K41" s="39">
+      <c r="K41" s="38">
         <v>0</v>
       </c>
-      <c r="L41" s="39">
+      <c r="L41" s="38">
         <v>1</v>
       </c>
-      <c r="M41" s="39">
+      <c r="M41" s="38">
         <v>0.5</v>
       </c>
-      <c r="N41" s="39">
+      <c r="N41" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R41" s="39" t="s">
+      <c r="R41" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6643,7 +6739,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>291</v>
@@ -6673,7 +6769,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -6693,35 +6789,35 @@
       <c r="Y43" s="15"/>
       <c r="Z43" s="15"/>
     </row>
-    <row r="44" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="39" t="s">
+    <row r="44" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="39" t="s">
-        <v>339</v>
-      </c>
-      <c r="E44" s="39" t="s">
+      <c r="D44" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="E44" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G44" s="39" t="s">
+      <c r="G44" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I44" s="39">
+      <c r="I44" s="38">
         <v>0.5</v>
       </c>
-      <c r="K44" s="39">
+      <c r="K44" s="38">
         <v>0</v>
       </c>
-      <c r="L44" s="39">
+      <c r="L44" s="38">
         <v>1</v>
       </c>
-      <c r="M44" s="39">
+      <c r="M44" s="38">
         <v>0.5</v>
       </c>
-      <c r="N44" s="39">
+      <c r="N44" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R44" s="39" t="s">
+      <c r="R44" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6730,7 +6826,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C45" s="37" t="s">
         <v>291</v>
@@ -6760,7 +6856,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -6780,35 +6876,35 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="39" t="s">
+    <row r="47" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="39" t="s">
-        <v>342</v>
-      </c>
-      <c r="E47" s="39" t="s">
+      <c r="D47" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="E47" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G47" s="39" t="s">
+      <c r="G47" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I47" s="39">
+      <c r="I47" s="38">
         <v>0.5</v>
       </c>
-      <c r="K47" s="39">
+      <c r="K47" s="38">
         <v>0</v>
       </c>
-      <c r="L47" s="39">
+      <c r="L47" s="38">
         <v>1</v>
       </c>
-      <c r="M47" s="39">
+      <c r="M47" s="38">
         <v>0.5</v>
       </c>
-      <c r="N47" s="39">
+      <c r="N47" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R47" s="39" t="s">
+      <c r="R47" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6817,7 +6913,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C48" s="37" t="s">
         <v>291</v>
@@ -6847,7 +6943,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -6867,44 +6963,44 @@
       <c r="Y49" s="15"/>
       <c r="Z49" s="15"/>
     </row>
-    <row r="50" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="39" t="s">
+    <row r="50" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D50" s="39" t="s">
-        <v>345</v>
-      </c>
-      <c r="E50" s="39" t="s">
+      <c r="D50" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="E50" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G50" s="39" t="s">
+      <c r="G50" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I50" s="39">
+      <c r="I50" s="38">
         <v>0.5</v>
       </c>
-      <c r="K50" s="39">
+      <c r="K50" s="38">
         <v>0</v>
       </c>
-      <c r="L50" s="39">
+      <c r="L50" s="38">
         <v>1</v>
       </c>
-      <c r="M50" s="39">
+      <c r="M50" s="38">
         <v>0.5</v>
       </c>
-      <c r="N50" s="39">
+      <c r="N50" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R50" s="39" t="s">
+      <c r="R50" s="38" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C51" s="37" t="s">
         <v>291</v>
@@ -6934,7 +7030,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -6954,44 +7050,44 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
     </row>
-    <row r="53" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="39" t="s">
+    <row r="53" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="39" t="s">
-        <v>348</v>
-      </c>
-      <c r="E53" s="39" t="s">
+      <c r="D53" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="E53" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G53" s="39" t="s">
+      <c r="G53" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I53" s="39">
+      <c r="I53" s="38">
         <v>0.5</v>
       </c>
-      <c r="K53" s="39">
+      <c r="K53" s="38">
         <v>0</v>
       </c>
-      <c r="L53" s="39">
+      <c r="L53" s="38">
         <v>1</v>
       </c>
-      <c r="M53" s="39">
+      <c r="M53" s="38">
         <v>0.5</v>
       </c>
-      <c r="N53" s="39">
+      <c r="N53" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R53" s="39" t="s">
+      <c r="R53" s="38" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C54" s="37" t="s">
         <v>291</v>
@@ -7021,7 +7117,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -7041,35 +7137,35 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
     </row>
-    <row r="56" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="39" t="s">
+    <row r="56" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="39" t="s">
-        <v>353</v>
-      </c>
-      <c r="E56" s="39" t="s">
+      <c r="D56" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="E56" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G56" s="39" t="s">
+      <c r="G56" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I56" s="39">
+      <c r="I56" s="38">
         <v>0.5</v>
       </c>
-      <c r="K56" s="39">
+      <c r="K56" s="38">
         <v>0</v>
       </c>
-      <c r="L56" s="39">
+      <c r="L56" s="38">
         <v>1</v>
       </c>
-      <c r="M56" s="39">
+      <c r="M56" s="38">
         <v>0.5</v>
       </c>
-      <c r="N56" s="39">
+      <c r="N56" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R56" s="39" t="s">
+      <c r="R56" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7078,7 +7174,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C57" s="37" t="s">
         <v>291</v>
@@ -7108,7 +7204,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -7128,35 +7224,35 @@
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
     </row>
-    <row r="59" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="39" t="s">
+    <row r="59" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="39" t="s">
-        <v>357</v>
-      </c>
-      <c r="E59" s="39" t="s">
+      <c r="D59" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="E59" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G59" s="39" t="s">
+      <c r="G59" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I59" s="39">
+      <c r="I59" s="38">
         <v>0.5</v>
       </c>
-      <c r="K59" s="39">
+      <c r="K59" s="38">
         <v>0</v>
       </c>
-      <c r="L59" s="39">
+      <c r="L59" s="38">
         <v>1</v>
       </c>
-      <c r="M59" s="39">
+      <c r="M59" s="38">
         <v>0.5</v>
       </c>
-      <c r="N59" s="39">
+      <c r="N59" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R59" s="39" t="s">
+      <c r="R59" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7165,7 +7261,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C60" s="37" t="s">
         <v>291</v>
@@ -7195,7 +7291,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -7215,35 +7311,35 @@
       <c r="Y61" s="15"/>
       <c r="Z61" s="15"/>
     </row>
-    <row r="62" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="39" t="s">
+    <row r="62" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D62" s="39" t="s">
-        <v>360</v>
-      </c>
-      <c r="E62" s="39" t="s">
+      <c r="D62" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="E62" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G62" s="39" t="s">
+      <c r="G62" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I62" s="39">
+      <c r="I62" s="38">
         <v>0.5</v>
       </c>
-      <c r="K62" s="39">
+      <c r="K62" s="38">
         <v>0</v>
       </c>
-      <c r="L62" s="39">
+      <c r="L62" s="38">
         <v>1</v>
       </c>
-      <c r="M62" s="39">
+      <c r="M62" s="38">
         <v>0.5</v>
       </c>
-      <c r="N62" s="39">
+      <c r="N62" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R62" s="39" t="s">
+      <c r="R62" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7252,7 +7348,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C63" s="37" t="s">
         <v>291</v>
@@ -7282,7 +7378,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -7302,35 +7398,35 @@
       <c r="Y64" s="15"/>
       <c r="Z64" s="15"/>
     </row>
-    <row r="65" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="39" t="s">
+    <row r="65" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="39" t="s">
-        <v>363</v>
-      </c>
-      <c r="E65" s="39" t="s">
+      <c r="D65" s="38" t="s">
+        <v>360</v>
+      </c>
+      <c r="E65" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G65" s="39" t="s">
+      <c r="G65" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I65" s="39">
+      <c r="I65" s="38">
         <v>0.5</v>
       </c>
-      <c r="K65" s="39">
+      <c r="K65" s="38">
         <v>0</v>
       </c>
-      <c r="L65" s="39">
+      <c r="L65" s="38">
         <v>1</v>
       </c>
-      <c r="M65" s="39">
+      <c r="M65" s="38">
         <v>0.5</v>
       </c>
-      <c r="N65" s="39">
+      <c r="N65" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R65" s="39" t="s">
+      <c r="R65" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7339,7 +7435,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C66" s="37" t="s">
         <v>291</v>
@@ -7369,7 +7465,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -7389,79 +7485,78 @@
       <c r="Y67" s="15"/>
       <c r="Z67" s="15"/>
     </row>
-    <row r="68" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="39" t="s">
+    <row r="68" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="39" t="s">
-        <v>366</v>
-      </c>
-      <c r="E68" s="39" t="s">
+      <c r="D68" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="E68" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="G68" s="39" t="s">
+      <c r="G68" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I68" s="39">
+      <c r="I68" s="38">
         <v>0.5</v>
       </c>
-      <c r="K68" s="39">
+      <c r="K68" s="38">
         <v>0</v>
       </c>
-      <c r="L68" s="39">
+      <c r="L68" s="38">
         <v>1</v>
       </c>
-      <c r="M68" s="39">
+      <c r="M68" s="38">
         <v>0.5</v>
       </c>
-      <c r="N68" s="39">
+      <c r="N68" s="38">
         <v>0.1666667</v>
       </c>
-      <c r="R68" s="39" t="s">
+      <c r="R68" s="38" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="38"/>
-      <c r="P69" s="38"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="15"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="15"/>
-      <c r="X69" s="15"/>
-      <c r="Y69" s="15"/>
-      <c r="Z69" s="15"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
+    <row r="69" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B69" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E69" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
       <c r="O70" s="15"/>
@@ -7477,75 +7572,78 @@
       <c r="Y70" s="15"/>
       <c r="Z70" s="15"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15"/>
-      <c r="K71" s="15"/>
-      <c r="L71" s="15"/>
-      <c r="M71" s="15"/>
-      <c r="N71" s="15"/>
-      <c r="O71" s="38"/>
-      <c r="P71" s="38"/>
-      <c r="Q71" s="15"/>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="15"/>
-      <c r="V71" s="15"/>
-      <c r="W71" s="15"/>
-      <c r="X71" s="15"/>
-      <c r="Y71" s="15"/>
-      <c r="Z71" s="15"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="15"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15"/>
-      <c r="K72" s="15"/>
-      <c r="L72" s="15"/>
-      <c r="M72" s="15"/>
-      <c r="N72" s="15"/>
-      <c r="O72" s="38"/>
-      <c r="P72" s="38"/>
-      <c r="Q72" s="15"/>
-      <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="15"/>
-      <c r="U72" s="15"/>
-      <c r="V72" s="15"/>
-      <c r="W72" s="15"/>
-      <c r="X72" s="15"/>
-      <c r="Y72" s="15"/>
-      <c r="Z72" s="15"/>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="15"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15"/>
-      <c r="K73" s="15"/>
-      <c r="L73" s="15"/>
+    <row r="71" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>366</v>
+      </c>
+      <c r="E71" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G71" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I71" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K71" s="38">
+        <v>0</v>
+      </c>
+      <c r="L71" s="38">
+        <v>1</v>
+      </c>
+      <c r="M71" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N71" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R71" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B72" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C72" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E72" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
       <c r="O73" s="15"/>
@@ -7561,79 +7659,82 @@
       <c r="Y73" s="15"/>
       <c r="Z73" s="15"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
-      <c r="H74" s="15"/>
-      <c r="I74" s="15"/>
-      <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
-      <c r="L74" s="15"/>
-      <c r="M74" s="15"/>
-      <c r="N74" s="15"/>
-      <c r="O74" s="38"/>
-      <c r="P74" s="38"/>
-      <c r="Q74" s="15"/>
-      <c r="R74" s="15"/>
-      <c r="S74" s="15"/>
-      <c r="T74" s="15"/>
-      <c r="U74" s="15"/>
-      <c r="V74" s="15"/>
-      <c r="W74" s="15"/>
-      <c r="X74" s="15"/>
-      <c r="Y74" s="15"/>
-      <c r="Z74" s="15"/>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="15"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="15"/>
-      <c r="R75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="15"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="15"/>
-      <c r="X75" s="15"/>
-      <c r="Y75" s="15"/>
-      <c r="Z75" s="15"/>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
-      <c r="H76" s="15"/>
-      <c r="I76" s="15"/>
-      <c r="J76" s="15"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="15"/>
+    <row r="74" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>369</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G74" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I74" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K74" s="38">
+        <v>0</v>
+      </c>
+      <c r="L74" s="38">
+        <v>1</v>
+      </c>
+      <c r="M74" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N74" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R74" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B75" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="C75" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D75" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E75" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="B76" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
-      <c r="O76" s="38"/>
-      <c r="P76" s="38"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
       <c r="S76" s="15"/>
@@ -7645,75 +7746,78 @@
       <c r="Y76" s="15"/>
       <c r="Z76" s="15"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
-      <c r="P77" s="15"/>
-      <c r="Q77" s="15"/>
-      <c r="R77" s="15"/>
-      <c r="S77" s="15"/>
-      <c r="T77" s="15"/>
-      <c r="U77" s="15"/>
-      <c r="V77" s="15"/>
-      <c r="W77" s="15"/>
-      <c r="X77" s="15"/>
-      <c r="Y77" s="15"/>
-      <c r="Z77" s="15"/>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="15"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="38"/>
-      <c r="P78" s="38"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="15"/>
-      <c r="V78" s="15"/>
-      <c r="W78" s="15"/>
-      <c r="X78" s="15"/>
-      <c r="Y78" s="15"/>
-      <c r="Z78" s="15"/>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
+    <row r="77" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>372</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G77" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I77" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K77" s="38">
+        <v>0</v>
+      </c>
+      <c r="L77" s="38">
+        <v>1</v>
+      </c>
+      <c r="M77" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N77" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R77" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B78" s="37" t="s">
+        <v>374</v>
+      </c>
+      <c r="C78" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D78" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E78" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="B79" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="J79" s="10"/>
+      <c r="K79" s="10"/>
+      <c r="L79" s="10"/>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
       <c r="O79" s="15"/>
@@ -7729,61 +7833,646 @@
       <c r="Y79" s="15"/>
       <c r="Z79" s="15"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="38"/>
-      <c r="P80" s="38"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="15"/>
-      <c r="U80" s="15"/>
-      <c r="V80" s="15"/>
-      <c r="W80" s="15"/>
-      <c r="X80" s="15"/>
-      <c r="Y80" s="15"/>
-      <c r="Z80" s="15"/>
-    </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="15"/>
-      <c r="V81" s="15"/>
-      <c r="W81" s="15"/>
-      <c r="X81" s="15"/>
-      <c r="Y81" s="15"/>
-      <c r="Z81" s="15"/>
+    <row r="80" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="E80" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G80" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I80" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K80" s="38">
+        <v>0</v>
+      </c>
+      <c r="L80" s="38">
+        <v>1</v>
+      </c>
+      <c r="M80" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N80" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R80" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B81" s="37" t="s">
+        <v>377</v>
+      </c>
+      <c r="C81" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D81" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E81" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="10"/>
+      <c r="B82" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15"/>
+      <c r="Q82" s="15"/>
+      <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="15"/>
+      <c r="U82" s="15"/>
+      <c r="V82" s="15"/>
+      <c r="W82" s="15"/>
+      <c r="X82" s="15"/>
+      <c r="Y82" s="15"/>
+      <c r="Z82" s="15"/>
+    </row>
+    <row r="83" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="E83" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I83" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K83" s="38">
+        <v>0</v>
+      </c>
+      <c r="L83" s="38">
+        <v>1</v>
+      </c>
+      <c r="M83" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N83" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R83" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B84" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="C84" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D84" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E84" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10"/>
+      <c r="B85" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="15"/>
+      <c r="U85" s="15"/>
+      <c r="V85" s="15"/>
+      <c r="W85" s="15"/>
+      <c r="X85" s="15"/>
+      <c r="Y85" s="15"/>
+      <c r="Z85" s="15"/>
+    </row>
+    <row r="86" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D86" s="38" t="s">
+        <v>381</v>
+      </c>
+      <c r="E86" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G86" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I86" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K86" s="38">
+        <v>0</v>
+      </c>
+      <c r="L86" s="38">
+        <v>1</v>
+      </c>
+      <c r="M86" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N86" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R86" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B87" s="37" t="s">
+        <v>383</v>
+      </c>
+      <c r="C87" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D87" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E87" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="B88" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="O88" s="15"/>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15"/>
+      <c r="S88" s="15"/>
+      <c r="T88" s="15"/>
+      <c r="U88" s="15"/>
+      <c r="V88" s="15"/>
+      <c r="W88" s="15"/>
+      <c r="X88" s="15"/>
+      <c r="Y88" s="15"/>
+      <c r="Z88" s="15"/>
+    </row>
+    <row r="89" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89" s="38" t="s">
+        <v>384</v>
+      </c>
+      <c r="E89" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G89" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I89" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K89" s="38">
+        <v>0</v>
+      </c>
+      <c r="L89" s="38">
+        <v>1</v>
+      </c>
+      <c r="M89" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N89" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R89" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B90" s="37" t="s">
+        <v>386</v>
+      </c>
+      <c r="C90" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D90" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E90" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="15"/>
+      <c r="N91" s="15"/>
+      <c r="O91" s="15"/>
+      <c r="P91" s="15"/>
+      <c r="Q91" s="15"/>
+      <c r="R91" s="15"/>
+      <c r="S91" s="15"/>
+      <c r="T91" s="15"/>
+      <c r="U91" s="15"/>
+      <c r="V91" s="15"/>
+      <c r="W91" s="15"/>
+      <c r="X91" s="15"/>
+      <c r="Y91" s="15"/>
+      <c r="Z91" s="15"/>
+    </row>
+    <row r="92" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" s="38" t="s">
+        <v>387</v>
+      </c>
+      <c r="E92" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G92" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I92" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K92" s="38">
+        <v>0</v>
+      </c>
+      <c r="L92" s="38">
+        <v>1</v>
+      </c>
+      <c r="M92" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N92" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R92" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B93" s="37" t="s">
+        <v>389</v>
+      </c>
+      <c r="C93" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D93" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E93" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="15"/>
+      <c r="O94" s="15"/>
+      <c r="P94" s="15"/>
+      <c r="Q94" s="15"/>
+      <c r="R94" s="15"/>
+      <c r="S94" s="15"/>
+      <c r="T94" s="15"/>
+      <c r="U94" s="15"/>
+      <c r="V94" s="15"/>
+      <c r="W94" s="15"/>
+      <c r="X94" s="15"/>
+      <c r="Y94" s="15"/>
+      <c r="Z94" s="15"/>
+    </row>
+    <row r="95" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D95" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="E95" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I95" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K95" s="38">
+        <v>0</v>
+      </c>
+      <c r="L95" s="38">
+        <v>1</v>
+      </c>
+      <c r="M95" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N95" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R95" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B96" s="37" t="s">
+        <v>395</v>
+      </c>
+      <c r="C96" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D96" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E96" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="10"/>
+      <c r="B97" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="15"/>
+      <c r="O97" s="15"/>
+      <c r="P97" s="15"/>
+      <c r="Q97" s="15"/>
+      <c r="R97" s="15"/>
+      <c r="S97" s="15"/>
+      <c r="T97" s="15"/>
+      <c r="U97" s="15"/>
+      <c r="V97" s="15"/>
+      <c r="W97" s="15"/>
+      <c r="X97" s="15"/>
+      <c r="Y97" s="15"/>
+      <c r="Z97" s="15"/>
+    </row>
+    <row r="98" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="E98" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G98" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I98" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K98" s="38">
+        <v>0</v>
+      </c>
+      <c r="L98" s="38">
+        <v>1</v>
+      </c>
+      <c r="M98" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N98" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R98" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B99" s="37" t="s">
+        <v>398</v>
+      </c>
+      <c r="C99" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="D99" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="E99" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10"/>
+      <c r="B100" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="J100" s="10"/>
+      <c r="K100" s="10"/>
+      <c r="L100" s="10"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="15"/>
+      <c r="O100" s="15"/>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="15"/>
+      <c r="R100" s="15"/>
+      <c r="S100" s="15"/>
+      <c r="T100" s="15"/>
+      <c r="U100" s="15"/>
+      <c r="V100" s="15"/>
+      <c r="W100" s="15"/>
+      <c r="X100" s="15"/>
+      <c r="Y100" s="15"/>
+      <c r="Z100" s="15"/>
+    </row>
+    <row r="101" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="E101" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G101" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="I101" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K101" s="38">
+        <v>0</v>
+      </c>
+      <c r="L101" s="38">
+        <v>1</v>
+      </c>
+      <c r="M101" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="N101" s="38">
+        <v>0.1666667</v>
+      </c>
+      <c r="R101" s="38" t="s">
+        <v>279</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -7804,7 +8493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>

</xml_diff>

<commit_message>
Reporting measure stub for getting option names in the results csv.
Will be fully implemented when runner.past_results in a reporting
measure works correctly.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="369">
   <si>
     <t>type</t>
   </si>
@@ -641,132 +641,18 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Unmet Cooling Hours</t>
-  </si>
-  <si>
-    <t>hrs</t>
-  </si>
-  <si>
-    <t>Unmet Heating Hours</t>
-  </si>
-  <si>
-    <t>Total Unmet Hours</t>
-  </si>
-  <si>
     <t>Building Area</t>
   </si>
   <si>
     <t>m2</t>
   </si>
   <si>
-    <t>Natural Gas Heating Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heating_natural_gas</t>
-  </si>
-  <si>
-    <t>Cooling Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.cooling_electricity</t>
-  </si>
-  <si>
-    <t>Interior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Exterior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_natural_gas</t>
-  </si>
-  <si>
-    <t>Experior Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Fans Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.fans_electricity</t>
-  </si>
-  <si>
-    <t>Pumps Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.pumps_electricity</t>
-  </si>
-  <si>
-    <t>Heat Rejection Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heat_rejection_electricity</t>
-  </si>
-  <si>
-    <t>Humidification Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.humidification_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_natural_gas</t>
-  </si>
-  <si>
-    <t>Refrigeration Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.refrigeration_electricity</t>
-  </si>
-  <si>
-    <t>Total Life Cycle Cost</t>
-  </si>
-  <si>
-    <t>standard_report.total_life_cycle_cost</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>NG EUI</t>
   </si>
   <si>
     <t>Elec EUI</t>
   </si>
   <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_cooling</t>
-  </si>
-  <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_heating</t>
-  </si>
-  <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_hours</t>
-  </si>
-  <si>
     <t>standard_reports.total_building_area</t>
   </si>
   <si>
@@ -1242,6 +1128,24 @@
   </si>
   <si>
     <t>doors.txt</t>
+  </si>
+  <si>
+    <t>ReportingMeasure</t>
+  </si>
+  <si>
+    <t>Res Stock Reporting</t>
+  </si>
+  <si>
+    <t>ResStockReporting</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Test Value</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.test_value</t>
   </si>
 </sst>
 </file>
@@ -2905,7 +2809,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2990,6 +2894,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4799,7 +4705,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4837,7 +4743,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>46</v>
@@ -4848,7 +4754,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>67</v>
@@ -4859,7 +4765,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>159</v>
@@ -4870,7 +4776,7 @@
         <v>80</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>82</v>
@@ -4938,21 +4844,21 @@
         <v>$0.28/hour</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>246</v>
+        <v>208</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -4970,7 +4876,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>81</v>
@@ -4981,7 +4887,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>160</v>
@@ -4992,7 +4898,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>160</v>
@@ -5017,7 +4923,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5327,7 +5233,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5353,13 +5259,13 @@
         <v>29</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>59</v>
@@ -5383,18 +5289,18 @@
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="8" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5409,18 +5315,18 @@
     </row>
     <row r="51" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" s="8" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -5454,10 +5360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z101"/>
+  <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5512,14 +5418,14 @@
       <c r="R1" s="31"/>
       <c r="S1" s="28"/>
       <c r="T1" s="28"/>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -5640,13 +5546,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>42</v>
@@ -5659,18 +5565,18 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -5695,13 +5601,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>42</v>
@@ -5714,18 +5620,18 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -5750,10 +5656,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G8" s="38" t="s">
         <v>174</v>
@@ -5774,7 +5680,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R8" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -5782,13 +5688,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>42</v>
@@ -5801,18 +5707,18 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -5837,10 +5743,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G11" s="38" t="s">
         <v>174</v>
@@ -5861,7 +5767,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R11" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -5869,13 +5775,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>42</v>
@@ -5888,18 +5794,18 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -5924,10 +5830,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G14" s="38" t="s">
         <v>174</v>
@@ -5948,7 +5854,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R14" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -5956,13 +5862,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>330</v>
+        <v>292</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E15" s="37" t="s">
         <v>42</v>
@@ -5975,18 +5881,18 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6011,10 +5917,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>331</v>
+        <v>293</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G17" s="38" t="s">
         <v>174</v>
@@ -6035,7 +5941,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R17" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6043,13 +5949,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E18" s="37" t="s">
         <v>42</v>
@@ -6062,18 +5968,18 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6098,10 +6004,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G20" s="38" t="s">
         <v>174</v>
@@ -6122,7 +6028,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R20" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6130,13 +6036,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>42</v>
@@ -6149,18 +6055,18 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6185,10 +6091,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G23" s="38" t="s">
         <v>174</v>
@@ -6209,7 +6115,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R23" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6217,13 +6123,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>42</v>
@@ -6236,18 +6142,18 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -6272,10 +6178,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G26" s="38" t="s">
         <v>174</v>
@@ -6296,7 +6202,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R26" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6304,13 +6210,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>42</v>
@@ -6323,18 +6229,18 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -6359,10 +6265,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G29" s="38" t="s">
         <v>174</v>
@@ -6383,7 +6289,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R29" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6391,13 +6297,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>392</v>
+        <v>354</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E30" s="37" t="s">
         <v>42</v>
@@ -6410,18 +6316,18 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>394</v>
+        <v>356</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -6446,10 +6352,10 @@
         <v>21</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G32" s="38" t="s">
         <v>174</v>
@@ -6470,7 +6376,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R32" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6478,13 +6384,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>42</v>
@@ -6497,18 +6403,18 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -6533,10 +6439,10 @@
         <v>21</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G35" s="38" t="s">
         <v>174</v>
@@ -6557,7 +6463,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R35" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6565,13 +6471,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>42</v>
@@ -6584,18 +6490,18 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -6620,10 +6526,10 @@
         <v>21</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G38" s="38" t="s">
         <v>174</v>
@@ -6644,7 +6550,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R38" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6652,13 +6558,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>332</v>
+        <v>294</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>42</v>
@@ -6671,18 +6577,18 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>334</v>
+        <v>296</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -6707,10 +6613,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
       <c r="E41" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G41" s="38" t="s">
         <v>174</v>
@@ -6731,7 +6637,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R41" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6739,13 +6645,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E42" s="37" t="s">
         <v>42</v>
@@ -6758,18 +6664,18 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -6794,10 +6700,10 @@
         <v>21</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G44" s="38" t="s">
         <v>174</v>
@@ -6818,7 +6724,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R44" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6826,13 +6732,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E45" s="37" t="s">
         <v>42</v>
@@ -6845,18 +6751,18 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>340</v>
+        <v>302</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -6881,10 +6787,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>339</v>
+        <v>301</v>
       </c>
       <c r="E47" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G47" s="38" t="s">
         <v>174</v>
@@ -6905,7 +6811,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R47" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6913,13 +6819,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D48" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E48" s="37" t="s">
         <v>42</v>
@@ -6932,18 +6838,18 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -6968,10 +6874,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
       <c r="E50" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G50" s="38" t="s">
         <v>174</v>
@@ -6992,7 +6898,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R50" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7000,13 +6906,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E51" s="37" t="s">
         <v>42</v>
@@ -7019,18 +6925,18 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -7055,10 +6961,10 @@
         <v>21</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="E53" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>174</v>
@@ -7079,7 +6985,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R53" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7087,13 +6993,13 @@
         <v>0</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="C54" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D54" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E54" s="37" t="s">
         <v>42</v>
@@ -7106,18 +7012,18 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -7142,10 +7048,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="E56" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G56" s="38" t="s">
         <v>174</v>
@@ -7166,7 +7072,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R56" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7174,13 +7080,13 @@
         <v>1</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>354</v>
+        <v>316</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E57" s="37" t="s">
         <v>42</v>
@@ -7193,18 +7099,18 @@
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>355</v>
+        <v>317</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -7229,10 +7135,10 @@
         <v>21</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
       <c r="E59" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G59" s="38" t="s">
         <v>174</v>
@@ -7253,7 +7159,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R59" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7261,13 +7167,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>42</v>
@@ -7280,18 +7186,18 @@
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -7316,10 +7222,10 @@
         <v>21</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="E62" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G62" s="38" t="s">
         <v>174</v>
@@ -7340,7 +7246,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R62" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7348,13 +7254,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>42</v>
@@ -7367,18 +7273,18 @@
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -7403,10 +7309,10 @@
         <v>21</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="E65" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G65" s="38" t="s">
         <v>174</v>
@@ -7427,7 +7333,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R65" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7435,13 +7341,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>362</v>
+        <v>324</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>42</v>
@@ -7454,18 +7360,18 @@
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -7490,10 +7396,10 @@
         <v>21</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="E68" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>174</v>
@@ -7514,7 +7420,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R68" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7522,13 +7428,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D69" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E69" s="37" t="s">
         <v>42</v>
@@ -7541,18 +7447,18 @@
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F70" s="10"/>
       <c r="G70" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -7577,10 +7483,10 @@
         <v>21</v>
       </c>
       <c r="D71" s="38" t="s">
-        <v>366</v>
+        <v>328</v>
       </c>
       <c r="E71" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G71" s="38" t="s">
         <v>174</v>
@@ -7601,7 +7507,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R71" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7609,13 +7515,13 @@
         <v>1</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
       <c r="C72" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D72" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E72" s="37" t="s">
         <v>42</v>
@@ -7628,18 +7534,18 @@
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F73" s="10"/>
       <c r="G73" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -7664,10 +7570,10 @@
         <v>21</v>
       </c>
       <c r="D74" s="38" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G74" s="38" t="s">
         <v>174</v>
@@ -7688,7 +7594,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R74" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="75" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7696,13 +7602,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E75" s="37" t="s">
         <v>42</v>
@@ -7715,18 +7621,18 @@
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F76" s="10"/>
       <c r="G76" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -7751,10 +7657,10 @@
         <v>21</v>
       </c>
       <c r="D77" s="38" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="E77" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G77" s="38" t="s">
         <v>174</v>
@@ -7775,7 +7681,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R77" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7783,13 +7689,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E78" s="37" t="s">
         <v>42</v>
@@ -7802,18 +7708,18 @@
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F79" s="10"/>
       <c r="G79" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -7838,10 +7744,10 @@
         <v>21</v>
       </c>
       <c r="D80" s="38" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="E80" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G80" s="38" t="s">
         <v>174</v>
@@ -7862,7 +7768,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R80" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7870,13 +7776,13 @@
         <v>1</v>
       </c>
       <c r="B81" s="37" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D81" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E81" s="37" t="s">
         <v>42</v>
@@ -7889,18 +7795,18 @@
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F82" s="10"/>
       <c r="G82" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -7925,10 +7831,10 @@
         <v>21</v>
       </c>
       <c r="D83" s="38" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
       <c r="E83" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G83" s="38" t="s">
         <v>174</v>
@@ -7949,7 +7855,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R83" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7957,13 +7863,13 @@
         <v>1</v>
       </c>
       <c r="B84" s="37" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="C84" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D84" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E84" s="37" t="s">
         <v>42</v>
@@ -7976,18 +7882,18 @@
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -8012,10 +7918,10 @@
         <v>21</v>
       </c>
       <c r="D86" s="38" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="E86" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G86" s="38" t="s">
         <v>174</v>
@@ -8036,7 +7942,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R86" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8044,13 +7950,13 @@
         <v>1</v>
       </c>
       <c r="B87" s="37" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="C87" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D87" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E87" s="37" t="s">
         <v>42</v>
@@ -8063,18 +7969,18 @@
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F88" s="10"/>
       <c r="G88" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -8099,10 +8005,10 @@
         <v>21</v>
       </c>
       <c r="D89" s="38" t="s">
-        <v>384</v>
+        <v>346</v>
       </c>
       <c r="E89" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G89" s="38" t="s">
         <v>174</v>
@@ -8123,7 +8029,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R89" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8131,13 +8037,13 @@
         <v>1</v>
       </c>
       <c r="B90" s="37" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
       <c r="C90" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D90" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E90" s="37" t="s">
         <v>42</v>
@@ -8150,18 +8056,18 @@
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F91" s="10"/>
       <c r="G91" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>388</v>
+        <v>350</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -8186,10 +8092,10 @@
         <v>21</v>
       </c>
       <c r="D92" s="38" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
       <c r="E92" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G92" s="38" t="s">
         <v>174</v>
@@ -8210,7 +8116,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R92" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8218,13 +8124,13 @@
         <v>1</v>
       </c>
       <c r="B93" s="37" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
       <c r="C93" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D93" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E93" s="37" t="s">
         <v>42</v>
@@ -8237,18 +8143,18 @@
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F94" s="10"/>
       <c r="G94" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>391</v>
+        <v>353</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -8273,10 +8179,10 @@
         <v>21</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>390</v>
+        <v>352</v>
       </c>
       <c r="E95" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G95" s="38" t="s">
         <v>174</v>
@@ -8297,7 +8203,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R95" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8305,13 +8211,13 @@
         <v>1</v>
       </c>
       <c r="B96" s="37" t="s">
-        <v>395</v>
+        <v>357</v>
       </c>
       <c r="C96" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D96" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E96" s="37" t="s">
         <v>42</v>
@@ -8324,18 +8230,18 @@
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F97" s="10"/>
       <c r="G97" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>397</v>
+        <v>359</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -8360,10 +8266,10 @@
         <v>21</v>
       </c>
       <c r="D98" s="38" t="s">
-        <v>396</v>
+        <v>358</v>
       </c>
       <c r="E98" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G98" s="38" t="s">
         <v>174</v>
@@ -8384,7 +8290,7 @@
         <v>0.1666667</v>
       </c>
       <c r="R98" s="38" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8392,13 +8298,13 @@
         <v>1</v>
       </c>
       <c r="B99" s="37" t="s">
-        <v>398</v>
+        <v>360</v>
       </c>
       <c r="C99" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D99" s="37" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="E99" s="37" t="s">
         <v>42</v>
@@ -8411,18 +8317,18 @@
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="F100" s="10"/>
       <c r="G100" s="10" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>400</v>
+        <v>362</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -8447,10 +8353,10 @@
         <v>21</v>
       </c>
       <c r="D101" s="38" t="s">
-        <v>399</v>
+        <v>361</v>
       </c>
       <c r="E101" s="38" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G101" s="38" t="s">
         <v>174</v>
@@ -8471,8 +8377,27 @@
         <v>0.1666667</v>
       </c>
       <c r="R101" s="38" t="s">
-        <v>279</v>
-      </c>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B102" s="40" t="s">
+        <v>364</v>
+      </c>
+      <c r="C102" s="40" t="s">
+        <v>365</v>
+      </c>
+      <c r="D102" s="40" t="s">
+        <v>365</v>
+      </c>
+      <c r="E102" s="40" t="s">
+        <v>363</v>
+      </c>
+      <c r="H102" s="41"/>
+      <c r="I102" s="41"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -8491,11 +8416,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8614,7 +8539,7 @@
         <v>176</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>177</v>
@@ -8649,7 +8574,7 @@
         <v>179</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>180</v>
@@ -8688,7 +8613,7 @@
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>201</v>
@@ -8710,20 +8635,18 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>202</v>
+        <v>367</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>201</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>41</v>
+        <v>366</v>
       </c>
       <c r="G7" s="15" t="b">
         <v>0</v>
@@ -8739,569 +8662,115 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>203</v>
-      </c>
+    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>204</v>
-      </c>
+    <row r="9" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>206</v>
-      </c>
+    <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-    </row>
-    <row r="20" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-    </row>
-    <row r="25" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-    </row>
-    <row r="27" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-    </row>
-    <row r="28" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="22"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="22"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="22"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="22"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="22"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -9435,60 +8904,6 @@
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="22"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="22"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="22"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="22"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="22"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="22"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="22"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="22"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="22"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="22"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="22"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="22"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="22"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="22"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="22"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="22"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="22"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="22"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9618,7 +9033,7 @@
         <v>192</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -9635,7 +9050,7 @@
         <v>190</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -9652,7 +9067,7 @@
         <v>191</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -9669,7 +9084,7 @@
         <v>193</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -9686,7 +9101,7 @@
         <v>195</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
@@ -9739,7 +9154,7 @@
         <v>98</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
@@ -9759,18 +9174,18 @@
         <v>101</v>
       </c>
       <c r="X18" s="22" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
       <c r="AA18" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="AD18" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="AG18" s="22" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="AH18" s="22"/>
       <c r="AI18" s="22"/>
@@ -9780,13 +9195,13 @@
         <v>98</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="G19" s="22">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="I19" t="s">
         <v>119</v>
@@ -9825,16 +9240,16 @@
         <v>128</v>
       </c>
       <c r="X19" s="22" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="Y19" s="22" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="Z19" s="22" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="AD19" s="22" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="AE19" s="22">
         <v>30</v>
@@ -9843,27 +9258,27 @@
         <v>137</v>
       </c>
       <c r="AG19" s="22" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="AH19" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AI19" s="22" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="G20" s="22">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="I20" t="s">
         <v>3</v>
@@ -9908,16 +9323,16 @@
         <v>2</v>
       </c>
       <c r="Z20" s="22" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="AG20" s="22" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="AH20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AI20" s="22" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
@@ -9925,7 +9340,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="G21" s="22">
         <v>1</v>
@@ -9967,10 +9382,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>107</v>
@@ -10014,13 +9429,13 @@
         <v>89</v>
       </c>
       <c r="O23" s="22" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="P23" s="22">
         <v>1</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="R23" s="23" t="s">
         <v>116</v>
@@ -10075,13 +9490,13 @@
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="L25" s="22" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="M25" s="23">
         <v>0</v>
       </c>
       <c r="N25" s="23" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>87</v>
@@ -10093,18 +9508,18 @@
         <v>126</v>
       </c>
       <c r="R25" s="23" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="S25" s="22">
         <v>2</v>
       </c>
       <c r="T25" s="22" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
@@ -10127,7 +9542,7 @@
     </row>
     <row r="27" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
@@ -10153,7 +9568,7 @@
     </row>
     <row r="28" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
@@ -10168,18 +9583,18 @@
         <v>123</v>
       </c>
       <c r="R28" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="S28" s="23">
         <v>0</v>
       </c>
       <c r="T28" s="23" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -10210,13 +9625,13 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="O31" s="22" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="P31" s="23">
         <v>0</v>
       </c>
       <c r="Q31" s="23" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
@@ -10224,13 +9639,13 @@
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="O32" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="P32" s="23">
         <v>1</v>
       </c>
       <c r="Q32" s="23" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added water heater measures into workflow. Marked some options as FIXME.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="396">
   <si>
     <t>type</t>
   </si>
@@ -1218,6 +1218,15 @@
   </si>
   <si>
     <t>plug_loads.txt</t>
+  </si>
+  <si>
+    <t>Set Water Heater</t>
+  </si>
+  <si>
+    <t>Water Heater Sample Value</t>
+  </si>
+  <si>
+    <t>water_heater.txt</t>
   </si>
 </sst>
 </file>
@@ -2984,10 +2993,10 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4982,7 +4991,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -5449,10 +5458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z126"/>
+  <dimension ref="A1:Z129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5507,14 +5516,14 @@
       <c r="R1" s="31"/>
       <c r="S1" s="28"/>
       <c r="T1" s="28"/>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -7865,7 +7874,7 @@
       <c r="X59" s="42"/>
     </row>
     <row r="60" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="b">
+      <c r="A60" s="45" t="b">
         <v>0</v>
       </c>
       <c r="B60" s="41" t="s">
@@ -9789,7 +9798,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="41" t="s">
-        <v>369</v>
+        <v>393</v>
       </c>
       <c r="C108" s="41" t="s">
         <v>253</v>
@@ -9838,7 +9847,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -9865,7 +9874,7 @@
       </c>
       <c r="C110" s="42"/>
       <c r="D110" s="42" t="s">
-        <v>370</v>
+        <v>394</v>
       </c>
       <c r="E110" s="42" t="s">
         <v>255</v>
@@ -9909,7 +9918,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="41" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C111" s="41" t="s">
         <v>253</v>
@@ -9958,7 +9967,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -9985,7 +9994,7 @@
       </c>
       <c r="C113" s="42"/>
       <c r="D113" s="42" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E113" s="42" t="s">
         <v>255</v>
@@ -10025,11 +10034,11 @@
       <c r="X113" s="42"/>
     </row>
     <row r="114" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="46" t="b">
-        <v>0</v>
+      <c r="A114" s="41" t="b">
+        <v>1</v>
       </c>
       <c r="B114" s="41" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C114" s="41" t="s">
         <v>253</v>
@@ -10078,7 +10087,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10105,7 +10114,7 @@
       </c>
       <c r="C116" s="42"/>
       <c r="D116" s="42" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>255</v>
@@ -10145,11 +10154,11 @@
       <c r="X116" s="42"/>
     </row>
     <row r="117" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="46" t="b">
-        <v>0</v>
+      <c r="A117" s="41" t="b">
+        <v>1</v>
       </c>
       <c r="B117" s="41" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C117" s="41" t="s">
         <v>253</v>
@@ -10198,7 +10207,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10225,7 +10234,7 @@
       </c>
       <c r="C119" s="42"/>
       <c r="D119" s="42" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E119" s="42" t="s">
         <v>255</v>
@@ -10269,7 +10278,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="41" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C120" s="41" t="s">
         <v>253</v>
@@ -10318,7 +10327,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10345,7 +10354,7 @@
       </c>
       <c r="C122" s="42"/>
       <c r="D122" s="42" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E122" s="42" t="s">
         <v>255</v>
@@ -10389,7 +10398,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="41" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C123" s="41" t="s">
         <v>253</v>
@@ -10438,7 +10447,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10465,7 +10474,7 @@
       </c>
       <c r="C125" s="42"/>
       <c r="D125" s="42" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E125" s="42" t="s">
         <v>255</v>
@@ -10504,41 +10513,161 @@
       <c r="W125" s="42"/>
       <c r="X125" s="42"/>
     </row>
-    <row r="126" spans="1:26" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="43" t="b">
+    <row r="126" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B126" s="43" t="s">
+      <c r="B126" s="41" t="s">
+        <v>390</v>
+      </c>
+      <c r="C126" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="D126" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="E126" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F126" s="41"/>
+      <c r="G126" s="41"/>
+      <c r="H126" s="41"/>
+      <c r="I126" s="41"/>
+      <c r="J126" s="41"/>
+      <c r="K126" s="41"/>
+      <c r="L126" s="41"/>
+      <c r="M126" s="41"/>
+      <c r="N126" s="41"/>
+      <c r="O126" s="41"/>
+      <c r="P126" s="41"/>
+      <c r="Q126" s="41"/>
+      <c r="R126" s="41"/>
+      <c r="S126" s="41"/>
+      <c r="T126" s="41"/>
+      <c r="U126" s="41"/>
+      <c r="V126" s="41"/>
+      <c r="W126" s="41"/>
+      <c r="X126" s="41"/>
+    </row>
+    <row r="127" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="10"/>
+      <c r="B127" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="J127" s="10"/>
+      <c r="K127" s="10"/>
+      <c r="L127" s="10"/>
+      <c r="M127" s="10"/>
+      <c r="N127" s="10"/>
+      <c r="O127" s="10"/>
+      <c r="P127" s="10"/>
+      <c r="Q127" s="10"/>
+      <c r="R127" s="10"/>
+      <c r="S127" s="10"/>
+      <c r="T127" s="10"/>
+      <c r="U127" s="10"/>
+      <c r="V127" s="10"/>
+      <c r="W127" s="10"/>
+      <c r="X127" s="10"/>
+      <c r="Y127" s="15"/>
+      <c r="Z127" s="15"/>
+    </row>
+    <row r="128" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="42"/>
+      <c r="B128" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C128" s="42"/>
+      <c r="D128" s="42" t="s">
+        <v>391</v>
+      </c>
+      <c r="E128" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="F128" s="42"/>
+      <c r="G128" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="H128" s="42"/>
+      <c r="I128" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="J128" s="42"/>
+      <c r="K128" s="42">
+        <v>0</v>
+      </c>
+      <c r="L128" s="42">
+        <v>1</v>
+      </c>
+      <c r="M128" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N128" s="42">
+        <v>0.1666667</v>
+      </c>
+      <c r="O128" s="42"/>
+      <c r="P128" s="42"/>
+      <c r="Q128" s="42"/>
+      <c r="R128" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="S128" s="42"/>
+      <c r="T128" s="42"/>
+      <c r="U128" s="42"/>
+      <c r="V128" s="42"/>
+      <c r="W128" s="42"/>
+      <c r="X128" s="42"/>
+    </row>
+    <row r="129" spans="1:24" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B129" s="43" t="s">
         <v>364</v>
       </c>
-      <c r="C126" s="43" t="s">
+      <c r="C129" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="D126" s="43" t="s">
+      <c r="D129" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="E126" s="43" t="s">
+      <c r="E129" s="43" t="s">
         <v>363</v>
       </c>
-      <c r="F126" s="43"/>
-      <c r="G126" s="43"/>
-      <c r="H126" s="44"/>
-      <c r="I126" s="44"/>
-      <c r="J126" s="43"/>
-      <c r="K126" s="43"/>
-      <c r="L126" s="43"/>
-      <c r="M126" s="43"/>
-      <c r="N126" s="43"/>
-      <c r="O126" s="43"/>
-      <c r="P126" s="43"/>
-      <c r="Q126" s="43"/>
-      <c r="R126" s="43"/>
-      <c r="S126" s="43"/>
-      <c r="T126" s="43"/>
-      <c r="U126" s="43"/>
-      <c r="V126" s="43"/>
-      <c r="W126" s="43"/>
-      <c r="X126" s="43"/>
+      <c r="F129" s="43"/>
+      <c r="G129" s="43"/>
+      <c r="H129" s="44"/>
+      <c r="I129" s="44"/>
+      <c r="J129" s="43"/>
+      <c r="K129" s="43"/>
+      <c r="L129" s="43"/>
+      <c r="M129" s="43"/>
+      <c r="N129" s="43"/>
+      <c r="O129" s="43"/>
+      <c r="P129" s="43"/>
+      <c r="Q129" s="43"/>
+      <c r="R129" s="43"/>
+      <c r="S129" s="43"/>
+      <c r="T129" s="43"/>
+      <c r="U129" s="43"/>
+      <c r="V129" s="43"/>
+      <c r="W129" s="43"/>
+      <c r="X129" s="43"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>

</xml_diff>

<commit_message>
Implemented reporting of option names in the results.csv.
Relied on fix pushed to nrel24b by Ry.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="474">
   <si>
     <t>type</t>
   </si>
@@ -1142,12 +1142,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>Test Value</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.test_value</t>
-  </si>
-  <si>
     <t>Set Refrigerator</t>
   </si>
   <si>
@@ -1227,6 +1221,246 @@
   </si>
   <si>
     <t>water_heater.txt</t>
+  </si>
+  <si>
+    <t>Location Region</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.location region</t>
+  </si>
+  <si>
+    <t>Location EPW</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.location epw</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.vintage</t>
+  </si>
+  <si>
+    <t>Heating Fuel</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.heating fuel</t>
+  </si>
+  <si>
+    <t>Usage Level</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.usage level</t>
+  </si>
+  <si>
+    <t>Foundation Type</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.foundation type</t>
+  </si>
+  <si>
+    <t>House Size</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.house size</t>
+  </si>
+  <si>
+    <t>Stories</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.stories</t>
+  </si>
+  <si>
+    <t>Garage</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.garage</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.geometry</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.orientation</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Attic</t>
+  </si>
+  <si>
+    <t>Insulation Walls</t>
+  </si>
+  <si>
+    <t>Insulation Walls Interzonal</t>
+  </si>
+  <si>
+    <t>Insulation Slab</t>
+  </si>
+  <si>
+    <t>Insulation Crawl</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Basement</t>
+  </si>
+  <si>
+    <t>Insulation Finished Basement</t>
+  </si>
+  <si>
+    <t>Insulation Floors Interzonal</t>
+  </si>
+  <si>
+    <t>Uninsulated Floor</t>
+  </si>
+  <si>
+    <t>Uninsulated Roof</t>
+  </si>
+  <si>
+    <t>Uninsulated Slab</t>
+  </si>
+  <si>
+    <t>Uninsulated Walls</t>
+  </si>
+  <si>
+    <t>Wall Sheathing</t>
+  </si>
+  <si>
+    <t>Exterior Finish</t>
+  </si>
+  <si>
+    <t>Roof Material</t>
+  </si>
+  <si>
+    <t>Floor Covering</t>
+  </si>
+  <si>
+    <t>Floor Mass</t>
+  </si>
+  <si>
+    <t>Exterior Wall Mass</t>
+  </si>
+  <si>
+    <t>Partition Wall Mass</t>
+  </si>
+  <si>
+    <t>Ceiling Mass</t>
+  </si>
+  <si>
+    <t>Door Area</t>
+  </si>
+  <si>
+    <t>Doors</t>
+  </si>
+  <si>
+    <t>Water Heater</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Cooking Range</t>
+  </si>
+  <si>
+    <t>Dishwasher</t>
+  </si>
+  <si>
+    <t>Clothes Washer</t>
+  </si>
+  <si>
+    <t>Clothes Dryer</t>
+  </si>
+  <si>
+    <t>Plug Loads</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation unfinished attic</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation walls</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation walls interzonal</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation slab</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation crawl</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation unfinished basement</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation finished basement</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.insulation floors interzonal</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.uninsulated floor</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.uninsulated roof</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.uninsulated slab</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.uninsulated walls</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.wall sheathing</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.exterior finish</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.roof material</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.floor covering</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.floor mass</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.exterior wall mass</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.partition wall mass</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.ceiling mass</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.door area</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.doors</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.water heater</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.refrigerator</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.cooking range</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.dishwasher</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.clothes washer</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.clothes dryer</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.plug loads</t>
   </si>
 </sst>
 </file>
@@ -2903,7 +3137,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2997,6 +3231,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5460,8 +5695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6078,7 +6313,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>253</v>
@@ -6127,7 +6362,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6154,7 +6389,7 @@
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="42" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>255</v>
@@ -6198,7 +6433,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C18" s="41" t="s">
         <v>253</v>
@@ -6247,7 +6482,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6274,7 +6509,7 @@
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E20" s="42" t="s">
         <v>255</v>
@@ -9798,7 +10033,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="41" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C108" s="41" t="s">
         <v>253</v>
@@ -9847,7 +10082,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -9874,7 +10109,7 @@
       </c>
       <c r="C110" s="42"/>
       <c r="D110" s="42" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E110" s="42" t="s">
         <v>255</v>
@@ -9918,7 +10153,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="41" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C111" s="41" t="s">
         <v>253</v>
@@ -9967,7 +10202,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -9994,7 +10229,7 @@
       </c>
       <c r="C113" s="42"/>
       <c r="D113" s="42" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E113" s="42" t="s">
         <v>255</v>
@@ -10038,7 +10273,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="41" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C114" s="41" t="s">
         <v>253</v>
@@ -10087,7 +10322,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10114,7 +10349,7 @@
       </c>
       <c r="C116" s="42"/>
       <c r="D116" s="42" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>255</v>
@@ -10158,7 +10393,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="41" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C117" s="41" t="s">
         <v>253</v>
@@ -10207,7 +10442,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10234,7 +10469,7 @@
       </c>
       <c r="C119" s="42"/>
       <c r="D119" s="42" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E119" s="42" t="s">
         <v>255</v>
@@ -10278,7 +10513,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="41" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C120" s="41" t="s">
         <v>253</v>
@@ -10327,7 +10562,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10354,7 +10589,7 @@
       </c>
       <c r="C122" s="42"/>
       <c r="D122" s="42" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E122" s="42" t="s">
         <v>255</v>
@@ -10398,7 +10633,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="41" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C123" s="41" t="s">
         <v>253</v>
@@ -10447,7 +10682,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10474,7 +10709,7 @@
       </c>
       <c r="C125" s="42"/>
       <c r="D125" s="42" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E125" s="42" t="s">
         <v>255</v>
@@ -10518,7 +10753,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="41" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C126" s="41" t="s">
         <v>253</v>
@@ -10567,7 +10802,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10594,7 +10829,7 @@
       </c>
       <c r="C128" s="42"/>
       <c r="D128" s="42" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E128" s="42" t="s">
         <v>255</v>
@@ -10686,18 +10921,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="2" style="1" customWidth="1"/>
     <col min="4" max="4" width="35.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -10907,12 +11142,12 @@
     </row>
     <row r="7" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>368</v>
+        <v>395</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
@@ -10932,163 +11167,913 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>396</v>
+      </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15" t="s">
+        <v>397</v>
+      </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G8" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>398</v>
+      </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>399</v>
+      </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G9" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+    <row r="10" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>400</v>
+      </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>401</v>
+      </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G10" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="22"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G11" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G12" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G13" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G14" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G15" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G16" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+    </row>
+    <row r="18" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G18" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G19" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+    </row>
+    <row r="20" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G21" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="47" t="s">
+        <v>420</v>
+      </c>
       <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D22" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G22" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="47" t="s">
+        <v>421</v>
+      </c>
       <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D23" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G23" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="47" t="s">
+        <v>422</v>
+      </c>
       <c r="B24" s="22"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D24" s="15" t="s">
+        <v>451</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G24" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="47" t="s">
+        <v>423</v>
+      </c>
       <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D25" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G25" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="47" t="s">
+        <v>424</v>
+      </c>
       <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D26" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G26" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="47" t="s">
+        <v>425</v>
+      </c>
       <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D27" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G27" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="47" t="s">
+        <v>426</v>
+      </c>
       <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D28" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G28" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="47" t="s">
+        <v>427</v>
+      </c>
       <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G29" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="47" t="s">
+        <v>428</v>
+      </c>
       <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D30" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G30" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="47" t="s">
+        <v>429</v>
+      </c>
       <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D31" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G31" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
+        <v>430</v>
+      </c>
       <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D32" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G32" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="47" t="s">
+        <v>431</v>
+      </c>
       <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D33" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G33" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
+        <v>432</v>
+      </c>
       <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D34" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G34" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="47" t="s">
+        <v>433</v>
+      </c>
       <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D35" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G35" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="47" t="s">
+        <v>434</v>
+      </c>
       <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D36" s="15" t="s">
+        <v>463</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G36" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="47" t="s">
+        <v>435</v>
+      </c>
       <c r="B37" s="22"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D37" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G37" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="47" t="s">
+        <v>436</v>
+      </c>
       <c r="B38" s="22"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D38" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G38" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="47" t="s">
+        <v>437</v>
+      </c>
       <c r="B39" s="22"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D39" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G39" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="47" t="s">
+        <v>438</v>
+      </c>
       <c r="B40" s="22"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D40" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G40" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="47" t="s">
+        <v>439</v>
+      </c>
       <c r="B41" s="22"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D41" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G41" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
+        <v>440</v>
+      </c>
       <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D42" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G42" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="47" t="s">
+        <v>441</v>
+      </c>
       <c r="B43" s="22"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D43" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G43" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="47" t="s">
+        <v>442</v>
+      </c>
       <c r="B44" s="22"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D44" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G44" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="47" t="s">
+        <v>443</v>
+      </c>
       <c r="B45" s="22"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D45" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G45" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="47" t="s">
+        <v>444</v>
+      </c>
       <c r="B46" s="22"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D46" s="15" t="s">
+        <v>473</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="G46" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="22"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -11172,12 +12157,9 @@
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="22"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="22"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added large uncommon loads to workflow. Updated uninsulated surfaces measure.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="501">
   <si>
     <t>type</t>
   </si>
@@ -956,42 +956,6 @@
     <t>insulation_floor_interzonal.txt</t>
   </si>
   <si>
-    <t>Set Uninsulated Floor</t>
-  </si>
-  <si>
-    <t>Uninsulated Floor Sample Value</t>
-  </si>
-  <si>
-    <t>uninsulated_floor.txt</t>
-  </si>
-  <si>
-    <t>Set Uninsulated Roof</t>
-  </si>
-  <si>
-    <t>Uninsulated Roof Sample Value</t>
-  </si>
-  <si>
-    <t>uninsulated_roof.txt</t>
-  </si>
-  <si>
-    <t>Set Uninsulated Slab</t>
-  </si>
-  <si>
-    <t>Uninsulated Slab Sample Value</t>
-  </si>
-  <si>
-    <t>uninsulated_slab.txt</t>
-  </si>
-  <si>
-    <t>Set Uninsulated Walls</t>
-  </si>
-  <si>
-    <t>Uninsulated Walls Sample Value</t>
-  </si>
-  <si>
-    <t>uninsulated_walls.txt</t>
-  </si>
-  <si>
     <t>Set Wall Sheathing</t>
   </si>
   <si>
@@ -1250,18 +1214,6 @@
     <t>Insulation Floors Interzonal</t>
   </si>
   <si>
-    <t>Uninsulated Floor</t>
-  </si>
-  <si>
-    <t>Uninsulated Roof</t>
-  </si>
-  <si>
-    <t>Uninsulated Slab</t>
-  </si>
-  <si>
-    <t>Uninsulated Walls</t>
-  </si>
-  <si>
     <t>Wall Sheathing</t>
   </si>
   <si>
@@ -1370,18 +1322,6 @@
     <t>res_stock_reporting.insulation_floor_interzonal</t>
   </si>
   <si>
-    <t>res_stock_reporting.uninsulated_floor</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.uninsulated_roof</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.uninsulated_slab</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.uninsulated_walls</t>
-  </si>
-  <si>
     <t>res_stock_reporting.wall_sheathing</t>
   </si>
   <si>
@@ -1467,6 +1407,141 @@
   </si>
   <si>
     <t>res_stock_reporting.overhangs</t>
+  </si>
+  <si>
+    <t>Set Uninsulated Surfaces</t>
+  </si>
+  <si>
+    <t>Uninsulated Surfaces Sample Value</t>
+  </si>
+  <si>
+    <t>uninsulated_surfaces.txt</t>
+  </si>
+  <si>
+    <t>Uninsulated Surfaces</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.uninsulated_surfaces</t>
+  </si>
+  <si>
+    <t>Set Extra Refrigerator</t>
+  </si>
+  <si>
+    <t>Extra Refrigerator Sample Value</t>
+  </si>
+  <si>
+    <t>Set Gas Grill</t>
+  </si>
+  <si>
+    <t>Gas Grill Sample Value</t>
+  </si>
+  <si>
+    <t>misc_gas_grill.txt</t>
+  </si>
+  <si>
+    <t>misc_extra_refrigerator.txt</t>
+  </si>
+  <si>
+    <t>Set Gas Lighting</t>
+  </si>
+  <si>
+    <t>Gas Lighting Sample Value</t>
+  </si>
+  <si>
+    <t>misc_gas_lighting.txt</t>
+  </si>
+  <si>
+    <t>Set Pool</t>
+  </si>
+  <si>
+    <t>Pool Sample Value</t>
+  </si>
+  <si>
+    <t>misc_pool.txt</t>
+  </si>
+  <si>
+    <t>Set Well Pump</t>
+  </si>
+  <si>
+    <t>Well Pump Sample Value</t>
+  </si>
+  <si>
+    <t>misc_well_pump.txt</t>
+  </si>
+  <si>
+    <t>Set Freezer</t>
+  </si>
+  <si>
+    <t>Freezer Sample Value</t>
+  </si>
+  <si>
+    <t>misc_freezer.txt</t>
+  </si>
+  <si>
+    <t>Set Gas Fireplace</t>
+  </si>
+  <si>
+    <t>Gas Fireplace Sample Value</t>
+  </si>
+  <si>
+    <t>misc_gas_fireplace.txt</t>
+  </si>
+  <si>
+    <t>Extra Refrigerator</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Gas Fireplace</t>
+  </si>
+  <si>
+    <t>Gas Grill</t>
+  </si>
+  <si>
+    <t>Gas Lighting</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>Hot Tub/Spa</t>
+  </si>
+  <si>
+    <t>Set Hot Tub/Spa</t>
+  </si>
+  <si>
+    <t>Hot Tub/Spa Sample Value</t>
+  </si>
+  <si>
+    <t>misc_hot_tub_spa.txt</t>
+  </si>
+  <si>
+    <t>Well Pump</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_extra_refrigerator</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_freezer</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_gas_fireplace</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_gas_grill</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_gas_lighting</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_hot_tub_spa</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_pool</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.misc_well_pump</t>
   </si>
 </sst>
 </file>
@@ -5699,10 +5774,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z138"/>
+  <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6319,7 +6394,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>240</v>
@@ -6368,7 +6443,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6395,7 +6470,7 @@
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="42" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>242</v>
@@ -6439,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="C18" s="41" t="s">
         <v>240</v>
@@ -6488,7 +6563,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6515,7 +6590,7 @@
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="E20" s="42" t="s">
         <v>242</v>
@@ -7159,7 +7234,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="C36" s="41" t="s">
         <v>240</v>
@@ -7208,7 +7283,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7235,7 +7310,7 @@
       </c>
       <c r="C38" s="42"/>
       <c r="D38" s="42" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>242</v>
@@ -7279,7 +7354,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>240</v>
@@ -7328,7 +7403,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>468</v>
+        <v>448</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7355,7 +7430,7 @@
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="42" t="s">
-        <v>467</v>
+        <v>447</v>
       </c>
       <c r="E41" s="42" t="s">
         <v>242</v>
@@ -7399,7 +7474,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>471</v>
+        <v>451</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>240</v>
@@ -7448,7 +7523,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>473</v>
+        <v>453</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7475,7 +7550,7 @@
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="42" t="s">
-        <v>472</v>
+        <v>452</v>
       </c>
       <c r="E44" s="42" t="s">
         <v>242</v>
@@ -7519,7 +7594,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
       <c r="C45" s="41" t="s">
         <v>240</v>
@@ -7568,7 +7643,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>463</v>
+        <v>443</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7595,7 +7670,7 @@
       </c>
       <c r="C47" s="42"/>
       <c r="D47" s="42" t="s">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="E47" s="42" t="s">
         <v>242</v>
@@ -8719,7 +8794,7 @@
         <v>1</v>
       </c>
       <c r="B75" s="41" t="s">
-        <v>305</v>
+        <v>456</v>
       </c>
       <c r="C75" s="41" t="s">
         <v>240</v>
@@ -8768,7 +8843,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>307</v>
+        <v>458</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8795,7 +8870,7 @@
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="42" t="s">
-        <v>306</v>
+        <v>457</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>242</v>
@@ -8839,7 +8914,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="41" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C78" s="41" t="s">
         <v>240</v>
@@ -8888,7 +8963,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -8915,7 +8990,7 @@
       </c>
       <c r="C80" s="42"/>
       <c r="D80" s="42" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E80" s="42" t="s">
         <v>242</v>
@@ -8959,7 +9034,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="41" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C81" s="41" t="s">
         <v>240</v>
@@ -9008,7 +9083,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9035,7 +9110,7 @@
       </c>
       <c r="C83" s="42"/>
       <c r="D83" s="42" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E83" s="42" t="s">
         <v>242</v>
@@ -9079,7 +9154,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="41" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C84" s="41" t="s">
         <v>240</v>
@@ -9128,7 +9203,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9155,7 +9230,7 @@
       </c>
       <c r="C86" s="42"/>
       <c r="D86" s="42" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E86" s="42" t="s">
         <v>242</v>
@@ -9199,7 +9274,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="41" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C87" s="41" t="s">
         <v>240</v>
@@ -9248,7 +9323,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9275,7 +9350,7 @@
       </c>
       <c r="C89" s="42"/>
       <c r="D89" s="42" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E89" s="42" t="s">
         <v>242</v>
@@ -9319,7 +9394,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="41" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C90" s="41" t="s">
         <v>240</v>
@@ -9368,7 +9443,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9395,7 +9470,7 @@
       </c>
       <c r="C92" s="42"/>
       <c r="D92" s="42" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E92" s="42" t="s">
         <v>242</v>
@@ -9439,7 +9514,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="41" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C93" s="41" t="s">
         <v>240</v>
@@ -9488,7 +9563,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9515,7 +9590,7 @@
       </c>
       <c r="C95" s="42"/>
       <c r="D95" s="42" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E95" s="42" t="s">
         <v>242</v>
@@ -9559,7 +9634,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="41" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C96" s="41" t="s">
         <v>240</v>
@@ -9608,7 +9683,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9635,7 +9710,7 @@
       </c>
       <c r="C98" s="42"/>
       <c r="D98" s="42" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E98" s="42" t="s">
         <v>242</v>
@@ -9679,7 +9754,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="41" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C99" s="41" t="s">
         <v>240</v>
@@ -9728,7 +9803,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9755,7 +9830,7 @@
       </c>
       <c r="C101" s="42"/>
       <c r="D101" s="42" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E101" s="42" t="s">
         <v>242</v>
@@ -10039,7 +10114,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="41" t="s">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="C108" s="41" t="s">
         <v>240</v>
@@ -10088,7 +10163,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>340</v>
+        <v>368</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10115,7 +10190,7 @@
       </c>
       <c r="C110" s="42"/>
       <c r="D110" s="42" t="s">
-        <v>339</v>
+        <v>367</v>
       </c>
       <c r="E110" s="42" t="s">
         <v>242</v>
@@ -10159,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="41" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C111" s="41" t="s">
         <v>240</v>
@@ -10208,7 +10283,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10235,7 +10310,7 @@
       </c>
       <c r="C113" s="42"/>
       <c r="D113" s="42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E113" s="42" t="s">
         <v>242</v>
@@ -10279,7 +10354,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="41" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C114" s="41" t="s">
         <v>240</v>
@@ -10328,7 +10403,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10355,7 +10430,7 @@
       </c>
       <c r="C116" s="42"/>
       <c r="D116" s="42" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>242</v>
@@ -10399,7 +10474,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="41" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="C117" s="41" t="s">
         <v>240</v>
@@ -10448,7 +10523,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10475,7 +10550,7 @@
       </c>
       <c r="C119" s="42"/>
       <c r="D119" s="42" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="E119" s="42" t="s">
         <v>242</v>
@@ -10519,7 +10594,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="41" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C120" s="41" t="s">
         <v>240</v>
@@ -10568,7 +10643,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10595,7 +10670,7 @@
       </c>
       <c r="C122" s="42"/>
       <c r="D122" s="42" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E122" s="42" t="s">
         <v>242</v>
@@ -10759,7 +10834,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="41" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C126" s="41" t="s">
         <v>240</v>
@@ -10808,7 +10883,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10835,7 +10910,7 @@
       </c>
       <c r="C128" s="42"/>
       <c r="D128" s="42" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E128" s="42" t="s">
         <v>242</v>
@@ -10879,7 +10954,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="41" t="s">
-        <v>369</v>
+        <v>461</v>
       </c>
       <c r="C129" s="41" t="s">
         <v>240</v>
@@ -10928,7 +11003,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>371</v>
+        <v>466</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -10955,7 +11030,7 @@
       </c>
       <c r="C131" s="42"/>
       <c r="D131" s="42" t="s">
-        <v>370</v>
+        <v>462</v>
       </c>
       <c r="E131" s="42" t="s">
         <v>242</v>
@@ -10999,7 +11074,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="41" t="s">
-        <v>372</v>
+        <v>476</v>
       </c>
       <c r="C132" s="41" t="s">
         <v>240</v>
@@ -11048,7 +11123,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>374</v>
+        <v>478</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11075,7 +11150,7 @@
       </c>
       <c r="C134" s="42"/>
       <c r="D134" s="42" t="s">
-        <v>373</v>
+        <v>477</v>
       </c>
       <c r="E134" s="42" t="s">
         <v>242</v>
@@ -11119,7 +11194,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="41" t="s">
-        <v>375</v>
+        <v>479</v>
       </c>
       <c r="C135" s="41" t="s">
         <v>240</v>
@@ -11168,7 +11243,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>377</v>
+        <v>481</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11195,7 +11270,7 @@
       </c>
       <c r="C137" s="42"/>
       <c r="D137" s="42" t="s">
-        <v>376</v>
+        <v>480</v>
       </c>
       <c r="E137" s="42" t="s">
         <v>242</v>
@@ -11234,41 +11309,641 @@
       <c r="W137" s="42"/>
       <c r="X137" s="42"/>
     </row>
-    <row r="138" spans="1:26" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="43" t="b">
+    <row r="138" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B138" s="43" t="s">
-        <v>351</v>
-      </c>
-      <c r="C138" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="D138" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="E138" s="43" t="s">
-        <v>350</v>
-      </c>
-      <c r="F138" s="43"/>
-      <c r="G138" s="43"/>
-      <c r="H138" s="44"/>
-      <c r="I138" s="44"/>
-      <c r="J138" s="43"/>
-      <c r="K138" s="43"/>
-      <c r="L138" s="43"/>
-      <c r="M138" s="43"/>
-      <c r="N138" s="43"/>
-      <c r="O138" s="43"/>
-      <c r="P138" s="43"/>
-      <c r="Q138" s="43"/>
-      <c r="R138" s="43"/>
-      <c r="S138" s="43"/>
-      <c r="T138" s="43"/>
-      <c r="U138" s="43"/>
-      <c r="V138" s="43"/>
-      <c r="W138" s="43"/>
-      <c r="X138" s="43"/>
+      <c r="B138" s="41" t="s">
+        <v>463</v>
+      </c>
+      <c r="C138" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D138" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E138" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F138" s="41"/>
+      <c r="G138" s="41"/>
+      <c r="H138" s="41"/>
+      <c r="I138" s="41"/>
+      <c r="J138" s="41"/>
+      <c r="K138" s="41"/>
+      <c r="L138" s="41"/>
+      <c r="M138" s="41"/>
+      <c r="N138" s="41"/>
+      <c r="O138" s="41"/>
+      <c r="P138" s="41"/>
+      <c r="Q138" s="41"/>
+      <c r="R138" s="41"/>
+      <c r="S138" s="41"/>
+      <c r="T138" s="41"/>
+      <c r="U138" s="41"/>
+      <c r="V138" s="41"/>
+      <c r="W138" s="41"/>
+      <c r="X138" s="41"/>
+    </row>
+    <row r="139" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="10"/>
+      <c r="B139" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E139" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="J139" s="10"/>
+      <c r="K139" s="10"/>
+      <c r="L139" s="10"/>
+      <c r="M139" s="10"/>
+      <c r="N139" s="10"/>
+      <c r="O139" s="10"/>
+      <c r="P139" s="10"/>
+      <c r="Q139" s="10"/>
+      <c r="R139" s="10"/>
+      <c r="S139" s="10"/>
+      <c r="T139" s="10"/>
+      <c r="U139" s="10"/>
+      <c r="V139" s="10"/>
+      <c r="W139" s="10"/>
+      <c r="X139" s="10"/>
+      <c r="Y139" s="15"/>
+      <c r="Z139" s="15"/>
+    </row>
+    <row r="140" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="42"/>
+      <c r="B140" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140" s="42"/>
+      <c r="D140" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E140" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F140" s="42"/>
+      <c r="G140" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H140" s="42"/>
+      <c r="I140" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="J140" s="42"/>
+      <c r="K140" s="42">
+        <v>0</v>
+      </c>
+      <c r="L140" s="42">
+        <v>1</v>
+      </c>
+      <c r="M140" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N140" s="42">
+        <v>0.1666667</v>
+      </c>
+      <c r="O140" s="42"/>
+      <c r="P140" s="42"/>
+      <c r="Q140" s="42"/>
+      <c r="R140" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="S140" s="42"/>
+      <c r="T140" s="42"/>
+      <c r="U140" s="42"/>
+      <c r="V140" s="42"/>
+      <c r="W140" s="42"/>
+      <c r="X140" s="42"/>
+    </row>
+    <row r="141" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A141" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B141" s="41" t="s">
+        <v>467</v>
+      </c>
+      <c r="C141" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D141" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E141" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F141" s="41"/>
+      <c r="G141" s="41"/>
+      <c r="H141" s="41"/>
+      <c r="I141" s="41"/>
+      <c r="J141" s="41"/>
+      <c r="K141" s="41"/>
+      <c r="L141" s="41"/>
+      <c r="M141" s="41"/>
+      <c r="N141" s="41"/>
+      <c r="O141" s="41"/>
+      <c r="P141" s="41"/>
+      <c r="Q141" s="41"/>
+      <c r="R141" s="41"/>
+      <c r="S141" s="41"/>
+      <c r="T141" s="41"/>
+      <c r="U141" s="41"/>
+      <c r="V141" s="41"/>
+      <c r="W141" s="41"/>
+      <c r="X141" s="41"/>
+    </row>
+    <row r="142" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="10"/>
+      <c r="B142" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" s="10"/>
+      <c r="D142" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E142" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H142" s="10"/>
+      <c r="I142" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="J142" s="10"/>
+      <c r="K142" s="10"/>
+      <c r="L142" s="10"/>
+      <c r="M142" s="10"/>
+      <c r="N142" s="10"/>
+      <c r="O142" s="10"/>
+      <c r="P142" s="10"/>
+      <c r="Q142" s="10"/>
+      <c r="R142" s="10"/>
+      <c r="S142" s="10"/>
+      <c r="T142" s="10"/>
+      <c r="U142" s="10"/>
+      <c r="V142" s="10"/>
+      <c r="W142" s="10"/>
+      <c r="X142" s="10"/>
+      <c r="Y142" s="15"/>
+      <c r="Z142" s="15"/>
+    </row>
+    <row r="143" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A143" s="42"/>
+      <c r="B143" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C143" s="42"/>
+      <c r="D143" s="42" t="s">
+        <v>468</v>
+      </c>
+      <c r="E143" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F143" s="42"/>
+      <c r="G143" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H143" s="42"/>
+      <c r="I143" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="J143" s="42"/>
+      <c r="K143" s="42">
+        <v>0</v>
+      </c>
+      <c r="L143" s="42">
+        <v>1</v>
+      </c>
+      <c r="M143" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N143" s="42">
+        <v>0.1666667</v>
+      </c>
+      <c r="O143" s="42"/>
+      <c r="P143" s="42"/>
+      <c r="Q143" s="42"/>
+      <c r="R143" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="S143" s="42"/>
+      <c r="T143" s="42"/>
+      <c r="U143" s="42"/>
+      <c r="V143" s="42"/>
+      <c r="W143" s="42"/>
+      <c r="X143" s="42"/>
+    </row>
+    <row r="144" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A144" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B144" s="41" t="s">
+        <v>489</v>
+      </c>
+      <c r="C144" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D144" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E144" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F144" s="41"/>
+      <c r="G144" s="41"/>
+      <c r="H144" s="41"/>
+      <c r="I144" s="41"/>
+      <c r="J144" s="41"/>
+      <c r="K144" s="41"/>
+      <c r="L144" s="41"/>
+      <c r="M144" s="41"/>
+      <c r="N144" s="41"/>
+      <c r="O144" s="41"/>
+      <c r="P144" s="41"/>
+      <c r="Q144" s="41"/>
+      <c r="R144" s="41"/>
+      <c r="S144" s="41"/>
+      <c r="T144" s="41"/>
+      <c r="U144" s="41"/>
+      <c r="V144" s="41"/>
+      <c r="W144" s="41"/>
+      <c r="X144" s="41"/>
+    </row>
+    <row r="145" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="10"/>
+      <c r="B145" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E145" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F145" s="10"/>
+      <c r="G145" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H145" s="10"/>
+      <c r="I145" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="J145" s="10"/>
+      <c r="K145" s="10"/>
+      <c r="L145" s="10"/>
+      <c r="M145" s="10"/>
+      <c r="N145" s="10"/>
+      <c r="O145" s="10"/>
+      <c r="P145" s="10"/>
+      <c r="Q145" s="10"/>
+      <c r="R145" s="10"/>
+      <c r="S145" s="10"/>
+      <c r="T145" s="10"/>
+      <c r="U145" s="10"/>
+      <c r="V145" s="10"/>
+      <c r="W145" s="10"/>
+      <c r="X145" s="10"/>
+      <c r="Y145" s="15"/>
+      <c r="Z145" s="15"/>
+    </row>
+    <row r="146" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A146" s="42"/>
+      <c r="B146" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C146" s="42"/>
+      <c r="D146" s="42" t="s">
+        <v>490</v>
+      </c>
+      <c r="E146" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F146" s="42"/>
+      <c r="G146" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H146" s="42"/>
+      <c r="I146" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="J146" s="42"/>
+      <c r="K146" s="42">
+        <v>0</v>
+      </c>
+      <c r="L146" s="42">
+        <v>1</v>
+      </c>
+      <c r="M146" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N146" s="42">
+        <v>0.1666667</v>
+      </c>
+      <c r="O146" s="42"/>
+      <c r="P146" s="42"/>
+      <c r="Q146" s="42"/>
+      <c r="R146" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="S146" s="42"/>
+      <c r="T146" s="42"/>
+      <c r="U146" s="42"/>
+      <c r="V146" s="42"/>
+      <c r="W146" s="42"/>
+      <c r="X146" s="42"/>
+    </row>
+    <row r="147" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B147" s="41" t="s">
+        <v>470</v>
+      </c>
+      <c r="C147" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D147" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E147" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F147" s="41"/>
+      <c r="G147" s="41"/>
+      <c r="H147" s="41"/>
+      <c r="I147" s="41"/>
+      <c r="J147" s="41"/>
+      <c r="K147" s="41"/>
+      <c r="L147" s="41"/>
+      <c r="M147" s="41"/>
+      <c r="N147" s="41"/>
+      <c r="O147" s="41"/>
+      <c r="P147" s="41"/>
+      <c r="Q147" s="41"/>
+      <c r="R147" s="41"/>
+      <c r="S147" s="41"/>
+      <c r="T147" s="41"/>
+      <c r="U147" s="41"/>
+      <c r="V147" s="41"/>
+      <c r="W147" s="41"/>
+      <c r="X147" s="41"/>
+    </row>
+    <row r="148" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="10"/>
+      <c r="B148" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E148" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F148" s="10"/>
+      <c r="G148" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H148" s="10"/>
+      <c r="I148" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="J148" s="10"/>
+      <c r="K148" s="10"/>
+      <c r="L148" s="10"/>
+      <c r="M148" s="10"/>
+      <c r="N148" s="10"/>
+      <c r="O148" s="10"/>
+      <c r="P148" s="10"/>
+      <c r="Q148" s="10"/>
+      <c r="R148" s="10"/>
+      <c r="S148" s="10"/>
+      <c r="T148" s="10"/>
+      <c r="U148" s="10"/>
+      <c r="V148" s="10"/>
+      <c r="W148" s="10"/>
+      <c r="X148" s="10"/>
+      <c r="Y148" s="15"/>
+      <c r="Z148" s="15"/>
+    </row>
+    <row r="149" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A149" s="42"/>
+      <c r="B149" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C149" s="42"/>
+      <c r="D149" s="42" t="s">
+        <v>471</v>
+      </c>
+      <c r="E149" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F149" s="42"/>
+      <c r="G149" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H149" s="42"/>
+      <c r="I149" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="J149" s="42"/>
+      <c r="K149" s="42">
+        <v>0</v>
+      </c>
+      <c r="L149" s="42">
+        <v>1</v>
+      </c>
+      <c r="M149" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N149" s="42">
+        <v>0.1666667</v>
+      </c>
+      <c r="O149" s="42"/>
+      <c r="P149" s="42"/>
+      <c r="Q149" s="42"/>
+      <c r="R149" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="S149" s="42"/>
+      <c r="T149" s="42"/>
+      <c r="U149" s="42"/>
+      <c r="V149" s="42"/>
+      <c r="W149" s="42"/>
+      <c r="X149" s="42"/>
+    </row>
+    <row r="150" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B150" s="41" t="s">
+        <v>473</v>
+      </c>
+      <c r="C150" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D150" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E150" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F150" s="41"/>
+      <c r="G150" s="41"/>
+      <c r="H150" s="41"/>
+      <c r="I150" s="41"/>
+      <c r="J150" s="41"/>
+      <c r="K150" s="41"/>
+      <c r="L150" s="41"/>
+      <c r="M150" s="41"/>
+      <c r="N150" s="41"/>
+      <c r="O150" s="41"/>
+      <c r="P150" s="41"/>
+      <c r="Q150" s="41"/>
+      <c r="R150" s="41"/>
+      <c r="S150" s="41"/>
+      <c r="T150" s="41"/>
+      <c r="U150" s="41"/>
+      <c r="V150" s="41"/>
+      <c r="W150" s="41"/>
+      <c r="X150" s="41"/>
+    </row>
+    <row r="151" spans="1:26" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="10"/>
+      <c r="B151" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E151" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F151" s="10"/>
+      <c r="G151" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H151" s="10"/>
+      <c r="I151" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="J151" s="10"/>
+      <c r="K151" s="10"/>
+      <c r="L151" s="10"/>
+      <c r="M151" s="10"/>
+      <c r="N151" s="10"/>
+      <c r="O151" s="10"/>
+      <c r="P151" s="10"/>
+      <c r="Q151" s="10"/>
+      <c r="R151" s="10"/>
+      <c r="S151" s="10"/>
+      <c r="T151" s="10"/>
+      <c r="U151" s="10"/>
+      <c r="V151" s="10"/>
+      <c r="W151" s="10"/>
+      <c r="X151" s="10"/>
+      <c r="Y151" s="15"/>
+      <c r="Z151" s="15"/>
+    </row>
+    <row r="152" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A152" s="42"/>
+      <c r="B152" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C152" s="42"/>
+      <c r="D152" s="42" t="s">
+        <v>474</v>
+      </c>
+      <c r="E152" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="F152" s="42"/>
+      <c r="G152" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H152" s="42"/>
+      <c r="I152" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="J152" s="42"/>
+      <c r="K152" s="42">
+        <v>0</v>
+      </c>
+      <c r="L152" s="42">
+        <v>1</v>
+      </c>
+      <c r="M152" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="N152" s="42">
+        <v>0.1666667</v>
+      </c>
+      <c r="O152" s="42"/>
+      <c r="P152" s="42"/>
+      <c r="Q152" s="42"/>
+      <c r="R152" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="S152" s="42"/>
+      <c r="T152" s="42"/>
+      <c r="U152" s="42"/>
+      <c r="V152" s="42"/>
+      <c r="W152" s="42"/>
+      <c r="X152" s="42"/>
+    </row>
+    <row r="153" spans="1:26" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="B153" s="43" t="s">
+        <v>339</v>
+      </c>
+      <c r="C153" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="D153" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="E153" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="F153" s="43"/>
+      <c r="G153" s="43"/>
+      <c r="H153" s="44"/>
+      <c r="I153" s="44"/>
+      <c r="J153" s="43"/>
+      <c r="K153" s="43"/>
+      <c r="L153" s="43"/>
+      <c r="M153" s="43"/>
+      <c r="N153" s="43"/>
+      <c r="O153" s="43"/>
+      <c r="P153" s="43"/>
+      <c r="Q153" s="43"/>
+      <c r="R153" s="43"/>
+      <c r="S153" s="43"/>
+      <c r="T153" s="43"/>
+      <c r="U153" s="43"/>
+      <c r="V153" s="43"/>
+      <c r="W153" s="43"/>
+      <c r="X153" s="43"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -11287,11 +11962,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11407,16 +12082,16 @@
     </row>
     <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
@@ -11434,16 +12109,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G5" s="15" t="b">
         <v>0</v>
@@ -11461,16 +12136,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G6" s="15" t="b">
         <v>0</v>
@@ -11488,16 +12163,16 @@
     </row>
     <row r="7" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G7" s="15" t="b">
         <v>0</v>
@@ -11515,16 +12190,16 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G8" s="15" t="b">
         <v>0</v>
@@ -11542,16 +12217,16 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G9" s="15" t="b">
         <v>0</v>
@@ -11569,16 +12244,16 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G10" s="15" t="b">
         <v>0</v>
@@ -11596,16 +12271,16 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G11" s="15" t="b">
         <v>0</v>
@@ -11623,16 +12298,16 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G12" s="15" t="b">
         <v>0</v>
@@ -11650,16 +12325,16 @@
     </row>
     <row r="13" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G13" s="15" t="b">
         <v>0</v>
@@ -11677,16 +12352,16 @@
     </row>
     <row r="14" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -11704,16 +12379,16 @@
     </row>
     <row r="15" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G15" s="15" t="b">
         <v>0</v>
@@ -11731,16 +12406,16 @@
     </row>
     <row r="16" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -11758,16 +12433,16 @@
     </row>
     <row r="17" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -11785,16 +12460,16 @@
     </row>
     <row r="18" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -11812,16 +12487,16 @@
     </row>
     <row r="19" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -11839,16 +12514,16 @@
     </row>
     <row r="20" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -11866,16 +12541,16 @@
     </row>
     <row r="21" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>0</v>
@@ -11893,14 +12568,14 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B22" s="22"/>
       <c r="D22" s="15" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>0</v>
@@ -11914,14 +12589,14 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="B23" s="22"/>
       <c r="D23" s="15" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>0</v>
@@ -11935,14 +12610,14 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B24" s="22"/>
       <c r="D24" s="15" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>0</v>
@@ -11956,14 +12631,14 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="B25" s="22"/>
       <c r="D25" s="15" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G25" s="15" t="b">
         <v>0</v>
@@ -11977,14 +12652,14 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>403</v>
+        <v>459</v>
       </c>
       <c r="B26" s="22"/>
       <c r="D26" s="15" t="s">
-        <v>443</v>
+        <v>460</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G26" s="15" t="b">
         <v>0</v>
@@ -11998,14 +12673,14 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="B27" s="22"/>
       <c r="D27" s="15" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G27" s="15" t="b">
         <v>0</v>
@@ -12019,14 +12694,14 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="B28" s="22"/>
       <c r="D28" s="15" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G28" s="15" t="b">
         <v>0</v>
@@ -12040,14 +12715,14 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="B29" s="22"/>
       <c r="D29" s="15" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G29" s="15" t="b">
         <v>0</v>
@@ -12061,14 +12736,14 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="B30" s="22"/>
       <c r="D30" s="15" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G30" s="15" t="b">
         <v>0</v>
@@ -12082,14 +12757,14 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="B31" s="22"/>
       <c r="D31" s="15" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G31" s="15" t="b">
         <v>0</v>
@@ -12103,14 +12778,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="B32" s="22"/>
       <c r="D32" s="15" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G32" s="15" t="b">
         <v>0</v>
@@ -12124,14 +12799,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="B33" s="22"/>
       <c r="D33" s="15" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G33" s="15" t="b">
         <v>0</v>
@@ -12145,14 +12820,14 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="B34" s="22"/>
       <c r="D34" s="15" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G34" s="15" t="b">
         <v>0</v>
@@ -12166,14 +12841,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="B35" s="22"/>
       <c r="D35" s="15" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G35" s="15" t="b">
         <v>0</v>
@@ -12187,14 +12862,14 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="B36" s="22"/>
       <c r="D36" s="15" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G36" s="15" t="b">
         <v>0</v>
@@ -12208,14 +12883,14 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="B37" s="22"/>
       <c r="D37" s="15" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G37" s="15" t="b">
         <v>0</v>
@@ -12229,14 +12904,14 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="B38" s="22"/>
       <c r="D38" s="15" t="s">
-        <v>455</v>
+        <v>409</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G38" s="15" t="b">
         <v>0</v>
@@ -12250,14 +12925,14 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="B39" s="22"/>
       <c r="D39" s="15" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G39" s="15" t="b">
         <v>0</v>
@@ -12271,14 +12946,14 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="B40" s="22"/>
       <c r="D40" s="15" t="s">
-        <v>456</v>
+        <v>410</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G40" s="15" t="b">
         <v>0</v>
@@ -12292,14 +12967,14 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="B41" s="22"/>
       <c r="D41" s="15" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G41" s="15" t="b">
         <v>0</v>
@@ -12313,14 +12988,14 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="B42" s="22"/>
       <c r="D42" s="15" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G42" s="15" t="b">
         <v>0</v>
@@ -12334,14 +13009,14 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="B43" s="22"/>
       <c r="D43" s="15" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G43" s="15" t="b">
         <v>0</v>
@@ -12355,14 +13030,15 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>421</v>
+        <v>482</v>
       </c>
       <c r="B44" s="22"/>
       <c r="D44" s="15" t="s">
-        <v>458</v>
-      </c>
+        <v>493</v>
+      </c>
+      <c r="E44" s="23"/>
       <c r="F44" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G44" s="15" t="b">
         <v>0</v>
@@ -12376,14 +13052,15 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="B45" s="22"/>
       <c r="D45" s="15" t="s">
-        <v>459</v>
-      </c>
+        <v>494</v>
+      </c>
+      <c r="E45" s="23"/>
       <c r="F45" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G45" s="15" t="b">
         <v>0</v>
@@ -12397,14 +13074,15 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>423</v>
+        <v>484</v>
       </c>
       <c r="B46" s="22"/>
       <c r="D46" s="15" t="s">
-        <v>460</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="E46" s="23"/>
       <c r="F46" s="15" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G46" s="15" t="b">
         <v>0</v>
@@ -12417,57 +13095,152 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="46" t="s">
+        <v>485</v>
+      </c>
       <c r="B47" s="22"/>
+      <c r="D47" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="E47" s="23"/>
+      <c r="F47" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G47" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
+        <v>486</v>
+      </c>
       <c r="B48" s="22"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D48" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="E48" s="23"/>
+      <c r="F48" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G48" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="46" t="s">
+        <v>488</v>
+      </c>
       <c r="B49" s="22"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D49" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="E49" s="23"/>
+      <c r="F49" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G49" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="46" t="s">
+        <v>487</v>
+      </c>
       <c r="B50" s="22"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D50" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="E50" s="23"/>
+      <c r="F50" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G50" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="46" t="s">
+        <v>492</v>
+      </c>
       <c r="B51" s="22"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D51" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="E51" s="23"/>
+      <c r="F51" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G51" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" s="22"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" s="22"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" s="22"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="22"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" s="22"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" s="22"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="22"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="22"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="22"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="22"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="22"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="22"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" s="22"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -12493,15 +13266,6 @@
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="22"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="22"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="22"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implemented quota-based sampling to map to BEopt options. Temporarily disabling garages from model.
Addresses #6 and #2.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -785,9 +785,6 @@
     <t>SetResStockMode</t>
   </si>
   <si>
-    <t>National</t>
-  </si>
-  <si>
     <t>Set Res Stock Mode - National</t>
   </si>
   <si>
@@ -1542,6 +1539,9 @@
   </si>
   <si>
     <t>res_stock_reporting.misc_well_pump</t>
+  </si>
+  <si>
+    <t>national</t>
   </si>
 </sst>
 </file>
@@ -5301,7 +5301,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>158</v>
@@ -5312,7 +5312,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>158</v>
@@ -5647,7 +5647,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5679,7 +5679,7 @@
         <v>38</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>58</v>
@@ -5776,8 +5776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,7 +5960,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>247</v>
@@ -5998,10 +5998,10 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>248</v>
+        <v>500</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -6034,7 +6034,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>240</v>
@@ -6072,7 +6072,7 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>243</v>
@@ -6083,7 +6083,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E8" s="42" t="s">
         <v>242</v>
@@ -6154,7 +6154,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C9" s="41" t="s">
         <v>240</v>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>243</v>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E11" s="42" t="s">
         <v>242</v>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>243</v>
@@ -6350,7 +6350,7 @@
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E14" s="42" t="s">
         <v>242</v>
@@ -6394,7 +6394,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>240</v>
@@ -6432,7 +6432,7 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>243</v>
@@ -6443,7 +6443,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6470,7 +6470,7 @@
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>242</v>
@@ -6514,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C18" s="41" t="s">
         <v>240</v>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>243</v>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6590,7 +6590,7 @@
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="42" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E20" s="42" t="s">
         <v>242</v>
@@ -6634,7 +6634,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C21" s="41" t="s">
         <v>240</v>
@@ -6672,7 +6672,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>243</v>
@@ -6683,7 +6683,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6710,7 +6710,7 @@
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E23" s="42" t="s">
         <v>242</v>
@@ -6754,7 +6754,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>240</v>
@@ -6792,7 +6792,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>243</v>
@@ -6803,7 +6803,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -6830,7 +6830,7 @@
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E26" s="42" t="s">
         <v>242</v>
@@ -6874,7 +6874,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>240</v>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>243</v>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -6950,7 +6950,7 @@
       </c>
       <c r="C29" s="42"/>
       <c r="D29" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E29" s="42" t="s">
         <v>242</v>
@@ -6994,7 +6994,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C30" s="41" t="s">
         <v>240</v>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>243</v>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7070,7 +7070,7 @@
       </c>
       <c r="C32" s="42"/>
       <c r="D32" s="42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E32" s="42" t="s">
         <v>242</v>
@@ -7114,7 +7114,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C33" s="41" t="s">
         <v>240</v>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>243</v>
@@ -7163,7 +7163,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7190,7 +7190,7 @@
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E35" s="42" t="s">
         <v>242</v>
@@ -7234,7 +7234,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C36" s="41" t="s">
         <v>240</v>
@@ -7272,7 +7272,7 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>243</v>
@@ -7283,7 +7283,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7310,7 +7310,7 @@
       </c>
       <c r="C38" s="42"/>
       <c r="D38" s="42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>242</v>
@@ -7354,7 +7354,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C39" s="41" t="s">
         <v>240</v>
@@ -7392,7 +7392,7 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>243</v>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7430,7 +7430,7 @@
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="42" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E41" s="42" t="s">
         <v>242</v>
@@ -7474,7 +7474,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C42" s="41" t="s">
         <v>240</v>
@@ -7512,7 +7512,7 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>243</v>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7550,7 +7550,7 @@
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E44" s="42" t="s">
         <v>242</v>
@@ -7594,7 +7594,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C45" s="41" t="s">
         <v>240</v>
@@ -7632,7 +7632,7 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>243</v>
@@ -7643,7 +7643,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7670,7 +7670,7 @@
       </c>
       <c r="C47" s="42"/>
       <c r="D47" s="42" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E47" s="42" t="s">
         <v>242</v>
@@ -7714,7 +7714,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C48" s="41" t="s">
         <v>240</v>
@@ -7752,7 +7752,7 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>243</v>
@@ -7763,7 +7763,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E50" s="42" t="s">
         <v>242</v>
@@ -7834,7 +7834,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C51" s="41" t="s">
         <v>240</v>
@@ -7872,7 +7872,7 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>243</v>
@@ -7910,7 +7910,7 @@
       </c>
       <c r="C53" s="42"/>
       <c r="D53" s="42" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E53" s="42" t="s">
         <v>242</v>
@@ -7954,7 +7954,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C54" s="41" t="s">
         <v>240</v>
@@ -7992,7 +7992,7 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>243</v>
@@ -8003,7 +8003,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8030,7 +8030,7 @@
       </c>
       <c r="C56" s="42"/>
       <c r="D56" s="42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E56" s="42" t="s">
         <v>242</v>
@@ -8074,7 +8074,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C57" s="41" t="s">
         <v>240</v>
@@ -8112,7 +8112,7 @@
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>243</v>
@@ -8123,7 +8123,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8150,7 +8150,7 @@
       </c>
       <c r="C59" s="42"/>
       <c r="D59" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E59" s="42" t="s">
         <v>242</v>
@@ -8194,7 +8194,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C60" s="41" t="s">
         <v>240</v>
@@ -8232,7 +8232,7 @@
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>243</v>
@@ -8243,7 +8243,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8270,7 +8270,7 @@
       </c>
       <c r="C62" s="42"/>
       <c r="D62" s="42" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E62" s="42" t="s">
         <v>242</v>
@@ -8314,7 +8314,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C63" s="41" t="s">
         <v>240</v>
@@ -8352,7 +8352,7 @@
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>243</v>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8390,7 +8390,7 @@
       </c>
       <c r="C65" s="42"/>
       <c r="D65" s="42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E65" s="42" t="s">
         <v>242</v>
@@ -8434,7 +8434,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="41" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C66" s="41" t="s">
         <v>240</v>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>243</v>
@@ -8483,7 +8483,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8510,7 +8510,7 @@
       </c>
       <c r="C68" s="42"/>
       <c r="D68" s="42" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E68" s="42" t="s">
         <v>242</v>
@@ -8554,7 +8554,7 @@
         <v>0</v>
       </c>
       <c r="B69" s="41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C69" s="41" t="s">
         <v>240</v>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>243</v>
@@ -8603,7 +8603,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8630,7 +8630,7 @@
       </c>
       <c r="C71" s="42"/>
       <c r="D71" s="42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E71" s="42" t="s">
         <v>242</v>
@@ -8674,7 +8674,7 @@
         <v>1</v>
       </c>
       <c r="B72" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C72" s="41" t="s">
         <v>240</v>
@@ -8712,7 +8712,7 @@
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>243</v>
@@ -8723,7 +8723,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -8750,7 +8750,7 @@
       </c>
       <c r="C74" s="42"/>
       <c r="D74" s="42" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E74" s="42" t="s">
         <v>242</v>
@@ -8794,7 +8794,7 @@
         <v>1</v>
       </c>
       <c r="B75" s="41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C75" s="41" t="s">
         <v>240</v>
@@ -8832,7 +8832,7 @@
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>243</v>
@@ -8843,7 +8843,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8870,7 +8870,7 @@
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="42" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>242</v>
@@ -8914,7 +8914,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C78" s="41" t="s">
         <v>240</v>
@@ -8952,7 +8952,7 @@
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>243</v>
@@ -8963,7 +8963,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -8990,7 +8990,7 @@
       </c>
       <c r="C80" s="42"/>
       <c r="D80" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E80" s="42" t="s">
         <v>242</v>
@@ -9034,7 +9034,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="41" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C81" s="41" t="s">
         <v>240</v>
@@ -9072,7 +9072,7 @@
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>243</v>
@@ -9083,7 +9083,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9110,7 +9110,7 @@
       </c>
       <c r="C83" s="42"/>
       <c r="D83" s="42" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E83" s="42" t="s">
         <v>242</v>
@@ -9154,7 +9154,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="41" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C84" s="41" t="s">
         <v>240</v>
@@ -9192,7 +9192,7 @@
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>243</v>
@@ -9203,7 +9203,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9230,7 +9230,7 @@
       </c>
       <c r="C86" s="42"/>
       <c r="D86" s="42" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E86" s="42" t="s">
         <v>242</v>
@@ -9274,7 +9274,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="41" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C87" s="41" t="s">
         <v>240</v>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>243</v>
@@ -9323,7 +9323,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9350,7 +9350,7 @@
       </c>
       <c r="C89" s="42"/>
       <c r="D89" s="42" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E89" s="42" t="s">
         <v>242</v>
@@ -9394,7 +9394,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="41" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C90" s="41" t="s">
         <v>240</v>
@@ -9432,7 +9432,7 @@
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>243</v>
@@ -9443,7 +9443,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9470,7 +9470,7 @@
       </c>
       <c r="C92" s="42"/>
       <c r="D92" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E92" s="42" t="s">
         <v>242</v>
@@ -9514,7 +9514,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C93" s="41" t="s">
         <v>240</v>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>243</v>
@@ -9563,7 +9563,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9590,7 +9590,7 @@
       </c>
       <c r="C95" s="42"/>
       <c r="D95" s="42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E95" s="42" t="s">
         <v>242</v>
@@ -9634,7 +9634,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C96" s="41" t="s">
         <v>240</v>
@@ -9672,7 +9672,7 @@
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>243</v>
@@ -9683,7 +9683,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9710,7 +9710,7 @@
       </c>
       <c r="C98" s="42"/>
       <c r="D98" s="42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E98" s="42" t="s">
         <v>242</v>
@@ -9754,7 +9754,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C99" s="41" t="s">
         <v>240</v>
@@ -9792,7 +9792,7 @@
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>243</v>
@@ -9803,7 +9803,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9830,7 +9830,7 @@
       </c>
       <c r="C101" s="42"/>
       <c r="D101" s="42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E101" s="42" t="s">
         <v>242</v>
@@ -9874,7 +9874,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C102" s="41" t="s">
         <v>240</v>
@@ -9912,7 +9912,7 @@
       </c>
       <c r="C103" s="10"/>
       <c r="D103" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>243</v>
@@ -9923,7 +9923,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -9950,7 +9950,7 @@
       </c>
       <c r="C104" s="42"/>
       <c r="D104" s="42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E104" s="42" t="s">
         <v>242</v>
@@ -9994,7 +9994,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C105" s="41" t="s">
         <v>240</v>
@@ -10032,7 +10032,7 @@
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E106" s="10" t="s">
         <v>243</v>
@@ -10043,7 +10043,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10070,7 +10070,7 @@
       </c>
       <c r="C107" s="42"/>
       <c r="D107" s="42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E107" s="42" t="s">
         <v>242</v>
@@ -10114,7 +10114,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="41" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C108" s="41" t="s">
         <v>240</v>
@@ -10152,7 +10152,7 @@
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E109" s="10" t="s">
         <v>243</v>
@@ -10163,7 +10163,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10190,7 +10190,7 @@
       </c>
       <c r="C110" s="42"/>
       <c r="D110" s="42" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E110" s="42" t="s">
         <v>242</v>
@@ -10234,7 +10234,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C111" s="41" t="s">
         <v>240</v>
@@ -10272,7 +10272,7 @@
       </c>
       <c r="C112" s="10"/>
       <c r="D112" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E112" s="10" t="s">
         <v>243</v>
@@ -10283,7 +10283,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10310,7 +10310,7 @@
       </c>
       <c r="C113" s="42"/>
       <c r="D113" s="42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E113" s="42" t="s">
         <v>242</v>
@@ -10354,7 +10354,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C114" s="41" t="s">
         <v>240</v>
@@ -10392,7 +10392,7 @@
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>243</v>
@@ -10403,7 +10403,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10430,7 +10430,7 @@
       </c>
       <c r="C116" s="42"/>
       <c r="D116" s="42" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E116" s="42" t="s">
         <v>242</v>
@@ -10474,7 +10474,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C117" s="41" t="s">
         <v>240</v>
@@ -10512,7 +10512,7 @@
       </c>
       <c r="C118" s="10"/>
       <c r="D118" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E118" s="10" t="s">
         <v>243</v>
@@ -10523,7 +10523,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10550,7 +10550,7 @@
       </c>
       <c r="C119" s="42"/>
       <c r="D119" s="42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E119" s="42" t="s">
         <v>242</v>
@@ -10594,7 +10594,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="41" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C120" s="41" t="s">
         <v>240</v>
@@ -10632,7 +10632,7 @@
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>243</v>
@@ -10643,7 +10643,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10670,7 +10670,7 @@
       </c>
       <c r="C122" s="42"/>
       <c r="D122" s="42" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E122" s="42" t="s">
         <v>242</v>
@@ -10714,7 +10714,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="41" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C123" s="41" t="s">
         <v>240</v>
@@ -10752,7 +10752,7 @@
       </c>
       <c r="C124" s="10"/>
       <c r="D124" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E124" s="10" t="s">
         <v>243</v>
@@ -10763,7 +10763,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10790,7 +10790,7 @@
       </c>
       <c r="C125" s="42"/>
       <c r="D125" s="42" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E125" s="42" t="s">
         <v>242</v>
@@ -10834,7 +10834,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C126" s="41" t="s">
         <v>240</v>
@@ -10872,7 +10872,7 @@
       </c>
       <c r="C127" s="10"/>
       <c r="D127" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E127" s="10" t="s">
         <v>243</v>
@@ -10883,7 +10883,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10910,7 +10910,7 @@
       </c>
       <c r="C128" s="42"/>
       <c r="D128" s="42" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E128" s="42" t="s">
         <v>242</v>
@@ -10954,7 +10954,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="41" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C129" s="41" t="s">
         <v>240</v>
@@ -10992,7 +10992,7 @@
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>243</v>
@@ -11003,7 +11003,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11030,7 +11030,7 @@
       </c>
       <c r="C131" s="42"/>
       <c r="D131" s="42" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E131" s="42" t="s">
         <v>242</v>
@@ -11074,7 +11074,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="41" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C132" s="41" t="s">
         <v>240</v>
@@ -11112,7 +11112,7 @@
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>243</v>
@@ -11123,7 +11123,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11150,7 +11150,7 @@
       </c>
       <c r="C134" s="42"/>
       <c r="D134" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E134" s="42" t="s">
         <v>242</v>
@@ -11194,7 +11194,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C135" s="41" t="s">
         <v>240</v>
@@ -11232,7 +11232,7 @@
       </c>
       <c r="C136" s="10"/>
       <c r="D136" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E136" s="10" t="s">
         <v>243</v>
@@ -11243,7 +11243,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11270,7 +11270,7 @@
       </c>
       <c r="C137" s="42"/>
       <c r="D137" s="42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E137" s="42" t="s">
         <v>242</v>
@@ -11314,7 +11314,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="41" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C138" s="41" t="s">
         <v>240</v>
@@ -11352,7 +11352,7 @@
       </c>
       <c r="C139" s="10"/>
       <c r="D139" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>243</v>
@@ -11363,7 +11363,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11390,7 +11390,7 @@
       </c>
       <c r="C140" s="42"/>
       <c r="D140" s="42" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E140" s="42" t="s">
         <v>242</v>
@@ -11434,7 +11434,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="41" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C141" s="41" t="s">
         <v>240</v>
@@ -11472,7 +11472,7 @@
       </c>
       <c r="C142" s="10"/>
       <c r="D142" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E142" s="10" t="s">
         <v>243</v>
@@ -11483,7 +11483,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11510,7 +11510,7 @@
       </c>
       <c r="C143" s="42"/>
       <c r="D143" s="42" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E143" s="42" t="s">
         <v>242</v>
@@ -11554,7 +11554,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="41" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C144" s="41" t="s">
         <v>240</v>
@@ -11592,7 +11592,7 @@
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E145" s="10" t="s">
         <v>243</v>
@@ -11603,7 +11603,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11630,7 +11630,7 @@
       </c>
       <c r="C146" s="42"/>
       <c r="D146" s="42" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E146" s="42" t="s">
         <v>242</v>
@@ -11674,7 +11674,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="41" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C147" s="41" t="s">
         <v>240</v>
@@ -11712,7 +11712,7 @@
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E148" s="10" t="s">
         <v>243</v>
@@ -11723,7 +11723,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11750,7 +11750,7 @@
       </c>
       <c r="C149" s="42"/>
       <c r="D149" s="42" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E149" s="42" t="s">
         <v>242</v>
@@ -11794,7 +11794,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="41" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C150" s="41" t="s">
         <v>240</v>
@@ -11832,7 +11832,7 @@
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E151" s="10" t="s">
         <v>243</v>
@@ -11843,7 +11843,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11870,7 +11870,7 @@
       </c>
       <c r="C152" s="42"/>
       <c r="D152" s="42" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E152" s="42" t="s">
         <v>242</v>
@@ -11914,16 +11914,16 @@
         <v>1</v>
       </c>
       <c r="B153" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="C153" s="43" t="s">
         <v>339</v>
       </c>
-      <c r="C153" s="43" t="s">
-        <v>340</v>
-      </c>
       <c r="D153" s="43" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E153" s="43" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F153" s="43"/>
       <c r="G153" s="43"/>
@@ -11964,7 +11964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
@@ -12082,16 +12082,16 @@
     </row>
     <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
@@ -12109,16 +12109,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G5" s="15" t="b">
         <v>0</v>
@@ -12136,16 +12136,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G6" s="15" t="b">
         <v>0</v>
@@ -12163,16 +12163,16 @@
     </row>
     <row r="7" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G7" s="15" t="b">
         <v>0</v>
@@ -12190,16 +12190,16 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G8" s="15" t="b">
         <v>0</v>
@@ -12217,16 +12217,16 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G9" s="15" t="b">
         <v>0</v>
@@ -12244,16 +12244,16 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G10" s="15" t="b">
         <v>0</v>
@@ -12271,16 +12271,16 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G11" s="15" t="b">
         <v>0</v>
@@ -12298,16 +12298,16 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G12" s="15" t="b">
         <v>0</v>
@@ -12325,16 +12325,16 @@
     </row>
     <row r="13" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G13" s="15" t="b">
         <v>0</v>
@@ -12352,16 +12352,16 @@
     </row>
     <row r="14" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -12379,16 +12379,16 @@
     </row>
     <row r="15" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G15" s="15" t="b">
         <v>0</v>
@@ -12406,16 +12406,16 @@
     </row>
     <row r="16" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -12433,16 +12433,16 @@
     </row>
     <row r="17" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -12460,16 +12460,16 @@
     </row>
     <row r="18" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -12487,16 +12487,16 @@
     </row>
     <row r="19" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -12514,16 +12514,16 @@
     </row>
     <row r="20" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -12541,16 +12541,16 @@
     </row>
     <row r="21" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>0</v>
@@ -12568,14 +12568,14 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B22" s="22"/>
       <c r="D22" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>0</v>
@@ -12589,14 +12589,14 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B23" s="22"/>
       <c r="D23" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>0</v>
@@ -12610,14 +12610,14 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B24" s="22"/>
       <c r="D24" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>0</v>
@@ -12631,14 +12631,14 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B25" s="22"/>
       <c r="D25" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G25" s="15" t="b">
         <v>0</v>
@@ -12652,14 +12652,14 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B26" s="22"/>
       <c r="D26" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G26" s="15" t="b">
         <v>0</v>
@@ -12673,14 +12673,14 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B27" s="22"/>
       <c r="D27" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G27" s="15" t="b">
         <v>0</v>
@@ -12694,14 +12694,14 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B28" s="22"/>
       <c r="D28" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G28" s="15" t="b">
         <v>0</v>
@@ -12715,14 +12715,14 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B29" s="22"/>
       <c r="D29" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G29" s="15" t="b">
         <v>0</v>
@@ -12736,14 +12736,14 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B30" s="22"/>
       <c r="D30" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G30" s="15" t="b">
         <v>0</v>
@@ -12757,14 +12757,14 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B31" s="22"/>
       <c r="D31" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G31" s="15" t="b">
         <v>0</v>
@@ -12778,14 +12778,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B32" s="22"/>
       <c r="D32" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G32" s="15" t="b">
         <v>0</v>
@@ -12799,14 +12799,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B33" s="22"/>
       <c r="D33" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G33" s="15" t="b">
         <v>0</v>
@@ -12820,14 +12820,14 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B34" s="22"/>
       <c r="D34" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G34" s="15" t="b">
         <v>0</v>
@@ -12841,14 +12841,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B35" s="22"/>
       <c r="D35" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G35" s="15" t="b">
         <v>0</v>
@@ -12862,14 +12862,14 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B36" s="22"/>
       <c r="D36" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G36" s="15" t="b">
         <v>0</v>
@@ -12883,14 +12883,14 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B37" s="22"/>
       <c r="D37" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G37" s="15" t="b">
         <v>0</v>
@@ -12904,14 +12904,14 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B38" s="22"/>
       <c r="D38" s="15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G38" s="15" t="b">
         <v>0</v>
@@ -12925,14 +12925,14 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B39" s="22"/>
       <c r="D39" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G39" s="15" t="b">
         <v>0</v>
@@ -12946,14 +12946,14 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B40" s="22"/>
       <c r="D40" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G40" s="15" t="b">
         <v>0</v>
@@ -12967,14 +12967,14 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B41" s="22"/>
       <c r="D41" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G41" s="15" t="b">
         <v>0</v>
@@ -12988,14 +12988,14 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B42" s="22"/>
       <c r="D42" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G42" s="15" t="b">
         <v>0</v>
@@ -13009,14 +13009,14 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B43" s="22"/>
       <c r="D43" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G43" s="15" t="b">
         <v>0</v>
@@ -13030,15 +13030,15 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B44" s="22"/>
       <c r="D44" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E44" s="23"/>
       <c r="F44" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G44" s="15" t="b">
         <v>0</v>
@@ -13052,15 +13052,15 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B45" s="22"/>
       <c r="D45" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E45" s="23"/>
       <c r="F45" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G45" s="15" t="b">
         <v>0</v>
@@ -13074,15 +13074,15 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B46" s="22"/>
       <c r="D46" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E46" s="23"/>
       <c r="F46" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G46" s="15" t="b">
         <v>0</v>
@@ -13096,15 +13096,15 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B47" s="22"/>
       <c r="D47" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E47" s="23"/>
       <c r="F47" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G47" s="15" t="b">
         <v>0</v>
@@ -13118,15 +13118,15 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B48" s="22"/>
       <c r="D48" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E48" s="23"/>
       <c r="F48" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G48" s="15" t="b">
         <v>0</v>
@@ -13140,15 +13140,15 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B49" s="22"/>
       <c r="D49" s="15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E49" s="23"/>
       <c r="F49" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G49" s="15" t="b">
         <v>0</v>
@@ -13162,15 +13162,15 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="46" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B50" s="22"/>
       <c r="D50" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E50" s="23"/>
       <c r="F50" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G50" s="15" t="b">
         <v>0</v>
@@ -13184,15 +13184,15 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B51" s="22"/>
       <c r="D51" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E51" s="23"/>
       <c r="F51" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G51" s="15" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Reverted quota-based sampling. Added window area and construction measures. Latest measures.
Quota-based sampling won't work for parameters with dependencies.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="508">
   <si>
     <t>type</t>
   </si>
@@ -1533,6 +1533,36 @@
   </si>
   <si>
     <t>national</t>
+  </si>
+  <si>
+    <t>Window Areas</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.window_areas</t>
+  </si>
+  <si>
+    <t>Set Window Areas</t>
+  </si>
+  <si>
+    <t>Window Areas Sample Value</t>
+  </si>
+  <si>
+    <t>window_areas.txt</t>
+  </si>
+  <si>
+    <t>Set Windows</t>
+  </si>
+  <si>
+    <t>Windows Sample Value</t>
+  </si>
+  <si>
+    <t>windows.txt</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.windows</t>
   </si>
 </sst>
 </file>
@@ -5106,8 +5136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5398,14 +5428,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="E24" s="22"/>
     </row>
@@ -5737,10 +5767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z153"/>
+  <dimension ref="A1:Z159"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I151" sqref="I151"/>
+    <sheetView topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7557,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>437</v>
+        <v>328</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>237</v>
@@ -7606,7 +7636,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>439</v>
+        <v>330</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7633,7 +7663,7 @@
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="41" t="s">
-        <v>438</v>
+        <v>329</v>
       </c>
       <c r="E47" s="41" t="s">
         <v>239</v>
@@ -7677,7 +7707,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>296</v>
+        <v>500</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>237</v>
@@ -7726,7 +7756,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>295</v>
+        <v>502</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -7753,7 +7783,7 @@
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="41" t="s">
-        <v>297</v>
+        <v>501</v>
       </c>
       <c r="E50" s="41" t="s">
         <v>239</v>
@@ -7797,7 +7827,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>267</v>
+        <v>437</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>237</v>
@@ -7846,7 +7876,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>242</v>
+        <v>439</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -7873,7 +7903,7 @@
       </c>
       <c r="C53" s="41"/>
       <c r="D53" s="41" t="s">
-        <v>268</v>
+        <v>438</v>
       </c>
       <c r="E53" s="41" t="s">
         <v>239</v>
@@ -7917,7 +7947,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>237</v>
@@ -7966,7 +7996,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -7993,7 +8023,7 @@
       </c>
       <c r="C56" s="41"/>
       <c r="D56" s="41" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="E56" s="41" t="s">
         <v>239</v>
@@ -8037,7 +8067,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>237</v>
@@ -8086,7 +8116,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8113,7 +8143,7 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="E59" s="41" t="s">
         <v>239</v>
@@ -8157,7 +8187,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>237</v>
@@ -8206,7 +8236,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8233,7 +8263,7 @@
       </c>
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>239</v>
@@ -8277,7 +8307,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C63" s="40" t="s">
         <v>237</v>
@@ -8326,7 +8356,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8353,7 +8383,7 @@
       </c>
       <c r="C65" s="41"/>
       <c r="D65" s="41" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E65" s="41" t="s">
         <v>239</v>
@@ -8397,7 +8427,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>237</v>
@@ -8446,7 +8476,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8473,7 +8503,7 @@
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="41" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>239</v>
@@ -8513,11 +8543,11 @@
       <c r="X68" s="41"/>
     </row>
     <row r="69" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="44" t="b">
-        <v>0</v>
+      <c r="A69" s="40" t="b">
+        <v>1</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C69" s="40" t="s">
         <v>237</v>
@@ -8566,7 +8596,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8593,7 +8623,7 @@
       </c>
       <c r="C71" s="41"/>
       <c r="D71" s="41" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E71" s="41" t="s">
         <v>239</v>
@@ -8637,7 +8667,7 @@
         <v>1</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C72" s="40" t="s">
         <v>237</v>
@@ -8686,7 +8716,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -8713,7 +8743,7 @@
       </c>
       <c r="C74" s="41"/>
       <c r="D74" s="41" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="E74" s="41" t="s">
         <v>239</v>
@@ -8753,11 +8783,11 @@
       <c r="X74" s="41"/>
     </row>
     <row r="75" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="40" t="b">
-        <v>1</v>
+      <c r="A75" s="44" t="b">
+        <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>452</v>
+        <v>292</v>
       </c>
       <c r="C75" s="40" t="s">
         <v>237</v>
@@ -8806,7 +8836,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>454</v>
+        <v>294</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8833,7 +8863,7 @@
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41" t="s">
-        <v>453</v>
+        <v>293</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>239</v>
@@ -8877,7 +8907,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C78" s="40" t="s">
         <v>237</v>
@@ -8926,7 +8956,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -8953,7 +8983,7 @@
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>239</v>
@@ -8997,7 +9027,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>304</v>
+        <v>452</v>
       </c>
       <c r="C81" s="40" t="s">
         <v>237</v>
@@ -9046,7 +9076,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>306</v>
+        <v>454</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9073,7 +9103,7 @@
       </c>
       <c r="C83" s="41"/>
       <c r="D83" s="41" t="s">
-        <v>305</v>
+        <v>453</v>
       </c>
       <c r="E83" s="41" t="s">
         <v>239</v>
@@ -9117,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C84" s="40" t="s">
         <v>237</v>
@@ -9166,7 +9196,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9193,7 +9223,7 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="41" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>239</v>
@@ -9237,7 +9267,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C87" s="40" t="s">
         <v>237</v>
@@ -9286,7 +9316,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9313,7 +9343,7 @@
       </c>
       <c r="C89" s="41"/>
       <c r="D89" s="41" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>239</v>
@@ -9357,7 +9387,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C90" s="40" t="s">
         <v>237</v>
@@ -9406,7 +9436,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9433,7 +9463,7 @@
       </c>
       <c r="C92" s="41"/>
       <c r="D92" s="41" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E92" s="41" t="s">
         <v>239</v>
@@ -9477,7 +9507,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C93" s="40" t="s">
         <v>237</v>
@@ -9526,7 +9556,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9553,7 +9583,7 @@
       </c>
       <c r="C95" s="41"/>
       <c r="D95" s="41" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E95" s="41" t="s">
         <v>239</v>
@@ -9597,7 +9627,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>237</v>
@@ -9646,7 +9676,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9673,7 +9703,7 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>239</v>
@@ -9717,7 +9747,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>237</v>
@@ -9766,7 +9796,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9793,7 +9823,7 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>239</v>
@@ -9837,7 +9867,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>237</v>
@@ -9886,7 +9916,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -9913,7 +9943,7 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>239</v>
@@ -9957,7 +9987,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>237</v>
@@ -10006,7 +10036,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10033,7 +10063,7 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>239</v>
@@ -10077,7 +10107,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>362</v>
+        <v>331</v>
       </c>
       <c r="C108" s="40" t="s">
         <v>237</v>
@@ -10126,7 +10156,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10153,7 +10183,7 @@
       </c>
       <c r="C110" s="41"/>
       <c r="D110" s="41" t="s">
-        <v>363</v>
+        <v>332</v>
       </c>
       <c r="E110" s="41" t="s">
         <v>239</v>
@@ -10197,7 +10227,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>338</v>
+        <v>503</v>
       </c>
       <c r="C111" s="40" t="s">
         <v>237</v>
@@ -10246,7 +10276,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>340</v>
+        <v>505</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10273,7 +10303,7 @@
       </c>
       <c r="C113" s="41"/>
       <c r="D113" s="41" t="s">
-        <v>339</v>
+        <v>504</v>
       </c>
       <c r="E113" s="41" t="s">
         <v>239</v>
@@ -10317,7 +10347,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>344</v>
+        <v>362</v>
       </c>
       <c r="C114" s="40" t="s">
         <v>237</v>
@@ -10366,7 +10396,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10393,7 +10423,7 @@
       </c>
       <c r="C116" s="41"/>
       <c r="D116" s="41" t="s">
-        <v>345</v>
+        <v>363</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>239</v>
@@ -10437,7 +10467,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>237</v>
@@ -10486,7 +10516,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10513,7 +10543,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>239</v>
@@ -10557,7 +10587,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>237</v>
@@ -10606,7 +10636,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10633,7 +10663,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>239</v>
@@ -10677,7 +10707,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>237</v>
@@ -10726,7 +10756,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10753,7 +10783,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>239</v>
@@ -10797,7 +10827,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>237</v>
@@ -10846,7 +10876,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10873,7 +10903,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>239</v>
@@ -10917,7 +10947,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>457</v>
+        <v>356</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>237</v>
@@ -10966,7 +10996,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>462</v>
+        <v>358</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -10993,7 +11023,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>458</v>
+        <v>357</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>239</v>
@@ -11037,7 +11067,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>472</v>
+        <v>359</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>237</v>
@@ -11086,7 +11116,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>474</v>
+        <v>361</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11113,7 +11143,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>473</v>
+        <v>360</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>239</v>
@@ -11157,7 +11187,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>237</v>
@@ -11206,7 +11236,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11233,7 +11263,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>239</v>
@@ -11277,7 +11307,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>459</v>
+        <v>472</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>237</v>
@@ -11326,7 +11356,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11353,7 +11383,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>460</v>
+        <v>473</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>239</v>
@@ -11397,7 +11427,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>237</v>
@@ -11446,7 +11476,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11473,7 +11503,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>239</v>
@@ -11517,7 +11547,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>237</v>
@@ -11566,7 +11596,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11593,7 +11623,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>239</v>
@@ -11637,7 +11667,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>237</v>
@@ -11686,7 +11716,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11713,7 +11743,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>239</v>
@@ -11757,7 +11787,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>469</v>
+        <v>485</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>237</v>
@@ -11806,7 +11836,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>471</v>
+        <v>487</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11833,7 +11863,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>470</v>
+        <v>486</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>239</v>
@@ -11872,41 +11902,281 @@
       <c r="W152" s="41"/>
       <c r="X152" s="41"/>
     </row>
-    <row r="153" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="42" t="b">
+    <row r="153" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B153" s="42" t="s">
+      <c r="B153" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="C153" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D153" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="E153" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F153" s="40"/>
+      <c r="G153" s="40"/>
+      <c r="H153" s="40"/>
+      <c r="I153" s="40"/>
+      <c r="J153" s="40"/>
+      <c r="K153" s="40"/>
+      <c r="L153" s="40"/>
+      <c r="M153" s="40"/>
+      <c r="N153" s="40"/>
+      <c r="O153" s="40"/>
+      <c r="P153" s="40"/>
+      <c r="Q153" s="40"/>
+      <c r="R153" s="40"/>
+      <c r="S153" s="40"/>
+      <c r="T153" s="40"/>
+      <c r="U153" s="40"/>
+      <c r="V153" s="40"/>
+      <c r="W153" s="40"/>
+      <c r="X153" s="40"/>
+    </row>
+    <row r="154" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="10"/>
+      <c r="B154" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C154" s="10"/>
+      <c r="D154" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E154" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F154" s="10"/>
+      <c r="G154" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H154" s="10"/>
+      <c r="I154" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="J154" s="10"/>
+      <c r="K154" s="10"/>
+      <c r="L154" s="10"/>
+      <c r="M154" s="10"/>
+      <c r="N154" s="10"/>
+      <c r="O154" s="10"/>
+      <c r="P154" s="10"/>
+      <c r="Q154" s="10"/>
+      <c r="R154" s="10"/>
+      <c r="S154" s="10"/>
+      <c r="T154" s="10"/>
+      <c r="U154" s="10"/>
+      <c r="V154" s="10"/>
+      <c r="W154" s="10"/>
+      <c r="X154" s="10"/>
+      <c r="Y154" s="15"/>
+      <c r="Z154" s="15"/>
+    </row>
+    <row r="155" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="41"/>
+      <c r="B155" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C155" s="41"/>
+      <c r="D155" s="41" t="s">
+        <v>467</v>
+      </c>
+      <c r="E155" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="F155" s="41"/>
+      <c r="G155" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H155" s="41"/>
+      <c r="I155" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J155" s="41"/>
+      <c r="K155" s="41">
+        <v>0</v>
+      </c>
+      <c r="L155" s="41">
+        <v>1</v>
+      </c>
+      <c r="M155" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N155" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O155" s="41"/>
+      <c r="P155" s="41"/>
+      <c r="Q155" s="41"/>
+      <c r="R155" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="S155" s="41"/>
+      <c r="T155" s="41"/>
+      <c r="U155" s="41"/>
+      <c r="V155" s="41"/>
+      <c r="W155" s="41"/>
+      <c r="X155" s="41"/>
+    </row>
+    <row r="156" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B156" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="C156" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D156" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="E156" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F156" s="40"/>
+      <c r="G156" s="40"/>
+      <c r="H156" s="40"/>
+      <c r="I156" s="40"/>
+      <c r="J156" s="40"/>
+      <c r="K156" s="40"/>
+      <c r="L156" s="40"/>
+      <c r="M156" s="40"/>
+      <c r="N156" s="40"/>
+      <c r="O156" s="40"/>
+      <c r="P156" s="40"/>
+      <c r="Q156" s="40"/>
+      <c r="R156" s="40"/>
+      <c r="S156" s="40"/>
+      <c r="T156" s="40"/>
+      <c r="U156" s="40"/>
+      <c r="V156" s="40"/>
+      <c r="W156" s="40"/>
+      <c r="X156" s="40"/>
+    </row>
+    <row r="157" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="10"/>
+      <c r="B157" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E157" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F157" s="10"/>
+      <c r="G157" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="J157" s="10"/>
+      <c r="K157" s="10"/>
+      <c r="L157" s="10"/>
+      <c r="M157" s="10"/>
+      <c r="N157" s="10"/>
+      <c r="O157" s="10"/>
+      <c r="P157" s="10"/>
+      <c r="Q157" s="10"/>
+      <c r="R157" s="10"/>
+      <c r="S157" s="10"/>
+      <c r="T157" s="10"/>
+      <c r="U157" s="10"/>
+      <c r="V157" s="10"/>
+      <c r="W157" s="10"/>
+      <c r="X157" s="10"/>
+      <c r="Y157" s="15"/>
+      <c r="Z157" s="15"/>
+    </row>
+    <row r="158" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A158" s="41"/>
+      <c r="B158" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158" s="41"/>
+      <c r="D158" s="41" t="s">
+        <v>470</v>
+      </c>
+      <c r="E158" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="F158" s="41"/>
+      <c r="G158" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H158" s="41"/>
+      <c r="I158" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J158" s="41"/>
+      <c r="K158" s="41">
+        <v>0</v>
+      </c>
+      <c r="L158" s="41">
+        <v>1</v>
+      </c>
+      <c r="M158" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N158" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O158" s="41"/>
+      <c r="P158" s="41"/>
+      <c r="Q158" s="41"/>
+      <c r="R158" s="41" t="s">
+        <v>225</v>
+      </c>
+      <c r="S158" s="41"/>
+      <c r="T158" s="41"/>
+      <c r="U158" s="41"/>
+      <c r="V158" s="41"/>
+      <c r="W158" s="41"/>
+      <c r="X158" s="41"/>
+    </row>
+    <row r="159" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A159" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B159" s="42" t="s">
         <v>335</v>
       </c>
-      <c r="C153" s="42" t="s">
+      <c r="C159" s="42" t="s">
         <v>336</v>
       </c>
-      <c r="D153" s="42" t="s">
+      <c r="D159" s="42" t="s">
         <v>336</v>
       </c>
-      <c r="E153" s="42" t="s">
+      <c r="E159" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="F153" s="42"/>
-      <c r="G153" s="42"/>
-      <c r="H153" s="43"/>
-      <c r="I153" s="43"/>
-      <c r="J153" s="42"/>
-      <c r="K153" s="42"/>
-      <c r="L153" s="42"/>
-      <c r="M153" s="42"/>
-      <c r="N153" s="42"/>
-      <c r="O153" s="42"/>
-      <c r="P153" s="42"/>
-      <c r="Q153" s="42"/>
-      <c r="R153" s="42"/>
-      <c r="S153" s="42"/>
-      <c r="T153" s="42"/>
-      <c r="U153" s="42"/>
-      <c r="V153" s="42"/>
-      <c r="W153" s="42"/>
-      <c r="X153" s="42"/>
+      <c r="F159" s="42"/>
+      <c r="G159" s="42"/>
+      <c r="H159" s="43"/>
+      <c r="I159" s="43"/>
+      <c r="J159" s="42"/>
+      <c r="K159" s="42"/>
+      <c r="L159" s="42"/>
+      <c r="M159" s="42"/>
+      <c r="N159" s="42"/>
+      <c r="O159" s="42"/>
+      <c r="P159" s="42"/>
+      <c r="Q159" s="42"/>
+      <c r="R159" s="42"/>
+      <c r="S159" s="42"/>
+      <c r="T159" s="42"/>
+      <c r="U159" s="42"/>
+      <c r="V159" s="42"/>
+      <c r="W159" s="42"/>
+      <c r="X159" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -11925,11 +12195,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12394,16 +12664,14 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="45" t="s">
+        <v>395</v>
+      </c>
+      <c r="B17" s="21"/>
       <c r="D17" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="E17" s="15"/>
+        <v>431</v>
+      </c>
       <c r="F17" s="15" t="s">
         <v>337</v>
       </c>
@@ -12416,21 +12684,15 @@
       <c r="I17" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+    </row>
+    <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
+        <v>498</v>
+      </c>
+      <c r="B18" s="21"/>
       <c r="D18" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="E18" s="15"/>
+        <v>499</v>
+      </c>
       <c r="F18" s="15" t="s">
         <v>337</v>
       </c>
@@ -12443,19 +12705,15 @@
       <c r="I18" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>380</v>
+        <v>440</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
@@ -12477,12 +12735,12 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
@@ -12504,12 +12762,12 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
@@ -12529,14 +12787,16 @@
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
-        <v>383</v>
-      </c>
-      <c r="B22" s="21"/>
+    <row r="22" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>419</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="E22" s="15"/>
       <c r="F22" s="15" t="s">
         <v>337</v>
       </c>
@@ -12549,15 +12809,21 @@
       <c r="I22" s="15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
-        <v>384</v>
-      </c>
-      <c r="B23" s="21"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+    </row>
+    <row r="23" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>420</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
         <v>337</v>
       </c>
@@ -12570,14 +12836,18 @@
       <c r="I23" s="15" t="b">
         <v>0</v>
       </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B24" s="21"/>
       <c r="D24" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>337</v>
@@ -12594,11 +12864,11 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B25" s="21"/>
       <c r="D25" s="15" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>337</v>
@@ -12615,11 +12885,11 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
-        <v>455</v>
+        <v>385</v>
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="15" t="s">
-        <v>456</v>
+        <v>421</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>337</v>
@@ -12636,11 +12906,11 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>337</v>
@@ -12657,11 +12927,11 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
-        <v>388</v>
+        <v>455</v>
       </c>
       <c r="B28" s="21"/>
       <c r="D28" s="15" t="s">
-        <v>424</v>
+        <v>456</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>337</v>
@@ -12678,11 +12948,11 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B29" s="21"/>
       <c r="D29" s="15" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>337</v>
@@ -12699,11 +12969,11 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B30" s="21"/>
       <c r="D30" s="15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>337</v>
@@ -12720,11 +12990,11 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B31" s="21"/>
       <c r="D31" s="15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>337</v>
@@ -12741,11 +13011,11 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B32" s="21"/>
       <c r="D32" s="15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>337</v>
@@ -12762,11 +13032,11 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="45" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B33" s="21"/>
       <c r="D33" s="15" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>337</v>
@@ -12783,11 +13053,11 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="45" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="15" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>337</v>
@@ -12804,11 +13074,11 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="45" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="15" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>337</v>
@@ -12825,11 +13095,11 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B36" s="21"/>
       <c r="D36" s="15" t="s">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>337</v>
@@ -12846,11 +13116,11 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="45" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B37" s="21"/>
       <c r="D37" s="15" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>337</v>
@@ -12865,13 +13135,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
-        <v>398</v>
+        <v>506</v>
       </c>
       <c r="B38" s="21"/>
       <c r="D38" s="15" t="s">
-        <v>405</v>
+        <v>507</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>337</v>
@@ -12888,11 +13158,11 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B39" s="21"/>
       <c r="D39" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>337</v>
@@ -12909,11 +13179,11 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>337</v>
@@ -12930,11 +13200,11 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>337</v>
@@ -12951,11 +13221,11 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>435</v>
+        <v>406</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>337</v>
@@ -12972,11 +13242,11 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>337</v>
@@ -12993,13 +13263,12 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="45" t="s">
-        <v>478</v>
+        <v>402</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="E44" s="22"/>
+        <v>435</v>
+      </c>
       <c r="F44" s="15" t="s">
         <v>337</v>
       </c>
@@ -13015,13 +13284,12 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
-        <v>479</v>
+        <v>403</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="E45" s="22"/>
+        <v>436</v>
+      </c>
       <c r="F45" s="15" t="s">
         <v>337</v>
       </c>
@@ -13037,11 +13305,11 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="45" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="15" t="s">
@@ -13059,11 +13327,11 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="45" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="15" t="s">
@@ -13081,11 +13349,11 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="45" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="15" t="s">
@@ -13103,11 +13371,11 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="45" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="15" t="s">
@@ -13125,11 +13393,11 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="45" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="15" t="s">
@@ -13147,11 +13415,11 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="45" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="15" t="s">
@@ -13168,10 +13436,48 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="45" t="s">
+        <v>483</v>
+      </c>
       <c r="B52" s="21"/>
+      <c r="D52" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="E52" s="22"/>
+      <c r="F52" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="G52" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="45" t="s">
+        <v>488</v>
+      </c>
       <c r="B53" s="21"/>
+      <c r="D53" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="E53" s="22"/>
+      <c r="F53" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="G53" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" s="21"/>
@@ -13229,6 +13535,12 @@
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="21"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="21"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Merged in PR #8 changes for running on AWS.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national.xlsx
+++ b/projects/res_stock_national.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -30,11 +30,6 @@
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -713,9 +708,6 @@
     <t>(TRUE/FALSE) If in_measure_combinations are TRUE, sets if static values be included in combinations</t>
   </si>
   <si>
-    <t>1.14.10</t>
-  </si>
-  <si>
     <t>uniform</t>
   </si>
   <si>
@@ -1578,6 +1570,9 @@
   </si>
   <si>
     <t>res_stock_reporting.lighting</t>
+  </si>
+  <si>
+    <t>1.15.7-resstock</t>
   </si>
 </sst>
 </file>
@@ -3254,7 +3249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3345,6 +3340,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1503">
@@ -5151,9 +5155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5196,45 +5198,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>224</v>
+      <c r="B5" s="47" t="s">
+        <v>512</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="46.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>136</v>
+      <c r="B7" s="48" t="s">
+        <v>138</v>
       </c>
       <c r="C7" s="23" t="str">
         <f>VLOOKUP($B7,instance_defs,5,FALSE)</f>
@@ -5242,21 +5244,21 @@
       </c>
       <c r="D7" s="23" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
-        <v>4 Cores with 40 GB</v>
+        <v>8 Cores with 80 GB</v>
       </c>
       <c r="E7" s="23" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
-        <v>$0.28/hour</v>
+        <v>$0.56/hour</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="49" t="s">
         <v>147</v>
       </c>
       <c r="C8" s="23" t="str">
@@ -5275,12 +5277,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5288,13 +5290,13 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$0.28/hour</v>
+        <v>$5.6/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="22" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>192</v>
       </c>
@@ -5323,7 +5325,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>77</v>
@@ -5334,7 +5336,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>156</v>
@@ -5345,7 +5347,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>156</v>
@@ -5443,14 +5445,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="E24" s="22"/>
     </row>
@@ -5658,7 +5660,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5684,13 +5686,13 @@
         <v>29</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>58</v>
@@ -5772,11 +5774,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5968,13 +5965,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>41</v>
@@ -6006,18 +6003,18 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -6042,13 +6039,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>41</v>
@@ -6080,18 +6077,18 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6118,10 +6115,10 @@
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="41" t="s">
@@ -6148,7 +6145,7 @@
       <c r="P8" s="41"/>
       <c r="Q8" s="41"/>
       <c r="R8" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S8" s="41"/>
       <c r="T8" s="41"/>
@@ -6162,13 +6159,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>41</v>
@@ -6200,18 +6197,18 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6238,10 +6235,10 @@
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F11" s="41"/>
       <c r="G11" s="41" t="s">
@@ -6268,7 +6265,7 @@
       <c r="P11" s="41"/>
       <c r="Q11" s="41"/>
       <c r="R11" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S11" s="41"/>
       <c r="T11" s="41"/>
@@ -6282,13 +6279,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E12" s="40" t="s">
         <v>41</v>
@@ -6320,18 +6317,18 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -6358,10 +6355,10 @@
       </c>
       <c r="C14" s="41"/>
       <c r="D14" s="41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="41" t="s">
@@ -6388,7 +6385,7 @@
       <c r="P14" s="41"/>
       <c r="Q14" s="41"/>
       <c r="R14" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S14" s="41"/>
       <c r="T14" s="41"/>
@@ -6402,13 +6399,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E15" s="40" t="s">
         <v>41</v>
@@ -6440,18 +6437,18 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6478,10 +6475,10 @@
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="41" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F17" s="41"/>
       <c r="G17" s="41" t="s">
@@ -6508,7 +6505,7 @@
       <c r="P17" s="41"/>
       <c r="Q17" s="41"/>
       <c r="R17" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S17" s="41"/>
       <c r="T17" s="41"/>
@@ -6522,13 +6519,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>41</v>
@@ -6560,18 +6557,18 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6598,10 +6595,10 @@
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F20" s="41"/>
       <c r="G20" s="41" t="s">
@@ -6628,7 +6625,7 @@
       <c r="P20" s="41"/>
       <c r="Q20" s="41"/>
       <c r="R20" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S20" s="41"/>
       <c r="T20" s="41"/>
@@ -6642,13 +6639,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>41</v>
@@ -6680,18 +6677,18 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6718,10 +6715,10 @@
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F23" s="41"/>
       <c r="G23" s="41" t="s">
@@ -6748,7 +6745,7 @@
       <c r="P23" s="41"/>
       <c r="Q23" s="41"/>
       <c r="R23" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S23" s="41"/>
       <c r="T23" s="41"/>
@@ -6762,13 +6759,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>41</v>
@@ -6800,18 +6797,18 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -6838,10 +6835,10 @@
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41" t="s">
@@ -6868,7 +6865,7 @@
       <c r="P26" s="41"/>
       <c r="Q26" s="41"/>
       <c r="R26" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S26" s="41"/>
       <c r="T26" s="41"/>
@@ -6882,13 +6879,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>41</v>
@@ -6920,18 +6917,18 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -6958,10 +6955,10 @@
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F29" s="41"/>
       <c r="G29" s="41" t="s">
@@ -6988,7 +6985,7 @@
       <c r="P29" s="41"/>
       <c r="Q29" s="41"/>
       <c r="R29" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S29" s="41"/>
       <c r="T29" s="41"/>
@@ -7002,13 +6999,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E30" s="40" t="s">
         <v>41</v>
@@ -7040,18 +7037,18 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7078,10 +7075,10 @@
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F32" s="41"/>
       <c r="G32" s="41" t="s">
@@ -7108,7 +7105,7 @@
       <c r="P32" s="41"/>
       <c r="Q32" s="41"/>
       <c r="R32" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S32" s="41"/>
       <c r="T32" s="41"/>
@@ -7122,13 +7119,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E33" s="40" t="s">
         <v>41</v>
@@ -7160,18 +7157,18 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7198,10 +7195,10 @@
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F35" s="41"/>
       <c r="G35" s="41" t="s">
@@ -7228,7 +7225,7 @@
       <c r="P35" s="41"/>
       <c r="Q35" s="41"/>
       <c r="R35" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S35" s="41"/>
       <c r="T35" s="41"/>
@@ -7242,13 +7239,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E36" s="40" t="s">
         <v>41</v>
@@ -7280,18 +7277,18 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7318,10 +7315,10 @@
       </c>
       <c r="C38" s="41"/>
       <c r="D38" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="41" t="s">
@@ -7348,7 +7345,7 @@
       <c r="P38" s="41"/>
       <c r="Q38" s="41"/>
       <c r="R38" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S38" s="41"/>
       <c r="T38" s="41"/>
@@ -7362,13 +7359,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E39" s="40" t="s">
         <v>41</v>
@@ -7400,18 +7397,18 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7438,10 +7435,10 @@
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="41" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E41" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F41" s="41"/>
       <c r="G41" s="41" t="s">
@@ -7468,7 +7465,7 @@
       <c r="P41" s="41"/>
       <c r="Q41" s="41"/>
       <c r="R41" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S41" s="41"/>
       <c r="T41" s="41"/>
@@ -7482,13 +7479,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E42" s="40" t="s">
         <v>41</v>
@@ -7520,18 +7517,18 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7558,10 +7555,10 @@
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F44" s="41"/>
       <c r="G44" s="41" t="s">
@@ -7588,7 +7585,7 @@
       <c r="P44" s="41"/>
       <c r="Q44" s="41"/>
       <c r="R44" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S44" s="41"/>
       <c r="T44" s="41"/>
@@ -7602,13 +7599,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E45" s="40" t="s">
         <v>41</v>
@@ -7640,18 +7637,18 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7678,10 +7675,10 @@
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="41" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="41" t="s">
@@ -7708,7 +7705,7 @@
       <c r="P47" s="41"/>
       <c r="Q47" s="41"/>
       <c r="R47" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S47" s="41"/>
       <c r="T47" s="41"/>
@@ -7722,13 +7719,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E48" s="40" t="s">
         <v>41</v>
@@ -7760,18 +7757,18 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -7798,10 +7795,10 @@
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="41" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E50" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F50" s="41"/>
       <c r="G50" s="41" t="s">
@@ -7828,7 +7825,7 @@
       <c r="P50" s="41"/>
       <c r="Q50" s="41"/>
       <c r="R50" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S50" s="41"/>
       <c r="T50" s="41"/>
@@ -7842,13 +7839,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>41</v>
@@ -7880,18 +7877,18 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -7918,10 +7915,10 @@
       </c>
       <c r="C53" s="41"/>
       <c r="D53" s="41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E53" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F53" s="41"/>
       <c r="G53" s="41" t="s">
@@ -7948,7 +7945,7 @@
       <c r="P53" s="41"/>
       <c r="Q53" s="41"/>
       <c r="R53" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S53" s="41"/>
       <c r="T53" s="41"/>
@@ -7962,13 +7959,13 @@
         <v>1</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E54" s="40" t="s">
         <v>41</v>
@@ -8000,18 +7997,18 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8038,10 +8035,10 @@
       </c>
       <c r="C56" s="41"/>
       <c r="D56" s="41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E56" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F56" s="41"/>
       <c r="G56" s="41" t="s">
@@ -8068,7 +8065,7 @@
       <c r="P56" s="41"/>
       <c r="Q56" s="41"/>
       <c r="R56" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S56" s="41"/>
       <c r="T56" s="41"/>
@@ -8082,13 +8079,13 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C57" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E57" s="40" t="s">
         <v>41</v>
@@ -8120,18 +8117,18 @@
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8158,10 +8155,10 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F59" s="41"/>
       <c r="G59" s="41" t="s">
@@ -8188,7 +8185,7 @@
       <c r="P59" s="41"/>
       <c r="Q59" s="41"/>
       <c r="R59" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S59" s="41"/>
       <c r="T59" s="41"/>
@@ -8202,13 +8199,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E60" s="40" t="s">
         <v>41</v>
@@ -8240,18 +8237,18 @@
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8278,10 +8275,10 @@
       </c>
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E62" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F62" s="41"/>
       <c r="G62" s="41" t="s">
@@ -8308,7 +8305,7 @@
       <c r="P62" s="41"/>
       <c r="Q62" s="41"/>
       <c r="R62" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S62" s="41"/>
       <c r="T62" s="41"/>
@@ -8322,13 +8319,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C63" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E63" s="40" t="s">
         <v>41</v>
@@ -8360,18 +8357,18 @@
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8398,10 +8395,10 @@
       </c>
       <c r="C65" s="41"/>
       <c r="D65" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E65" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F65" s="41"/>
       <c r="G65" s="41" t="s">
@@ -8428,7 +8425,7 @@
       <c r="P65" s="41"/>
       <c r="Q65" s="41"/>
       <c r="R65" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S65" s="41"/>
       <c r="T65" s="41"/>
@@ -8442,13 +8439,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E66" s="40" t="s">
         <v>41</v>
@@ -8480,18 +8477,18 @@
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8518,10 +8515,10 @@
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E68" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F68" s="41"/>
       <c r="G68" s="41" t="s">
@@ -8548,7 +8545,7 @@
       <c r="P68" s="41"/>
       <c r="Q68" s="41"/>
       <c r="R68" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S68" s="41"/>
       <c r="T68" s="41"/>
@@ -8562,13 +8559,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C69" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D69" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E69" s="40" t="s">
         <v>41</v>
@@ -8600,18 +8597,18 @@
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F70" s="10"/>
       <c r="G70" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8638,10 +8635,10 @@
       </c>
       <c r="C71" s="41"/>
       <c r="D71" s="41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E71" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F71" s="41"/>
       <c r="G71" s="41" t="s">
@@ -8668,7 +8665,7 @@
       <c r="P71" s="41"/>
       <c r="Q71" s="41"/>
       <c r="R71" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S71" s="41"/>
       <c r="T71" s="41"/>
@@ -8682,13 +8679,13 @@
         <v>1</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C72" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>41</v>
@@ -8720,18 +8717,18 @@
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F73" s="10"/>
       <c r="G73" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -8758,10 +8755,10 @@
       </c>
       <c r="C74" s="41"/>
       <c r="D74" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E74" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F74" s="41"/>
       <c r="G74" s="41" t="s">
@@ -8788,7 +8785,7 @@
       <c r="P74" s="41"/>
       <c r="Q74" s="41"/>
       <c r="R74" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S74" s="41"/>
       <c r="T74" s="41"/>
@@ -8802,13 +8799,13 @@
         <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C75" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D75" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E75" s="40" t="s">
         <v>41</v>
@@ -8840,18 +8837,18 @@
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F76" s="10"/>
       <c r="G76" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8878,10 +8875,10 @@
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E77" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F77" s="41"/>
       <c r="G77" s="41" t="s">
@@ -8908,7 +8905,7 @@
       <c r="P77" s="41"/>
       <c r="Q77" s="41"/>
       <c r="R77" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S77" s="41"/>
       <c r="T77" s="41"/>
@@ -8922,13 +8919,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>41</v>
@@ -8960,18 +8957,18 @@
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F79" s="10"/>
       <c r="G79" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -8998,10 +8995,10 @@
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E80" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F80" s="41"/>
       <c r="G80" s="41" t="s">
@@ -9028,7 +9025,7 @@
       <c r="P80" s="41"/>
       <c r="Q80" s="41"/>
       <c r="R80" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S80" s="41"/>
       <c r="T80" s="41"/>
@@ -9042,13 +9039,13 @@
         <v>1</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E81" s="40" t="s">
         <v>41</v>
@@ -9080,18 +9077,18 @@
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F82" s="10"/>
       <c r="G82" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9118,10 +9115,10 @@
       </c>
       <c r="C83" s="41"/>
       <c r="D83" s="41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E83" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F83" s="41"/>
       <c r="G83" s="41" t="s">
@@ -9148,7 +9145,7 @@
       <c r="P83" s="41"/>
       <c r="Q83" s="41"/>
       <c r="R83" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S83" s="41"/>
       <c r="T83" s="41"/>
@@ -9162,13 +9159,13 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C84" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E84" s="40" t="s">
         <v>41</v>
@@ -9200,18 +9197,18 @@
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9238,10 +9235,10 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F86" s="41"/>
       <c r="G86" s="41" t="s">
@@ -9268,7 +9265,7 @@
       <c r="P86" s="41"/>
       <c r="Q86" s="41"/>
       <c r="R86" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S86" s="41"/>
       <c r="T86" s="41"/>
@@ -9282,13 +9279,13 @@
         <v>1</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C87" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E87" s="40" t="s">
         <v>41</v>
@@ -9320,18 +9317,18 @@
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F88" s="10"/>
       <c r="G88" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9358,10 +9355,10 @@
       </c>
       <c r="C89" s="41"/>
       <c r="D89" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E89" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F89" s="41"/>
       <c r="G89" s="41" t="s">
@@ -9388,7 +9385,7 @@
       <c r="P89" s="41"/>
       <c r="Q89" s="41"/>
       <c r="R89" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S89" s="41"/>
       <c r="T89" s="41"/>
@@ -9402,13 +9399,13 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C90" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E90" s="40" t="s">
         <v>41</v>
@@ -9440,18 +9437,18 @@
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F91" s="10"/>
       <c r="G91" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9478,10 +9475,10 @@
       </c>
       <c r="C92" s="41"/>
       <c r="D92" s="41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E92" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F92" s="41"/>
       <c r="G92" s="41" t="s">
@@ -9508,7 +9505,7 @@
       <c r="P92" s="41"/>
       <c r="Q92" s="41"/>
       <c r="R92" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S92" s="41"/>
       <c r="T92" s="41"/>
@@ -9522,13 +9519,13 @@
         <v>1</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C93" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E93" s="40" t="s">
         <v>41</v>
@@ -9560,18 +9557,18 @@
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F94" s="10"/>
       <c r="G94" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9598,10 +9595,10 @@
       </c>
       <c r="C95" s="41"/>
       <c r="D95" s="41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E95" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F95" s="41"/>
       <c r="G95" s="41" t="s">
@@ -9628,7 +9625,7 @@
       <c r="P95" s="41"/>
       <c r="Q95" s="41"/>
       <c r="R95" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S95" s="41"/>
       <c r="T95" s="41"/>
@@ -9642,13 +9639,13 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C96" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D96" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E96" s="40" t="s">
         <v>41</v>
@@ -9680,18 +9677,18 @@
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F97" s="10"/>
       <c r="G97" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9718,10 +9715,10 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E98" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F98" s="41"/>
       <c r="G98" s="41" t="s">
@@ -9748,7 +9745,7 @@
       <c r="P98" s="41"/>
       <c r="Q98" s="41"/>
       <c r="R98" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S98" s="41"/>
       <c r="T98" s="41"/>
@@ -9762,13 +9759,13 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C99" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D99" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E99" s="40" t="s">
         <v>41</v>
@@ -9800,18 +9797,18 @@
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F100" s="10"/>
       <c r="G100" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9838,10 +9835,10 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E101" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F101" s="41"/>
       <c r="G101" s="41" t="s">
@@ -9868,7 +9865,7 @@
       <c r="P101" s="41"/>
       <c r="Q101" s="41"/>
       <c r="R101" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S101" s="41"/>
       <c r="T101" s="41"/>
@@ -9882,13 +9879,13 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C102" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E102" s="40" t="s">
         <v>41</v>
@@ -9920,18 +9917,18 @@
       </c>
       <c r="C103" s="10"/>
       <c r="D103" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F103" s="10"/>
       <c r="G103" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -9958,10 +9955,10 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E104" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F104" s="41"/>
       <c r="G104" s="41" t="s">
@@ -9988,7 +9985,7 @@
       <c r="P104" s="41"/>
       <c r="Q104" s="41"/>
       <c r="R104" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S104" s="41"/>
       <c r="T104" s="41"/>
@@ -10002,13 +9999,13 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C105" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E105" s="40" t="s">
         <v>41</v>
@@ -10040,18 +10037,18 @@
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F106" s="10"/>
       <c r="G106" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10078,10 +10075,10 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E107" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F107" s="41"/>
       <c r="G107" s="41" t="s">
@@ -10108,7 +10105,7 @@
       <c r="P107" s="41"/>
       <c r="Q107" s="41"/>
       <c r="R107" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S107" s="41"/>
       <c r="T107" s="41"/>
@@ -10122,13 +10119,13 @@
         <v>1</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C108" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E108" s="40" t="s">
         <v>41</v>
@@ -10160,18 +10157,18 @@
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F109" s="10"/>
       <c r="G109" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10198,10 +10195,10 @@
       </c>
       <c r="C110" s="41"/>
       <c r="D110" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E110" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F110" s="41"/>
       <c r="G110" s="41" t="s">
@@ -10228,7 +10225,7 @@
       <c r="P110" s="41"/>
       <c r="Q110" s="41"/>
       <c r="R110" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S110" s="41"/>
       <c r="T110" s="41"/>
@@ -10242,13 +10239,13 @@
         <v>1</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C111" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E111" s="40" t="s">
         <v>41</v>
@@ -10280,18 +10277,18 @@
       </c>
       <c r="C112" s="10"/>
       <c r="D112" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F112" s="10"/>
       <c r="G112" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10318,10 +10315,10 @@
       </c>
       <c r="C113" s="41"/>
       <c r="D113" s="41" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E113" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F113" s="41"/>
       <c r="G113" s="41" t="s">
@@ -10348,7 +10345,7 @@
       <c r="P113" s="41"/>
       <c r="Q113" s="41"/>
       <c r="R113" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S113" s="41"/>
       <c r="T113" s="41"/>
@@ -10362,13 +10359,13 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C114" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E114" s="40" t="s">
         <v>41</v>
@@ -10400,18 +10397,18 @@
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E115" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F115" s="10"/>
       <c r="G115" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10438,10 +10435,10 @@
       </c>
       <c r="C116" s="41"/>
       <c r="D116" s="41" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E116" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F116" s="41"/>
       <c r="G116" s="41" t="s">
@@ -10468,7 +10465,7 @@
       <c r="P116" s="41"/>
       <c r="Q116" s="41"/>
       <c r="R116" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S116" s="41"/>
       <c r="T116" s="41"/>
@@ -10482,13 +10479,13 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C117" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D117" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E117" s="40" t="s">
         <v>41</v>
@@ -10520,18 +10517,18 @@
       </c>
       <c r="C118" s="10"/>
       <c r="D118" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F118" s="10"/>
       <c r="G118" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10558,10 +10555,10 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E119" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F119" s="41"/>
       <c r="G119" s="41" t="s">
@@ -10588,7 +10585,7 @@
       <c r="P119" s="41"/>
       <c r="Q119" s="41"/>
       <c r="R119" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S119" s="41"/>
       <c r="T119" s="41"/>
@@ -10602,13 +10599,13 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C120" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D120" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E120" s="40" t="s">
         <v>41</v>
@@ -10640,18 +10637,18 @@
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F121" s="10"/>
       <c r="G121" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10678,10 +10675,10 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E122" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F122" s="41"/>
       <c r="G122" s="41" t="s">
@@ -10708,7 +10705,7 @@
       <c r="P122" s="41"/>
       <c r="Q122" s="41"/>
       <c r="R122" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S122" s="41"/>
       <c r="T122" s="41"/>
@@ -10722,13 +10719,13 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C123" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D123" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E123" s="40" t="s">
         <v>41</v>
@@ -10760,18 +10757,18 @@
       </c>
       <c r="C124" s="10"/>
       <c r="D124" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F124" s="10"/>
       <c r="G124" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10798,10 +10795,10 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E125" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F125" s="41"/>
       <c r="G125" s="41" t="s">
@@ -10828,7 +10825,7 @@
       <c r="P125" s="41"/>
       <c r="Q125" s="41"/>
       <c r="R125" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S125" s="41"/>
       <c r="T125" s="41"/>
@@ -10842,13 +10839,13 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C126" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D126" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E126" s="40" t="s">
         <v>41</v>
@@ -10880,18 +10877,18 @@
       </c>
       <c r="C127" s="10"/>
       <c r="D127" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F127" s="10"/>
       <c r="G127" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10918,10 +10915,10 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E128" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F128" s="41"/>
       <c r="G128" s="41" t="s">
@@ -10948,7 +10945,7 @@
       <c r="P128" s="41"/>
       <c r="Q128" s="41"/>
       <c r="R128" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S128" s="41"/>
       <c r="T128" s="41"/>
@@ -10962,13 +10959,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C129" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D129" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E129" s="40" t="s">
         <v>41</v>
@@ -11000,18 +10997,18 @@
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F130" s="10"/>
       <c r="G130" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11038,10 +11035,10 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E131" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F131" s="41"/>
       <c r="G131" s="41" t="s">
@@ -11068,7 +11065,7 @@
       <c r="P131" s="41"/>
       <c r="Q131" s="41"/>
       <c r="R131" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S131" s="41"/>
       <c r="T131" s="41"/>
@@ -11082,13 +11079,13 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C132" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D132" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E132" s="40" t="s">
         <v>41</v>
@@ -11120,18 +11117,18 @@
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F133" s="10"/>
       <c r="G133" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11158,10 +11155,10 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E134" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F134" s="41"/>
       <c r="G134" s="41" t="s">
@@ -11188,7 +11185,7 @@
       <c r="P134" s="41"/>
       <c r="Q134" s="41"/>
       <c r="R134" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S134" s="41"/>
       <c r="T134" s="41"/>
@@ -11202,13 +11199,13 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C135" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D135" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E135" s="40" t="s">
         <v>41</v>
@@ -11240,18 +11237,18 @@
       </c>
       <c r="C136" s="10"/>
       <c r="D136" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F136" s="10"/>
       <c r="G136" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11278,10 +11275,10 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E137" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F137" s="41"/>
       <c r="G137" s="41" t="s">
@@ -11308,7 +11305,7 @@
       <c r="P137" s="41"/>
       <c r="Q137" s="41"/>
       <c r="R137" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S137" s="41"/>
       <c r="T137" s="41"/>
@@ -11322,13 +11319,13 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C138" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D138" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E138" s="40" t="s">
         <v>41</v>
@@ -11360,18 +11357,18 @@
       </c>
       <c r="C139" s="10"/>
       <c r="D139" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F139" s="10"/>
       <c r="G139" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11398,10 +11395,10 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E140" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F140" s="41"/>
       <c r="G140" s="41" t="s">
@@ -11428,7 +11425,7 @@
       <c r="P140" s="41"/>
       <c r="Q140" s="41"/>
       <c r="R140" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S140" s="41"/>
       <c r="T140" s="41"/>
@@ -11442,13 +11439,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C141" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D141" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E141" s="40" t="s">
         <v>41</v>
@@ -11480,18 +11477,18 @@
       </c>
       <c r="C142" s="10"/>
       <c r="D142" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F142" s="10"/>
       <c r="G142" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11518,10 +11515,10 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E143" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F143" s="41"/>
       <c r="G143" s="41" t="s">
@@ -11548,7 +11545,7 @@
       <c r="P143" s="41"/>
       <c r="Q143" s="41"/>
       <c r="R143" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S143" s="41"/>
       <c r="T143" s="41"/>
@@ -11562,13 +11559,13 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C144" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D144" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E144" s="40" t="s">
         <v>41</v>
@@ -11600,18 +11597,18 @@
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E145" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F145" s="10"/>
       <c r="G145" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11638,10 +11635,10 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E146" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F146" s="41"/>
       <c r="G146" s="41" t="s">
@@ -11668,7 +11665,7 @@
       <c r="P146" s="41"/>
       <c r="Q146" s="41"/>
       <c r="R146" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S146" s="41"/>
       <c r="T146" s="41"/>
@@ -11682,13 +11679,13 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C147" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D147" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E147" s="40" t="s">
         <v>41</v>
@@ -11720,18 +11717,18 @@
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F148" s="10"/>
       <c r="G148" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11758,10 +11755,10 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E149" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F149" s="41"/>
       <c r="G149" s="41" t="s">
@@ -11788,7 +11785,7 @@
       <c r="P149" s="41"/>
       <c r="Q149" s="41"/>
       <c r="R149" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S149" s="41"/>
       <c r="T149" s="41"/>
@@ -11802,13 +11799,13 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C150" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D150" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E150" s="40" t="s">
         <v>41</v>
@@ -11840,18 +11837,18 @@
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E151" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F151" s="10"/>
       <c r="G151" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11878,10 +11875,10 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E152" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F152" s="41"/>
       <c r="G152" s="41" t="s">
@@ -11908,7 +11905,7 @@
       <c r="P152" s="41"/>
       <c r="Q152" s="41"/>
       <c r="R152" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S152" s="41"/>
       <c r="T152" s="41"/>
@@ -11922,13 +11919,13 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C153" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D153" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E153" s="40" t="s">
         <v>41</v>
@@ -11960,18 +11957,18 @@
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E154" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F154" s="10"/>
       <c r="G154" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -11998,10 +11995,10 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E155" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F155" s="41"/>
       <c r="G155" s="41" t="s">
@@ -12028,7 +12025,7 @@
       <c r="P155" s="41"/>
       <c r="Q155" s="41"/>
       <c r="R155" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S155" s="41"/>
       <c r="T155" s="41"/>
@@ -12042,13 +12039,13 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C156" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D156" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E156" s="40" t="s">
         <v>41</v>
@@ -12080,18 +12077,18 @@
       </c>
       <c r="C157" s="10"/>
       <c r="D157" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E157" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F157" s="10"/>
       <c r="G157" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12118,10 +12115,10 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E158" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F158" s="41"/>
       <c r="G158" s="41" t="s">
@@ -12148,7 +12145,7 @@
       <c r="P158" s="41"/>
       <c r="Q158" s="41"/>
       <c r="R158" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S158" s="41"/>
       <c r="T158" s="41"/>
@@ -12162,13 +12159,13 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C159" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D159" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E159" s="40" t="s">
         <v>41</v>
@@ -12200,18 +12197,18 @@
       </c>
       <c r="C160" s="10"/>
       <c r="D160" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E160" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F160" s="10"/>
       <c r="G160" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12238,10 +12235,10 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E161" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F161" s="41"/>
       <c r="G161" s="41" t="s">
@@ -12268,7 +12265,7 @@
       <c r="P161" s="41"/>
       <c r="Q161" s="41"/>
       <c r="R161" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S161" s="41"/>
       <c r="T161" s="41"/>
@@ -12282,16 +12279,16 @@
         <v>1</v>
       </c>
       <c r="B162" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="C162" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="C162" s="42" t="s">
-        <v>334</v>
-      </c>
       <c r="D162" s="42" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E162" s="42" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F162" s="42"/>
       <c r="G162" s="42"/>
@@ -12332,7 +12329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
@@ -12450,16 +12447,16 @@
     </row>
     <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
@@ -12477,16 +12474,16 @@
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G5" s="15" t="b">
         <v>0</v>
@@ -12504,16 +12501,16 @@
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G6" s="15" t="b">
         <v>0</v>
@@ -12531,16 +12528,16 @@
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G7" s="15" t="b">
         <v>0</v>
@@ -12558,16 +12555,16 @@
     </row>
     <row r="8" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G8" s="15" t="b">
         <v>0</v>
@@ -12585,16 +12582,16 @@
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G9" s="15" t="b">
         <v>0</v>
@@ -12612,16 +12609,16 @@
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G10" s="15" t="b">
         <v>0</v>
@@ -12639,16 +12636,16 @@
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G11" s="15" t="b">
         <v>0</v>
@@ -12666,16 +12663,16 @@
     </row>
     <row r="12" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G12" s="15" t="b">
         <v>0</v>
@@ -12693,16 +12690,16 @@
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G13" s="15" t="b">
         <v>0</v>
@@ -12720,16 +12717,16 @@
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -12747,16 +12744,16 @@
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G15" s="15" t="b">
         <v>0</v>
@@ -12774,16 +12771,16 @@
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -12801,14 +12798,14 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B17" s="21"/>
       <c r="D17" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -12822,14 +12819,14 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B18" s="21"/>
       <c r="D18" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -12843,16 +12840,16 @@
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -12870,16 +12867,16 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -12897,16 +12894,16 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>0</v>
@@ -12924,16 +12921,16 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>0</v>
@@ -12951,16 +12948,16 @@
     </row>
     <row r="23" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>0</v>
@@ -12978,14 +12975,14 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B24" s="21"/>
       <c r="D24" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>0</v>
@@ -12999,14 +12996,14 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B25" s="21"/>
       <c r="D25" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G25" s="15" t="b">
         <v>0</v>
@@ -13020,14 +13017,14 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G26" s="15" t="b">
         <v>0</v>
@@ -13041,14 +13038,14 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G27" s="15" t="b">
         <v>0</v>
@@ -13062,14 +13059,14 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B28" s="21"/>
       <c r="D28" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G28" s="15" t="b">
         <v>0</v>
@@ -13083,14 +13080,14 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B29" s="21"/>
       <c r="D29" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G29" s="15" t="b">
         <v>0</v>
@@ -13104,14 +13101,14 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B30" s="21"/>
       <c r="D30" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G30" s="15" t="b">
         <v>0</v>
@@ -13125,14 +13122,14 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B31" s="21"/>
       <c r="D31" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G31" s="15" t="b">
         <v>0</v>
@@ -13146,14 +13143,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B32" s="21"/>
       <c r="D32" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G32" s="15" t="b">
         <v>0</v>
@@ -13167,14 +13164,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B33" s="21"/>
       <c r="D33" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G33" s="15" t="b">
         <v>0</v>
@@ -13188,14 +13185,14 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="45" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G34" s="15" t="b">
         <v>0</v>
@@ -13209,14 +13206,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="45" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G35" s="15" t="b">
         <v>0</v>
@@ -13230,14 +13227,14 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B36" s="21"/>
       <c r="D36" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G36" s="15" t="b">
         <v>0</v>
@@ -13251,14 +13248,14 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="45" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B37" s="21"/>
       <c r="D37" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G37" s="15" t="b">
         <v>0</v>
@@ -13272,14 +13269,14 @@
     </row>
     <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B38" s="21"/>
       <c r="D38" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G38" s="15" t="b">
         <v>0</v>
@@ -13293,14 +13290,14 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B39" s="21"/>
       <c r="D39" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G39" s="15" t="b">
         <v>0</v>
@@ -13314,14 +13311,14 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G40" s="15" t="b">
         <v>0</v>
@@ -13335,14 +13332,14 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G41" s="15" t="b">
         <v>0</v>
@@ -13356,14 +13353,14 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G42" s="15" t="b">
         <v>0</v>
@@ -13377,14 +13374,14 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G43" s="15" t="b">
         <v>0</v>
@@ -13398,14 +13395,14 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="45" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G44" s="15" t="b">
         <v>0</v>
@@ -13419,14 +13416,14 @@
     </row>
     <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G45" s="15" t="b">
         <v>0</v>
@@ -13440,14 +13437,14 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="45" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G46" s="15" t="b">
         <v>0</v>
@@ -13461,15 +13458,15 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="45" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G47" s="15" t="b">
         <v>0</v>
@@ -13483,15 +13480,15 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="45" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G48" s="15" t="b">
         <v>0</v>
@@ -13505,15 +13502,15 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="45" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G49" s="15" t="b">
         <v>0</v>
@@ -13527,15 +13524,15 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="45" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G50" s="15" t="b">
         <v>0</v>
@@ -13549,15 +13546,15 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="45" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G51" s="15" t="b">
         <v>0</v>
@@ -13571,15 +13568,15 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="45" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B52" s="21"/>
       <c r="D52" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G52" s="15" t="b">
         <v>0</v>
@@ -13593,15 +13590,15 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="45" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G53" s="15" t="b">
         <v>0</v>
@@ -13615,15 +13612,15 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="45" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G54" s="15" t="b">
         <v>0</v>
@@ -13947,7 +13944,7 @@
         <v>94</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -13988,13 +13985,13 @@
         <v>94</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G19" s="21">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I19" t="s">
         <v>115</v>
@@ -14062,16 +14059,16 @@
     </row>
     <row r="20" spans="1:35" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G20" s="21">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I20" t="s">
         <v>3</v>
@@ -14133,7 +14130,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G21" s="21">
         <v>1</v>
@@ -14175,10 +14172,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>103</v>

</xml_diff>